<commit_message>
Add date excel resources
</commit_message>
<xml_diff>
--- a/resources/excel/Uploaded resources.xlsx
+++ b/resources/excel/Uploaded resources.xlsx
@@ -22,1745 +22,2016 @@
     <t>Elementët Kyç të Ditës së Karrierës</t>
   </si>
   <si>
-    <t>Fuqizoni nxënësit të eksplorojnë karriera në teknologji përmes punëtorive tërheqëse, fjalimeve frymëzuese dhe aktiviteteve praktike. I projektuar për formate fleksibël dhe planifikim të lehtë, ky udhëzues vizual ndihmon organizatorët të krijojnë ngjarje me ndikim dhe të përqendruara te nxënësit në çdo mjedis.</t>
+    <t>Uploaded 4 September 2025
+Fuqizoni nxënësit të eksplorojnë karriera në teknologji përmes punëtorive tërheqëse, fjalimeve frymëzuese dhe aktiviteteve praktike. I projektuar për formate fleksibël dhe planifikim të lehtë, ky udhëzues vizual ndihmon organizatorët të krijojnë ngjarje me ndikim dhe të përqendruara te nxënësit në çdo mjedis.</t>
   </si>
   <si>
     <t xml:space="preserve"> 
 Ключови елементи на Деня на кариерата  </t>
   </si>
   <si>
-    <t>Насърчете учениците да  разгледат кариери в технологиите чрез ангажиращи работилници, вдъхновяващи лекции и практически дейности. Създаден за гъвкави формати и лесно планиране, този визуален наръчник помага на организаторите да създадат въздействащи събития, насочени към учениците, във всякаква среда.</t>
+    <t>Uploaded 4 September 2025
+Насърчете учениците да  разгледат кариери в технологиите чрез ангажиращи работилници, вдъхновяващи лекции и практически дейности. Създаден за гъвкави формати и лесно планиране, този визуален наръчник помага на организаторите да създадат въздействащи събития, насочени към учениците, във всякаква среда.</t>
   </si>
   <si>
     <t>Ključni dijelovi Dana karijera</t>
   </si>
   <si>
-    <t>Osnažite učenike da istražuju karijere u tehnologiji kroz zanimljive radionice, inspirativna predavanja i praktične aktivnosti. Ovaj vizualni vodič pomaže vam da na jednostavan i fleksibilan način isplanirate događaje usmjerene na učenike u bilo kojem okruženju.</t>
+    <t>Uploaded 4 September 2025
+Osnažite učenike da istražuju karijere u tehnologiji kroz zanimljive radionice, inspirativna predavanja i praktične aktivnosti. Ovaj vizualni vodič pomaže vam da na jednostavan i fleksibilan način isplanirate događaje usmjerene na učenike u bilo kojem okruženju.</t>
   </si>
   <si>
     <t>Klíčové prvky Dne kariéry</t>
   </si>
   <si>
-    <t>Umožněte studentům objevovat kariéru v oblasti technologií prostřednictvím poutavých workshopů, inspirativních přednášek a praktických aktivit. Tento vizuální průvodce je navržen pro flexibilní formáty a snadné plánování a pomáhá organizátorům vytvářet smysluplné akce zaměřené na studenty v jakémkoli prostředí.</t>
+    <t>Uploaded 4 September 2025
+Umožněte studentům objevovat kariéru v oblasti technologií prostřednictvím poutavých workshopů, inspirativních přednášek a praktických aktivit. Tento vizuální průvodce je navržen pro flexibilní formáty a snadné plánování a pomáhá organizátorům vytvářet smysluplné akce zaměřené na studenty v jakémkoli prostředí.</t>
   </si>
   <si>
     <t>Infografik om Karrieredag</t>
   </si>
   <si>
-    <t>Giv eleverne mulighed for at udforske karrierer inden for teknologi gennem engagerende workshops, inspirerende oplæg og praktiske aktiviteter. Denne visuelle guide hjælper dig med at planlægge elevfokuserede arrangementer i ethvert miljø på en enkel og fleksibel måde.</t>
+    <t>Uploaded 4 September 2025
+Giv eleverne mulighed for at udforske karrierer inden for teknologi gennem engagerende workshops, inspirerende oplæg og praktiske aktiviteter. Denne visuelle guide hjælper dig med at planlægge elevfokuserede arrangementer i ethvert miljø på en enkel og fleksibel måde.</t>
   </si>
   <si>
     <t>Sleutelelementen van een carrièredag</t>
   </si>
   <si>
-    <t>Stimuleer studenten om een carrière in technologie te verkennen door middel van boeiende workshops, inspirerende presentaties en praktische activiteiten. Deze visuele gids is ontworpen voor flexibele formats en een eenvoudige planning, en helpt organisatoren om impactvolle, studentgerichte evenementen te creëren in elke context.</t>
+    <t>Uploaded 4 September 2025
+Stimuleer studenten om een carrière in technologie te verkennen door middel van boeiende workshops, inspirerende presentaties en praktische activiteiten. Deze visuele gids is ontworpen voor flexibele formats en een eenvoudige planning, en helpt organisatoren om impactvolle, studentgerichte evenementen te creëren in elke context.</t>
   </si>
   <si>
     <t>Career Day Infographic</t>
   </si>
   <si>
-    <t>Empower students to explore careers in technology through engaging workshops, inspiring talks, and hands-on activities. This visual guide helps you plan student-focused events in any setting in a simple and flexible way.</t>
+    <t>Uploaded 4 September 2025
+Empower students to explore careers in technology through engaging workshops, inspiring talks, and hands-on activities. This visual guide helps you plan student-focused events in any setting in a simple and flexible way.</t>
   </si>
   <si>
     <t>Éléments clés d’une journée orientation</t>
   </si>
   <si>
-    <t>Aidez les élèves à découvrir les métiers de la technologie grâce à des ateliers interactifs, des conférences inspirantes et des activités pratiques. Conçu pour des formats flexibles et une organisation simplifiée, ce guide visuel aide les organisateurs à créer des événements pertinents centrés sur les élèves, quel que soit le contexte.</t>
+    <t>Uploaded 4 September 2025
+Aidez les élèves à découvrir les métiers de la technologie grâce à des ateliers interactifs, des conférences inspirantes et des activités pratiques. Conçu pour des formats flexibles et une organisation simplifiée, ce guide visuel aide les organisateurs à créer des événements pertinents centrés sur les élèves, quel que soit le contexte.</t>
   </si>
   <si>
     <t>Schlüsselfaktoren eines Karrieretags</t>
   </si>
   <si>
-    <t>Ermögliche Schüler*innen, sich durch spannende Workshops, inspirierende Vorträge und praxisnahe Aktivitäten mit technischen Berufen vertraut zu machen. Dieser visuelle Leitfaden wurde zur Erleichterung deiner Planung für flexible Formate entwickelt und unterstützt Organisator*innen dabei, wirkungsvolle, schülerorientierte Veranstaltungen in jedem Umfeld zu gestalten.</t>
+    <t>Uploaded 4 September 2025
+Ermögliche Schüler*innen, sich durch spannende Workshops, inspirierende Vorträge und praxisnahe Aktivitäten mit technischen Berufen vertraut zu machen. Dieser visuelle Leitfaden wurde zur Erleichterung deiner Planung für flexible Formate entwickelt und unterstützt Organisator*innen dabei, wirkungsvolle, schülerorientierte Veranstaltungen in jedem Umfeld zu gestalten.</t>
   </si>
   <si>
     <t>Βασικά Στοιχεία Μιας Ημέρας Σταδιοδρομίας</t>
   </si>
   <si>
-    <t>Βοηθήστε τους μαθητές να εξερευνήσουν επαγγέλματα στον τομέα της τεχνολογίας μέσα από διαδραστικά εργαστήρια, εμπνευσμένες ομιλίες και βιωματικές δραστηριότητες. Οπτικά σχεδιασμένος για ευέλικτη μορφή και εύκολο προγραμματισμό, αυτός ο οδηγός βοηθά τους διοργανωτές να δημιουργούν ουσιαστικές, εκδηλώσεις με κέντρο τους μαθητές.</t>
+    <t>Uploaded 4 September 2025
+Βοηθήστε τους μαθητές να εξερευνήσουν επαγγέλματα στον τομέα της τεχνολογίας μέσα από διαδραστικά εργαστήρια, εμπνευσμένες ομιλίες και βιωματικές δραστηριότητες. Οπτικά σχεδιασμένος για ευέλικτη μορφή και εύκολο προγραμματισμό, αυτός ο οδηγός βοηθά τους διοργανωτές να δημιουργούν ουσιαστικές, εκδηλώσεις με κέντρο τους μαθητές.</t>
   </si>
   <si>
     <t>Elementi Chiave di un Career Day</t>
   </si>
   <si>
-    <t>Offri agli studenti l'opportunità di esplorare le carriere tecnologiche tramite workshop coinvolgenti, keynote ispirazionali e attività pratiche. Progettata per formati flessibili e pianificazione semplice, questa guida visiva aiuta gli organizzatori a creare eventi di grande impatto, incentrati sugli studenti, in qualsiasi contesto.</t>
+    <t>Uploaded 4 September 2025
+Offri agli studenti l'opportunità di esplorare le carriere tecnologiche tramite workshop coinvolgenti, keynote ispirazionali e attività pratiche. Progettata per formati flessibili e pianificazione semplice, questa guida visiva aiuta gli organizzatori a creare eventi di grande impatto, incentrati sugli studenti, in qualsiasi contesto.</t>
   </si>
   <si>
     <t>Karjeras dienas galvenie elementi</t>
   </si>
   <si>
-    <t>Iedrošiniet skolēnus izpētīt tehnoloģiju karjeras, piedaloties aizraujošās darbnīcās, iedvesmojošās lekcijās un praktiskās aktivitātēs. Šī vizuālā rokasgrāmata ir paredzēta elastīgam formātam un vienkāršai plānošanai, palīdzot organizatoriem radīt iedarbīgus un skolēniem pielāgotus pasākumus jebkurā vidē.</t>
+    <t>Uploaded 4 September 2025
+Iedrošiniet skolēnus izpētīt tehnoloģiju karjeras, piedaloties aizraujošās darbnīcās, iedvesmojošās lekcijās un praktiskās aktivitātēs. Šī vizuālā rokasgrāmata ir paredzēta elastīgam formātam un vienkāršai plānošanai, palīdzot organizatoriem radīt iedarbīgus un skolēniem pielāgotus pasākumus jebkurā vidē.</t>
   </si>
   <si>
     <t>Pagrindinės karjeros dienos dalys</t>
   </si>
   <si>
-    <t>Suteikite mokiniams galimybę pažinti technologijų karjerą įdomiuose seminaruose, įkvepiančiose paskaitose ir praktiniuose užsiėmimuose. Šis vaizdus vadovas, pritaikytas lanksčiam formatui ir patogiam planavimui, padės organizatoriams surengti moksleiviams patrauklius, įtraukiančius renginius bet kokioje aplinkoje.</t>
+    <t>Uploaded 4 September 2025
+Suteikite mokiniams galimybę pažinti technologijų karjerą įdomiuose seminaruose, įkvepiančiose paskaitose ir praktiniuose užsiėmimuose. Šis vaizdus vadovas, pritaikytas lanksčiam formatui ir patogiam planavimui, padės organizatoriams surengti moksleiviams patrauklius, įtraukiančius renginius bet kokioje aplinkoje.</t>
   </si>
   <si>
     <t>Elementi Ewlenin ta’ Jum il-Karriera</t>
   </si>
   <si>
-    <t>Għin lill-istudenti jesploraw karrieri fit-teknoloġija permezz ta’ workshops interattivi, diskorsi ta’ ispirazzjoni u attivitajiet prattiċi. Dan il-gwida viżiva, iddisinjata għal formati flessibbli u ppjanar faċli, tgħin lill-organizzaturi joħolqu avvenimenti ta’ impatt iffukati fuq l-istudenti f’kull ambjent.</t>
+    <t>Uploaded 4 September 2025
+Għin lill-istudenti jesploraw karrieri fit-teknoloġija permezz ta’ workshops interattivi, diskorsi ta’ ispirazzjoni u attivitajiet prattiċi. Dan il-gwida viżiva, iddisinjata għal formati flessibbli u ppjanar faċli, tgħin lill-organizzaturi joħolqu avvenimenti ta’ impatt iffukati fuq l-istudenti f’kull ambjent.</t>
   </si>
   <si>
     <t>Kluczowe Elementy Dnia Kariery</t>
   </si>
   <si>
-    <t>Wspieraj uczniów w odkrywaniu ścieżek kariery w technologii poprzez angażujące warsztaty, inspirujące prelekcje i zajęcia praktyczne. Ten wizualny przewodnik, zaprojektowany z myślą o elastycznych formatach i łatwym planowaniu, pomaga organizatorom tworzyć efektywne wydarzenia skoncentrowane na uczniach w dowolnym środowisku.</t>
+    <t>Uploaded 4 September 2025
+Wspieraj uczniów w odkrywaniu ścieżek kariery w technologii poprzez angażujące warsztaty, inspirujące prelekcje i zajęcia praktyczne. Ten wizualny przewodnik, zaprojektowany z myślą o elastycznych formatach i łatwym planowaniu, pomaga organizatorom tworzyć efektywne wydarzenia skoncentrowane na uczniach w dowolnym środowisku.</t>
   </si>
   <si>
     <t>Infografia do Dia de Carreira</t>
   </si>
   <si>
-    <t>Capacite os alunos a explorarem carreiras em tecnologia por meio de workshops envolventes, palestras inspiradoras e atividades práticas.
+    <t>Uploaded 4 September 2025
+Capacite os alunos a explorarem carreiras em tecnologia por meio de workshops envolventes, palestras inspiradoras e atividades práticas.
 Este guia visual ajuda você a planejar eventos focados nos estudantes em qualquer ambiente de forma simples e flexível.</t>
   </si>
   <si>
-    <t>Elemente cheie ale unei zile de carieră</t>
-  </si>
-  <si>
-    <t>Inspiră elevii să exploreze carierele în tehnologie prin ateliere interactive, discursuri inspiraționale și activități practice. Acest ghid vizual, conceput pentru formate flexibile și planificare ușoară, îi ajută pe organizatori să creeze evenimente cu impact, axate pe elevi, în orice context.</t>
-  </si>
-  <si>
-    <t>Kľúčové prvky dňa kariéry</t>
-  </si>
-  <si>
-    <t>Umožnite študentom objavovať kariéru v oblasti technológií prostredníctvom zaujímavých workshopov, inšpiratívnych prednášok a praktických aktivít. Tento vizuálny sprievodca je navrhnutý pre flexibilné formáty a jednoduché plánovanie a pomáha organizátorom vytvárať zmysluplné podujatia zamerané na študentov v akomkoľvek prostredí.</t>
+    <t xml:space="preserve">Elemente cheie ale unei zile de carieră  </t>
+  </si>
+  <si>
+    <t>Uploaded 4 September 2025
+Inspiră elevii să exploreze carierele în tehnologie prin ateliere interactive, discursuri inspiraționale și activități practice. Acest ghid vizual, conceput pentru formate flexibile și planificare ușoară, îi ajută pe organizatori să creeze evenimente cu impact, axate pe elevi, în orice context.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kľúčové prvky dňa kariéry  </t>
+  </si>
+  <si>
+    <t>Uploaded 4 September 2025
+Umožnite študentom objavovať kariéru v oblasti technológií prostredníctvom zaujímavých workshopov, inšpiratívnych prednášok a praktických aktivít. Tento vizuálny sprievodca je navrhnutý pre flexibilné formáty a jednoduché plánovanie a pomáha organizátorom vytvárať zmysluplné podujatia zamerané na študentov v akomkoľvek prostredí.</t>
   </si>
   <si>
     <t>Ključni elementi kariernega dne</t>
   </si>
   <si>
-    <t>Opolnomočite učence, da raziskujejo kariere na področju tehnologije, skozi zanimive delavnice, navdihujoče govore in praktične aktivnosti. Vizualni vodnik, zasnovan za prilagodljive formate in preprosto načrtovanje, organizatorjem pomaga ustvarjati učinkovite, na učence usmerjene dogodke, primerno za katerokoli okolje.</t>
-  </si>
-  <si>
-    <t>Elementos clave de un día de carrera</t>
-  </si>
-  <si>
-    <t>Empodera a los estudiantes para explorar carreras tecnológicas mediante talleres interactivos, conferencias inspiradoras y actividades prácticas. Diseñada para formatos flexibles y planificación sencilla, esta guía visual ayuda a los organizadores a crear eventos impactantes centrados en los estudiantes en cualquier entorno.</t>
+    <t>Uploaded 4 September 2025
+Opolnomočite učence, da raziskujejo kariere na področju tehnologije, skozi zanimive delavnice, navdihujoče govore in praktične aktivnosti. Vizualni vodnik, zasnovan za prilagodljive formate in preprosto načrtovanje, organizatorjem pomaga ustvarjati učinkovite, na učence usmerjene dogodke, primerno za katerokoli okolje.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elementos clave de un día de carrera  </t>
+  </si>
+  <si>
+    <t>Uploaded 4 September 2025
+Empodera a los estudiantes para explorar carreras tecnológicas mediante talleres interactivos, conferencias inspiradoras y actividades prácticas. Diseñada para formatos flexibles y planificación sencilla, esta guía visual ayuda a los organizadores a crear eventos impactantes centrados en los estudiantes en cualquier entorno.</t>
   </si>
   <si>
     <t>Uranpäivän keskeiset elementit</t>
   </si>
   <si>
-    <t>Mahdollista oppilaille urien tutkiminen teknologia-alalla innostavien työpajojen, inspiroivien puheiden ja käytännönläheisten aktiviteettien kautta. Tämä visuaalinen opas auttaa sinua suunnittelemaan oppilaskeskeisiä tapahtumia helposti ja joustavasti missä tahansa ympäristössä.</t>
+    <t>Uploaded 4 September 2025
+Mahdollista oppilaille urien tutkiminen teknologia-alalla innostavien työpajojen, inspiroivien puheiden ja käytännönläheisten aktiviteettien kautta. Tämä visuaalinen opas auttaa sinua suunnittelemaan oppilaskeskeisiä tapahtumia helposti ja joustavasti missä tahansa ympäristössä.</t>
   </si>
   <si>
     <t>Infografik för Karriärdagen</t>
   </si>
   <si>
-    <t>Ge elever möjlighet att utforska karriärer inom teknik genom engagerande workshops, inspirerande föreläsningar och praktiska aktiviteter. Denna visuella guide hjälper dig att planera elevfokuserade evenemang på ett enkelt och flexibelt sätt i alla miljöer.</t>
+    <t>Uploaded 4 September 2025
+Ge elever möjlighet att utforska karriärer inom teknik genom engagerande workshops, inspirerande föreläsningar och praktiska aktiviteter. Denna visuella guide hjälper dig att planera elevfokuserade evenemang på ett enkelt och flexibelt sätt i alla miljöer.</t>
   </si>
   <si>
     <t>Kariyer Günü Temel Unsurları</t>
   </si>
   <si>
-    <t>Öğrencilerin teknoloji kariyerlerini keşfetmelerini ilham verici konuşmalar, etkileşimli atölyeler ve uygulamalı etkinliklerle destekleyin. Esnek formatlar ve kolay planlama için tasarlanan bu görsel rehber, düzenleyicilere her ortamda etkili, öğrenci odaklı etkinlikler oluşturma konusunda yardımcı olur.</t>
+    <t>Uploaded 4 September 2025
+Öğrencilerin teknoloji kariyerlerini keşfetmelerini ilham verici konuşmalar, etkileşimli atölyeler ve uygulamalı etkinliklerle destekleyin. Esnek formatlar ve kolay planlama için tasarlanan bu görsel rehber, düzenleyicilere her ortamda etkili, öğrenci odaklı etkinlikler oluşturma konusunda yardımcı olur.</t>
   </si>
   <si>
     <t>Ключові Елементи Дня Кар’єри</t>
   </si>
   <si>
-    <t>Надихайте учнів досліджувати кар’єри в галузі технологій за допомогою цікавих майстер-класів, надихаючих виступів і практичних занять. Цей візуальний посібник розроблений для гнучких форматів і легкого планування, допомагаючи організаторам створювати ефективні заходи, орієнтовані на учнів, у будь-якому середовищі.</t>
+    <t>Uploaded 4 September 2025
+Надихайте учнів досліджувати кар’єри в галузі технологій за допомогою цікавих майстер-класів, надихаючих виступів і практичних занять. Цей візуальний посібник розроблений для гнучких форматів і легкого планування, допомагаючи організаторам створювати ефективні заходи, орієнтовані на учнів, у будь-якому середовищі.</t>
   </si>
   <si>
     <t>Udhëzuesi juaj për Karriera Digjitale</t>
   </si>
   <si>
-    <t>Një përmbledhje frymëzuese e rrugëve kryesore të karrierës në fushën digjitale, kjo infografikë thekson pse teknologjia është një zgjedhje e mençur për të ardhmen. Paraqet role shumë të kërkuara, këshilla për të filluar dhe hapa konkretë për të ndihmuar nxënësit të zbulojnë interesat e tyre dhe të zhvillojnë aftësi digjitale. E përkryer për të nxitur kuriozitetin dhe për të udhëzuar hapat e para në botën e teknologjisë.</t>
+    <t>Uploaded 4 September 2025
+Një përmbledhje frymëzuese e rrugëve kryesore të karrierës në fushën digjitale, kjo infografikë thekson pse teknologjia është një zgjedhje e mençur për të ardhmen. Paraqet role shumë të kërkuara, këshilla për të filluar dhe hapa konkretë për të ndihmuar nxënësit të zbulojnë interesat e tyre dhe të zhvillojnë aftësi digjitale. E përkryer për të nxitur kuriozitetin dhe për të udhëzuar hapat e para në botën e teknologjisë.</t>
   </si>
   <si>
     <t xml:space="preserve">Вашият наръчник за кариери в дигиталния свят 
 </t>
   </si>
   <si>
-    <t>Вдъхновяващ преглед на водещите дигитални професии, тази инфографика показва защо кариерите с технологии са правилен избор за бъдещето. Включва търсени професии, съвети за започване и конкретни стъпки, които помагат на учениците да разгледат интересите си и развиват дигитални умения. Идеална за събуждане на любопитство и ориентиране в първите стъпки към света на технологиите.</t>
+    <t>Uploaded 4 September 2025
+Вдъхновяващ преглед на водещите дигитални професии, тази инфографика показва защо кариерите с технологии са правилен избор за бъдещето. Включва търсени професии, съвети за започване и конкретни стъпки, които помагат на учениците да разгледат интересите си и развиват дигитални умения. Идеална за събуждане на любопитство и ориентиране в първите стъпки към света на технологиите.</t>
   </si>
   <si>
     <t>Tvoj vodič za karijere u digitalnom svijetu</t>
   </si>
   <si>
-    <t>Infografika prikazuje najtraženije digitalne karijere i ističe zašto je tehnologija pametan izbor za buduću karijeru. Sadrži tražene poslove i zanimanja, savjete za početak i konkretne korake koji pomažu učenicima i studentima istražiti svoje interese i razviti digitalne vještine. Materijal je polazna točka za poticanje znatiželje i usmjeravanje prvih koraka u svijet tehnologije.</t>
+    <t>Uploaded 4 September 2025
+Infografika prikazuje najtraženije digitalne karijere i ističe zašto je tehnologija pametan izbor za buduću karijeru. Sadrži tražene poslove i zanimanja, savjete za početak i konkretne korake koji pomažu učenicima i studentima istražiti svoje interese i razviti digitalne vještine. Materijal je polazna točka za poticanje znatiželje i usmjeravanje prvih koraka u svijet tehnologije.</t>
   </si>
   <si>
     <t>Váš průvodce digitálními kariérami</t>
   </si>
   <si>
-    <t>Inspirativní přehled nejžádanějších digitálních kariérních cest, tato infografika ukazuje, proč je technologie chytrou volbou pro budoucnost. Obsahuje žádané pozice, tipy, jak začít, a praktické kroky, které studentům pomohou objevit své zájmy a rozvíjet digitální dovednosti. Ideální pro vzbuzení zvědavosti a vedení prvních kroků do světa technologií.</t>
+    <t>Uploaded 4 September 2025
+Inspirativní přehled nejžádanějších digitálních kariérních cest, tato infografika ukazuje, proč je technologie chytrou volbou pro budoucnost. Obsahuje žádané pozice, tipy, jak začít, a praktické kroky, které studentům pomohou objevit své zájmy a rozvíjet digitální dovednosti. Ideální pro vzbuzení zvědavosti a vedení prvních kroků do světa technologií.</t>
   </si>
   <si>
     <t>Din guide til karrierer i den digitale verden</t>
   </si>
   <si>
-    <t>Infografikken viser de mest efterspurgte digitale karrierer og fremhæver, hvorfor teknologi er et klogt valg for en fremtidig karriere. Den indeholder eftertragtede jobs og erhverv, tips til at komme i gang og konkrete trin, der hjælper elever og studerende med at udforske deres interesser og udvikle digitale færdigheder. Materialet er et udgangspunkt for at vække nysgerrighed og guide de første skridt ind i teknologiens verden.</t>
+    <t>Uploaded 4 September 2025
+Infografikken viser de mest efterspurgte digitale karrierer og fremhæver, hvorfor teknologi er et klogt valg for en fremtidig karriere. Den indeholder eftertragtede jobs og erhverv, tips til at komme i gang og konkrete trin, der hjælper elever og studerende med at udforske deres interesser og udvikle digitale færdigheder. Materialet er et udgangspunkt for at vække nysgerrighed og guide de første skridt ind i teknologiens verden.</t>
   </si>
   <si>
     <t>Jouw gids voor digitale carrières</t>
   </si>
   <si>
-    <t>Deze inspirerende infographic biedt een overzicht van de belangrijkste digitale loopbaantrajecten en laat zien waarom technologie een slimme keuze is voor de toekomst. Inclusief gewilde functies, tips om te starten en praktische stappen om leerlingen te helpen hun interesses te verkennen en digitale vaardigheden te ontwikkelen. Perfect om nieuwsgierigheid te prikkelen en de eerste stappen in de techwereld te zetten.</t>
+    <t>Uploaded 4 September 2025
+Deze inspirerende infographic biedt een overzicht van de belangrijkste digitale loopbaantrajecten en laat zien waarom technologie een slimme keuze is voor de toekomst. Inclusief gewilde functies, tips om te starten en praktische stappen om leerlingen te helpen hun interesses te verkennen en digitale vaardigheden te ontwikkelen. Perfect om nieuwsgierigheid te prikkelen en de eerste stappen in de techwereld te zetten.</t>
   </si>
   <si>
     <t>Careers in Digital Infographic</t>
   </si>
   <si>
-    <t>This infographic provides an inspiring overview of the main career paths in tech and digital fields, showing why technology is a smart choice for the future. It highlights the most in-demand jobs, offers tips for getting started, and outlines concrete steps to help students explore their interests and develop their digital skills. Perfect for sparking curiosity and guiding the first steps into the tech world.</t>
+    <t>Uploaded 4 September 2025
+This infographic provides an inspiring overview of the main career paths in tech and digital fields, showing why technology is a smart choice for the future. It highlights the most in-demand jobs, offers tips for getting started, and outlines concrete steps to help students explore their interests and develop their digital skills. Perfect for sparking curiosity and guiding the first steps into the tech world.</t>
   </si>
   <si>
     <t>Guide des métiers de la tech et du numérique</t>
   </si>
   <si>
-    <t>Cette infographie offre un aperçu inspirant des principales voies de carrière dans la tech et le numérique, en montrant pourquoi la technologie est un choix d’avenir judicieux. Elle met en lumière les métiers les plus recherchés, donne des conseils pour se lancer et propose des étapes concrètes pour aider les élèves à explorer leurs intérêts et développer leurs compétences numériques. Parfait pour éveiller la curiosité et guider les premiers pas dans le monde technologique.</t>
+    <t>Uploaded 4 September 2025
+Cette infographie offre un aperçu inspirant des principales voies de carrière dans la tech et le numérique, en montrant pourquoi la technologie est un choix d’avenir judicieux. Elle met en lumière les métiers les plus recherchés, donne des conseils pour se lancer et propose des étapes concrètes pour aider les élèves à explorer leurs intérêts et développer leurs compétences numériques. Parfait pour éveiller la curiosité et guider les premiers pas dans le monde technologique.</t>
   </si>
   <si>
     <t>Careers in Digital – Wege zum Erfolg</t>
   </si>
   <si>
-    <t>Diese ansprechende Infografik bietet einen Überblick über Berufe im digitalen Bereich und zeigt, warum IT eine kluge Wahl für die Zukunft ist. Sie enthält gefragte Berufe, Tipps für den Einstieg und konkrete Schritte, die Schüler*innen helfen, ihre Interessen zu entdecken und digitale Kompetenzen zu entwickeln. Ideal, um Neugier zu wecken und erste Schritte in die IT-Welt zu begleiten.</t>
+    <t>Uploaded 4 September 2025
+Diese ansprechende Infografik bietet einen Überblick über Berufe im digitalen Bereich und zeigt, warum IT eine kluge Wahl für die Zukunft ist. Sie enthält gefragte Berufe, Tipps für den Einstieg und konkrete Schritte, die Schüler*innen helfen, ihre Interessen zu entdecken und digitale Kompetenzen zu entwickeln. Ideal, um Neugier zu wecken und erste Schritte in die IT-Welt zu begleiten.</t>
   </si>
   <si>
     <t>Ο οδηγός σας για ρταδιοδρομίες στον Ψηφιακό Τομέα</t>
   </si>
   <si>
-    <t>Μια εμπνευσμένη επισκόπηση των κορυφαίων ψηφιακών επαγγελματικών διαδρομών, αυτό το infographic αναδεικνύει γιατί η τεχνολογία είναι μια έξυπνη επιλογή για το μέλλον. Περιλαμβάνει επαγγέλματα με υψηλή ζήτηση, συμβουλές για να ξεκινήσει κανείς και πρακτικά βήματα για να βοηθήσει τους μαθητές να ανακαλύψουν τα ενδιαφέροντά τους και να αναπτύξουν ψηφιακές δεξιότητες. Ιδανικό για να ξυπνήσει την περιέργεια και να καθοδηγήσει τα πρώτα βήματα στον κόσμο της τεχνολογίας.</t>
+    <t>Uploaded 4 September 2025
+Μια εμπνευσμένη επισκόπηση των κορυφαίων ψηφιακών επαγγελματικών διαδρομών, αυτό το infographic αναδεικνύει γιατί η τεχνολογία είναι μια έξυπνη επιλογή για το μέλλον. Περιλαμβάνει επαγγέλματα με υψηλή ζήτηση, συμβουλές για να ξεκινήσει κανείς και πρακτικά βήματα για να βοηθήσει τους μαθητές να ανακαλύψουν τα ενδιαφέροντά τους και να αναπτύξουν ψηφιακές δεξιότητες. Ιδανικό για να ξυπνήσει την περιέργεια και να καθοδηγήσει τα πρώτα βήματα στον κόσμο της τεχνολογίας.</t>
   </si>
   <si>
     <t>La tua guida alle carriere digitali</t>
   </si>
   <si>
-    <t>Una panoramica ispiratrice dei principali percorsi di carriera digitale: questa infografica mostra perché la tecnologia è una scelta intelligente per il futuro. Include ruoli molto richiesti, consigli per iniziare e azioni concrete per aiutare gli studenti a esplorare i propri interessi e sviluppare competenze digitali. Perfetta per stimolare la curiosità e guidare i primi passi nel mondo tech.</t>
+    <t>Uploaded 4 September 2025
+Una panoramica ispiratrice dei principali percorsi di carriera digitale: questa infografica mostra perché la tecnologia è una scelta intelligente per il futuro. Include ruoli molto richiesti, consigli per iniziare e azioni concrete per aiutare gli studenti a esplorare i propri interessi e sviluppare competenze digitali. Perfetta per stimolare la curiosità e guidare i primi passi nel mondo tech.</t>
   </si>
   <si>
     <t>Tavs ceļvedis digitālajām karjerām</t>
   </si>
   <si>
-    <t>Iedvesmojošs pārskats par populārākajām digitālajām karjerām — šī infografika izceļ, kāpēc tehnoloģijas ir gudra izvēle nākotnei. Tajā iekļautas pieprasītas profesijas, padomi, kā sākt, un konkrēti soļi, kas palīdz skolēniem izzināt intereses un attīstīt digitālās prasmes. Ideāli piemērots zinātkāres veicināšanai un pirmajiem soļiem tehnoloģiju pasaulē.</t>
+    <t>Uploaded 4 September 2025
+Iedvesmojošs pārskats par populārākajām digitālajām karjerām — šī infografika izceļ, kāpēc tehnoloģijas ir gudra izvēle nākotnei. Tajā iekļautas pieprasītas profesijas, padomi, kā sākt, un konkrēti soļi, kas palīdz skolēniem izzināt intereses un attīstīt digitālās prasmes. Ideāli piemērots zinātkāres veicināšanai un pirmajiem soļiem tehnoloģiju pasaulē.</t>
   </si>
   <si>
     <t>Jūsų karjeros skaitmeninėje srityje vadovas</t>
   </si>
   <si>
-    <t>Įkvepiantis infografikas, kuriame pateikiamos populiariausios skaitmeninės profesijos ir paaiškinama, kodėl technologijos yra protingas ateities pasirinkimas. Jame pateikiamos paklausios profesijos, patarimai, kaip pradėti dirbti, ir konkretūs veiksmai, padedantys mokiniams tyrinėti savo interesus ir tobulinti skaitmeninius įgūdžius. Puikiai tinka sužadinti smalsumą ir žengti pirmąjį žingsnį į technologijų pasaulį.</t>
+    <t>Uploaded 4 September 2025
+Įkvepiantis infografikas, kuriame pateikiamos populiariausios skaitmeninės profesijos ir paaiškinama, kodėl technologijos yra protingas ateities pasirinkimas. Jame pateikiamos paklausios profesijos, patarimai, kaip pradėti dirbti, ir konkretūs veiksmai, padedantys mokiniams tyrinėti savo interesus ir tobulinti skaitmeninius įgūdžius. Puikiai tinka sužadinti smalsumą ir žengti pirmąjį žingsnį į technologijų pasaulį.</t>
   </si>
   <si>
     <t>Il-Gwida Tiegħek għall-Karriera Diġitali</t>
   </si>
   <si>
-    <t>Ħarsa ispiranti lejn l-aqwa toroq ta’ karriera diġitali – din l-infografika tenfasizza għaliex it-teknoloġija hija għażla intelliġenti għall-futur. Tinkludi rwoli mfittxija, pariri biex tibda u passi prattiċi biex tgħin lill-istudenti jesploraw l-interessi tagħhom u jkabbru l-ħiliet diġitali. Perfetta biex tqanqal il-kurżità u tiggwida l-ewwel passi fid-dinja tat-teknoloġija.</t>
+    <t>Uploaded 4 September 2025
+Ħarsa ispiranti lejn l-aqwa toroq ta’ karriera diġitali – din l-infografika tenfasizza għaliex it-teknoloġija hija għażla intelliġenti għall-futur. Tinkludi rwoli mfittxija, pariri biex tibda u passi prattiċi biex tgħin lill-istudenti jesploraw l-interessi tagħhom u jkabbru l-ħiliet diġitali. Perfetta biex tqanqal il-kurżità u tiggwida l-ewwel passi fid-dinja tat-teknoloġija.</t>
   </si>
   <si>
     <t>Twój przewodnik po karierach cyfrowych</t>
   </si>
   <si>
-    <t>Inspirujący przegląd najważniejszych ścieżek kariery cyfrowej – ta infografika pokazuje, dlaczego technologia to mądry wybór na przyszłość. Zawiera poszukiwane role, wskazówki na start i konkretne kroki, które pomogą uczniom odkrywać swoje zainteresowania i rozwijać kompetencje cyfrowe. Idealna, by wzbudzić ciekawość i pokierować pierwszymi krokami w świecie technologii.</t>
+    <t>Uploaded 4 September 2025
+Inspirujący przegląd najważniejszych ścieżek kariery cyfrowej – ta infografika pokazuje, dlaczego technologia to mądry wybór na przyszłość. Zawiera poszukiwane role, wskazówki na start i konkretne kroki, które pomogą uczniom odkrywać swoje zainteresowania i rozwijać kompetencje cyfrowe. Idealna, by wzbudzić ciekawość i pokierować pierwszymi krokami w świecie technologii.</t>
   </si>
   <si>
     <t>Infográfico sobre Carreiras no Mundo Digital</t>
   </si>
   <si>
-    <t>Este infográfico oferece uma visão geral inspiradora dos principais caminhos profissionais nas áreas de tecnologia e digital, mostrando por que a tecnologia é uma escolha inteligente para o futuro. Ele destaca as profissões mais procuradas, fornece dicas para começar e apresenta passos concretos para ajudar os estudantes a explorar seus interesses e desenvolver suas competências digitais. Perfeito para despertar a curiosidade e orientar os primeiros passos no mundo da tecnologia.</t>
+    <t>Uploaded 4 September 2025
+Este infográfico oferece uma visão geral inspiradora dos principais caminhos profissionais nas áreas de tecnologia e digital, mostrando por que a tecnologia é uma escolha inteligente para o futuro. Ele destaca as profissões mais procuradas, fornece dicas para começar e apresenta passos concretos para ajudar os estudantes a explorar seus interesses e desenvolver suas competências digitais. Perfeito para despertar a curiosidade e orientar os primeiros passos no mundo da tecnologia.</t>
   </si>
   <si>
     <t xml:space="preserve">Ghidul tău pentru cariere digitale 
 </t>
   </si>
   <si>
-    <t>O prezentare generală de inspirație a principalelor căi în a obține o carieră digitală – această infografică evidențiază de ce tehnologia este o alegere inteligentă pentru viitor. Include roluri des căutate, sfaturi pentru început și pași practici care îi ajută pe elevi să își descopere interesele și să-și dezvolte abilitățile digitale. Perfect pentru a trezi curiozitatea și a ghida primii pași în lumea tehnologiei.</t>
+    <t>Uploaded 4 September 2025
+O prezentare generală de inspirație a principalelor căi în a obține o carieră digitală – această infografică evidențiază de ce tehnologia este o alegere inteligentă pentru viitor. Include roluri des căutate, sfaturi pentru început și pași practici care îi ajută pe elevi să își descopere interesele și să-și dezvolte abilitățile digitale. Perfect pentru a trezi curiozitatea și a ghida primii pași în lumea tehnologiei.</t>
   </si>
   <si>
     <t>Váš sprievodca kariérou v digitálnom svete</t>
   </si>
   <si>
-    <t>Infografika predstavuje najžiadanejšie digitálne kariéry a zdôrazňuje, prečo je technológia múdra voľba pre budúcu kariéru. Obsahuje vyhľadávané pracovné pozície a povolania, tipy na začiatok a konkrétne kroky, ktoré pomáhajú žiakom a študentom preskúmať svoje záujmy a rozvíjať digitálne zručnosti.Materiál je východiskovým bodom na podporu zvedavosti a usmernenie prvých krokov do sveta technológií.</t>
+    <t>Uploaded 4 September 2025
+Infografika predstavuje najžiadanejšie digitálne kariéry a zdôrazňuje, prečo je technológia múdra voľba pre budúcu kariéru. Obsahuje vyhľadávané pracovné pozície a povolania, tipy na začiatok a konkrétne kroky, ktoré pomáhajú žiakom a študentom preskúmať svoje záujmy a rozvíjať digitálne zručnosti.Materiál je východiskovým bodom na podporu zvedavosti a usmernenie prvých krokov do sveta technológií.</t>
   </si>
   <si>
     <t>Tvoj vodnik za kariere v digitalnem svetu</t>
   </si>
   <si>
-    <t>Infografika prikazuje najbolj iskane digitalne poklice in poudarja, zakaj je tehnologija pametna izbira za prihodnjo kariero. Vsebuje iskana delovna mesta, nasvete za začetek in konkretne korake, ki pomagajo učencem in študentom raziskovati svoje interese ter razvijati digitalne kompetence. Gradivo je izhodiščna točka za spodbujanje radovednosti in usmerjanje prvih korakov v svet tehnologije.</t>
+    <t>Uploaded 4 September 2025
+Infografika prikazuje najbolj iskane digitalne poklice in poudarja, zakaj je tehnologija pametna izbira za prihodnjo kariero. Vsebuje iskana delovna mesta, nasvete za začetek in konkretne korake, ki pomagajo učencem in študentom raziskovati svoje interese ter razvijati digitalne kompetence. Gradivo je izhodiščna točka za spodbujanje radovednosti in usmerjanje prvih korakov v svet tehnologije.</t>
   </si>
   <si>
     <t>Tu guía para carreras en el mundo digital</t>
   </si>
   <si>
-    <t>La infografía muestra las profesiones digitales más demandadas y destaca por qué la tecnología es una elección inteligente para una carrera futura. Incluye empleos solicitados, consejos para empezar y pasos concretos que ayudan a los alumnos y estudiantes a explorar sus intereses y desarrollar competencias digitales. Es un punto de partida ideal para despertar la curiosidad y orientar los primeros pasos en el mundo de la tecnología.</t>
+    <t>Uploaded 4 September 2025
+La infografía muestra las profesiones digitales más demandadas y destaca por qué la tecnología es una elección inteligente para una carrera futura. Incluye empleos solicitados, consejos para empezar y pasos concretos que ayudan a los alumnos y estudiantes a explorar sus intereses y desarrollar competencias digitales. Es un punto de partida ideal para despertar la curiosidad y orientar los primeros pasos en el mundo de la tecnología.</t>
   </si>
   <si>
     <t>Oppaasi digitaalisen maailman uramahdollisuuksiin</t>
   </si>
   <si>
-    <t>Infografiikka esittelee kysytyimmät digitaaliset urat ja korostaa, miksi teknologia on viisas valinta tulevaisuuden uralle. Se sisältää kysyttyjä ammatteja, vinkkejä aloittamiseen ja konkreettisia askeleita, jotka auttavat oppilaita ja opiskelijoita tutkimaan omia kiinnostuksen kohteitaan ja kehittämään digitaalisia taitoja. Materiaali toimii lähtökohtana uteliaisuuden herättämiselle ja ensimmäisten askelten ohjaamiselle teknologiamaailmaan.</t>
+    <t>Uploaded 4 September 2025
+Infografiikka esittelee kysytyimmät digitaaliset urat ja korostaa, miksi teknologia on viisas valinta tulevaisuuden uralle. Se sisältää kysyttyjä ammatteja, vinkkejä aloittamiseen ja konkreettisia askeleita, jotka auttavat oppilaita ja opiskelijoita tutkimaan omia kiinnostuksen kohteitaan ja kehittämään digitaalisia taitoja. Materiaali toimii lähtökohtana uteliaisuuden herättämiselle ja ensimmäisten askelten ohjaamiselle teknologiamaailmaan.</t>
   </si>
   <si>
     <t>Din guide till karriärer i den digitala världen</t>
   </si>
   <si>
-    <t>Infografiken visar de mest efterfrågade digitala karriärerna och lyfter fram varför teknik är ett smart val för en framtida karriär. Den innehåller eftertraktade jobb och yrken, tips för att komma igång samt konkreta steg som hjälper elever och studenter att utforska sina intressen och utveckla digitala färdigheter. Materialet är en utgångspunkt för att väcka nyfikenhet och vägleda de första stegen in i teknikens värld.</t>
+    <t>Uploaded 4 September 2025
+Infografiken visar de mest efterfrågade digitala karriärerna och lyfter fram varför teknik är ett smart val för en framtida karriär. Den innehåller eftertraktade jobb och yrken, tips för att komma igång samt konkreta steg som hjälper elever och studenter att utforska sina intressen och utveckla digitala färdigheter. Materialet är en utgångspunkt för att väcka nyfikenhet och vägleda de första stegen in i teknikens värld.</t>
   </si>
   <si>
     <t>Dijital Kariyerler Rehberiniz</t>
   </si>
   <si>
-    <t>En popüler dijital kariyer yollarına ilham verici bir bakış sunan bu infografik, teknolojinin neden geleceğe yönelik akıllı bir seçim olduğunu vurguluyor. Talep gören roller, başlamaya yönelik ipuçları ve öğrencilerin ilgi alanlarını keşfetmesine ve dijital becerilerini geliştirmesine yardımcı olacak somut adımlar içerir. Merak uyandırmak ve teknoloji dünyasına ilk adımları yönlendirmek için mükemmel bir araçtır.</t>
+    <t>Uploaded 4 September 2025
+En popüler dijital kariyer yollarına ilham verici bir bakış sunan bu infografik, teknolojinin neden geleceğe yönelik akıllı bir seçim olduğunu vurguluyor. Talep gören roller, başlamaya yönelik ipuçları ve öğrencilerin ilgi alanlarını keşfetmesine ve dijital becerilerini geliştirmesine yardımcı olacak somut adımlar içerir. Merak uyandırmak ve teknoloji dünyasına ilk adımları yönlendirmek için mükemmel bir araçtır.</t>
   </si>
   <si>
     <t>Ваш гід у світ цифрових кар’єр</t>
   </si>
   <si>
-    <t>Натхненна інфографіка, що знайомить з найпопулярнішими цифровими професіями і пояснює, чому технології — це вибір майбутнього. У ній ви знайдете перелік затребуваних спеціальностей, корисні поради для старту та практичні кроки, які допоможуть учням дослідити свої інтереси й розвинути цифрові навички. Ідеальний інструмент для пробудження інтересу та першого кроку у сферу технологій.</t>
+    <t>Uploaded 4 September 2025
+Натхненна інфографіка, що знайомить з найпопулярнішими цифровими професіями і пояснює, чому технології — це вибір майбутнього. У ній ви знайдете перелік затребуваних спеціальностей, корисні поради для старту та практичні кроки, які допоможуть учням дослідити свої інтереси й розвинути цифрові навички. Ідеальний інструмент для пробудження інтересу та першого кроку у сферу технологій.</t>
   </si>
   <si>
     <t>Krijo çelësin tënd për mësuesit</t>
   </si>
   <si>
-    <t>Ky aktivitet praktik prezanton nxënësit me modelimin 3D duke përdorur Tinkercad përmes udhëzimeve për krijimin e një çelësi personal. Ideale për një sesion njëorësh, ky mjet ndihmon në zhvillimin e krijimtarisë, mendimit projektues dhe aftësive digjitale – nuk kërkohet përvojë e mëparshme. E përshtatshme për klasat, klubet apo hapësirat "lab".</t>
+    <t>Uploaded 4 September 2025
+Ky aktivitet praktik prezanton nxënësit me modelimin 3D duke përdorur Tinkercad përmes udhëzimeve për krijimin e një çelësi personal. Ideale për një sesion njëorësh, ky mjet ndihmon në zhvillimin e krijimtarisë, mendimit projektues dhe aftësive digjitale – nuk kërkohet përvojë e mëparshme. E përshtatshme për klasat, klubet apo hapësirat "lab".</t>
   </si>
   <si>
     <t>Създай свой ключодържател за учители</t>
   </si>
   <si>
-    <t>Тази практическа дейност запознава учениците с 3D моделирането чрез Tinkercad, като ги насочва към създаването на персонализиран ключодържател. Подходяща за едночасова сесия, тя развива креативност, дизайнерско мислене и дигитални умения – не се изисква предишен опит. Идеална за класни стаи, клубове или „maker“ пространства.</t>
+    <t>Uploaded 4 September 2025
+Тази практическа дейност запознава учениците с 3D моделирането чрез Tinkercad, като ги насочва към създаването на персонализиран ключодържател. Подходяща за едночасова сесия, тя развива креативност, дизайнерско мислене и дигитални умения – не се изисква предишен опит. Идеална за класни стаи, клубове или „maker“ пространства.</t>
   </si>
   <si>
     <t>Izradi svoj privjesak za ključeve - za učitelje i nastavnike</t>
   </si>
   <si>
-    <t>Ova praktična aktivnost uvodi učenike u 3D modeliranje pomoću alata Tinkercad, vodeći ih kroz izradu personaliziranog privjeska. Aktivnost traje sat vremena. Potiče kreativnost, dizajnersko razmišljanje i digitalne vještine – prethodno iskustvo nije potrebno. Prikladna je za učionice, klubove ili makerspace prostore.</t>
+    <t>Uploaded 4 September 2025
+Ova praktična aktivnost uvodi učenike u 3D modeliranje pomoću alata Tinkercad, vodeći ih kroz izradu personaliziranog privjeska. Aktivnost traje sat vremena. Potiče kreativnost, dizajnersko razmišljanje i digitalne vještine – prethodno iskustvo nije potrebno. Prikladna je za učionice, klubove ili makerspace prostore.</t>
   </si>
   <si>
     <t xml:space="preserve">Vytvoř si vlastní klíčenku pro učitele
 </t>
   </si>
   <si>
-    <t>Tato praktická aktivita seznamuje studenty s 3D modelováním v programu Tinkercad skrze tvorbu vlastního personalizovaného přívěsku na klíče. Ideální pro hodinovou lekci, rozvíjí kreativitu, designové myšlení a digitální dovednosti – žádné předchozí zkušenosti nejsou nutné. Skvělé pro třídy, kroužky nebo makerspace prostředí.</t>
+    <t>Uploaded 4 September 2025
+Tato praktická aktivita seznamuje studenty s 3D modelováním v programu Tinkercad skrze tvorbu vlastního personalizovaného přívěsku na klíče. Ideální pro hodinovou lekci, rozvíjí kreativitu, designové myšlení a digitální dovednosti – žádné předchozí zkušenosti nejsou nutné. Skvělé pro třídy, kroužky nebo makerspace prostředí.</t>
   </si>
   <si>
     <t>Lav din egen nøglering til undervisere</t>
   </si>
   <si>
-    <t>Denne praktiske aktivitet introducerer eleverne til 3D-modellering med Tinkercad gennem design af en personlig nøglering. Perfekt til en lektion på én time, den styrker kreativitet, designtænkning og digitale færdigheder – ingen tidligere erfaring kræves. Ideel til klasselokaler, klubber eller makerspaces.</t>
+    <t>Uploaded 4 September 2025
+Denne praktiske aktivitet introducerer eleverne til 3D-modellering med Tinkercad gennem design af en personlig nøglering. Perfekt til en lektion på én time, den styrker kreativitet, designtænkning og digitale færdigheder – ingen tidligere erfaring kræves. Ideel til klasselokaler, klubber eller makerspaces.</t>
   </si>
   <si>
     <t>Maak je eigen sleutelhanger voor docenten</t>
   </si>
   <si>
-    <t>Deze praktische activiteit laat leerlingen kennismaken met 3D-modelleren in Tinkercad via het maken van een gepersonaliseerde sleutelhanger. Perfect voor een sessie van een uur, het bevordert creativiteit, ontwerpdenken en digitale vaardigheden – geen ervaring vereist. Ideaal voor klaslokalen, clubs of makerspaces.</t>
-  </si>
-  <si>
-    <t>Create your keychain for educators</t>
-  </si>
-  <si>
-    <t>This hands-on activity introduces students to 3D modeling using Tinkercad by guiding them through the creation of a personalized keychain. Ideal for a one-hour session, it builds creativity, design thinking, and digital skills—no prior experience needed. Perfect for classrooms, clubs, or maker spaces.</t>
+    <t>Uploaded 4 September 2025
+Deze praktische activiteit laat leerlingen kennismaken met 3D-modelleren in Tinkercad via het maken van een gepersonaliseerde sleutelhanger. Perfect voor een sessie van een uur, het bevordert creativiteit, ontwerpdenken en digitale vaardigheden – geen ervaring vereist. Ideaal voor klaslokalen, clubs of makerspaces.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create your keychain for educators </t>
+  </si>
+  <si>
+    <t>Uploaded 4 September 2025
+This hands-on activity introduces students to 3D modeling using Tinkercad by guiding them through the creation of a personalized keychain. Ideal for a one-hour session, it builds creativity, design thinking, and digital skills—no prior experience needed. Perfect for classrooms, clubs, or maker spaces.</t>
   </si>
   <si>
     <t>Crée ton porte-clés - Ressource pour les éducateurs</t>
   </si>
   <si>
-    <t>Cette activité pratique initie les élèves à la modélisation 3D avec Tinkercad en les guidant dans la création d’un porte-clés personnalisé. Parfaite pour une session d’une heure, elle développe la créativité, la pensée design et les compétences numériques – aucune expérience préalable n’est requise. Idéal pour les classes, clubs ou Fablabs.</t>
+    <t>Uploaded 4 September 2025
+Cette activité pratique initie les élèves à la modélisation 3D avec Tinkercad en les guidant dans la création d’un porte-clés personnalisé. Parfaite pour une session d’une heure, elle développe la créativité, la pensée design et les compétences numériques – aucune expérience préalable n’est requise. Idéal pour les classes, clubs ou Fablabs.</t>
   </si>
   <si>
     <t>Erstelle deinen eigenen Schlüsselanhänger - für Lehrkräfte</t>
   </si>
   <si>
-    <t xml:space="preserve"> Diese praxisorientierte Aktivität führt Schüler*innen spielerisch in die Welt des 3D-Designs mit Tinkercad ein. Durch die Gestaltung eines personalisierten Schlüsselanhängers entwickeln sie Kreativität, Design Thinking und digitale Kompetenzen – ganz ohne Vorkenntnisse. Die Aktivität ist auf eine Dauer von ca. 60 Minuten ausgelegt und eignet sich ideal für den Einsatz im Klassenzimmer, in AGs oder Maker Spaces.</t>
+    <t>Uploaded 4 September 2025
+ Diese praxisorientierte Aktivität führt Schüler*innen spielerisch in die Welt des 3D-Designs mit Tinkercad ein. Durch die Gestaltung eines personalisierten Schlüsselanhängers entwickeln sie Kreativität, Design Thinking und digitale Kompetenzen – ganz ohne Vorkenntnisse. Die Aktivität ist auf eine Dauer von ca. 60 Minuten ausgelegt und eignet sich ideal für den Einsatz im Klassenzimmer, in AGs oder Maker Spaces.</t>
   </si>
   <si>
     <t>Δημιούργηστε το μπρελόκ σας για εκπαιδευτικούς</t>
   </si>
   <si>
-    <t>Αυτή η βιωματική δραστηριότητα εισάγει τους μαθητές στη 3D μοντελοποίηση μέσω του Tinkercad, καθοδηγώντας τους στη δημιουργία ενός εξατομικευμένου μπρελόκ. Ιδανικό για μια συνεδρία μίας ώρας, ενισχύει τη δημιουργικότητα, τη σχεδιαστική σκέψη και τις ψηφιακές δεξιότητες – δεν απαιτείται προηγούμενη εμπειρία. Κατάλληλο για τάξεις, λέσχες ή maker spaces.</t>
+    <t>Uploaded 4 September 2025
+Αυτή η βιωματική δραστηριότητα εισάγει τους μαθητές στη 3D μοντελοποίηση μέσω του Tinkercad, καθοδηγώντας τους στη δημιουργία ενός εξατομικευμένου μπρελόκ. Ιδανικό για μια συνεδρία μίας ώρας, ενισχύει τη δημιουργικότητα, τη σχεδιαστική σκέψη και τις ψηφιακές δεξιότητες – δεν απαιτείται προηγούμενη εμπειρία. Κατάλληλο για τάξεις, λέσχες ή maker spaces.</t>
   </si>
   <si>
     <t>Crea il tuo portachiavi - per insegnanti</t>
   </si>
   <si>
-    <t>Questa attività pratica introduce gli studenti alla modellazione 3D con Tinkercad guidandoli nella creazione di un portachiavi personalizzato. Perfetta per una sessione di un’ora, sviluppa creatività, pensiero progettuale e competenze digitali – non è richiesta esperienza pregressa. Ideale per classi, club o spazi creativi.</t>
+    <t>Uploaded 4 September 2025
+Questa attività pratica introduce gli studenti alla modellazione 3D con Tinkercad guidandoli nella creazione di un portachiavi personalizzato. Perfetta per una sessione di un’ora, sviluppa creatività, pensiero progettuale e competenze digitali – non è richiesta esperienza pregressa. Ideale per classi, club o spazi creativi.</t>
   </si>
   <si>
     <t>Izveido savu atslēgu piekariņu pedagogiem</t>
   </si>
   <si>
-    <t xml:space="preserve"> Šī praktiskā aktivitāte iepazīstina skolēnus ar 3D modelēšanu, izmantojot Tinkercad, vadot viņus cauri personalizēta atslēgu piekariņa izveidei. Ideāli piemērota stundas ilgai nodarbībai, tā attīsta radošumu, dizaina domāšanu un digitālās prasmes — iepriekšēja pieredze nav nepieciešama. Lieliski piemērota klases nodarbībām, pulciņiem vai radošajām darbnīcām.</t>
+    <t>Uploaded 4 September 2025
+ Šī praktiskā aktivitāte iepazīstina skolēnus ar 3D modelēšanu, izmantojot Tinkercad, vadot viņus cauri personalizēta atslēgu piekariņa izveidei. Ideāli piemērota stundas ilgai nodarbībai, tā attīsta radošumu, dizaina domāšanu un digitālās prasmes — iepriekšēja pieredze nav nepieciešama. Lieliski piemērota klases nodarbībām, pulciņiem vai radošajām darbnīcām.</t>
   </si>
   <si>
     <t>Sukurk savo raktų pakabuką (mokytojams)</t>
   </si>
   <si>
-    <t xml:space="preserve"> ši praktinė veikla kuriant asmeninį raktų pakabuką supažindina mokinius su trimačio modeliavimo „Tinkercad“ aplinkoje pagrindais. Puikiai tinka vienos valandos pamokai – ugdo kūrybiškumą, projektinį mąstymą ir skaitmeninius įgūdžius. Ankstesnė patirtis nereikalinga. Puikiai tinka klasėms, būreliams ar kūrybinėms dirbtuvėms.</t>
+    <t>Uploaded 4 September 2025
+ ši praktinė veikla kuriant asmeninį raktų pakabuką supažindina mokinius su trimačio modeliavimo „Tinkercad“ aplinkoje pagrindais. Puikiai tinka vienos valandos pamokai – ugdo kūrybiškumą, projektinį mąstymą ir skaitmeninius įgūdžius. Ankstesnė patirtis nereikalinga. Puikiai tinka klasėms, būreliams ar kūrybinėms dirbtuvėms.</t>
   </si>
   <si>
     <t>Oħloq keychain tiegħek għall-edukaturi</t>
   </si>
   <si>
-    <t>Din l-attività prattika tintroduċi lill-istudenti għall-immudellar 3D billi jużaw Tinkercad biex joħolqu keychain personalizzat. Ideali għal sessjoni ta’ siegħa, tiżviluppa l-kreattività, il-ħsieb tad-disinn u ħiliet diġitali – ma hemmx bżonn ta’ esperjenza minn qabel. Perfetta għall-klassijiet, klabbs jew makerspaces.</t>
+    <t>Uploaded 4 September 2025
+Din l-attività prattika tintroduċi lill-istudenti għall-immudellar 3D billi jużaw Tinkercad biex joħolqu keychain personalizzat. Ideali għal sessjoni ta’ siegħa, tiżviluppa l-kreattività, il-ħsieb tad-disinn u ħiliet diġitali – ma hemmx bżonn ta’ esperjenza minn qabel. Perfetta għall-klassijiet, klabbs jew makerspaces.</t>
   </si>
   <si>
     <t>Stwórz własny brelok dla nauczycieli</t>
   </si>
   <si>
-    <t>Ta praktyczna aktywność wprowadza uczniów w modelowanie 3D przy użyciu programu Tinkercad, prowadząc ich przez tworzenie spersonalizowanego breloka. Idealna na godzinne zajęcia, rozwija kreatywność, myślenie projektowe i umiejętności cyfrowe – nie wymaga wcześniejszego doświadczenia. Doskonała do klas, kółek zainteresowań i pracowni technicznych.</t>
+    <t>Uploaded 4 September 2025
+Ta praktyczna aktywność wprowadza uczniów w modelowanie 3D przy użyciu programu Tinkercad, prowadząc ich przez tworzenie spersonalizowanego breloka. Idealna na godzinne zajęcia, rozwija kreatywność, myślenie projektowe i umiejętności cyfrowe – nie wymaga wcześniejszego doświadczenia. Doskonała do klas, kółek zainteresowań i pracowni technicznych.</t>
   </si>
   <si>
     <t>Cria o teu porta-chaves para professores</t>
   </si>
   <si>
-    <t xml:space="preserve"> Esta atividade prática apresenta aos alunos a modelação 3D com o Tinkercad, guiando-os na criação de um porta-chaves personalizado. Ideal para uma sessão de uma hora, desenvolve criatividade, pensamento de design e competências digitais – não é necessária experiência prévia. Perfeita para salas de aula, clubes ou espaços criativos.</t>
+    <t>Uploaded 4 September 2025
+ Esta atividade prática apresenta aos alunos a modelação 3D com o Tinkercad, guiando-os na criação de um porta-chaves personalizado. Ideal para uma sessão de uma hora, desenvolve criatividade, pensamento de design e competências digitais – não é necessária experiência prévia. Perfeita para salas de aula, clubes ou espaços criativos.</t>
   </si>
   <si>
     <t>Creează brelocul tău pentru profesori</t>
   </si>
   <si>
-    <t>Această activitate practică le prezintă elevilor modelarea 3D folosind Tinkercad, ghidându-i în crearea unui breloc personalizat. Ideală pentru o sesiune de o oră, dezvoltă creativitatea, gândirea orientată spre soluții  și abilitățile digitale – nu este necesară experiență anterioară. Perfectă pentru școală, cluburi sau spații de creație.</t>
+    <t>Uploaded 4 September 2025
+Această activitate practică le prezintă elevilor modelarea 3D folosind Tinkercad, ghidându-i în crearea unui breloc personalizat. Ideală pentru o sesiune de o oră, dezvoltă creativitatea, gândirea orientată spre soluții  și abilitățile digitale – nu este necesară experiență anterioară. Perfectă pentru școală, cluburi sau spații de creație.</t>
   </si>
   <si>
     <t xml:space="preserve">Vytvor si vlastný prívesok pre učiteľov
 </t>
   </si>
   <si>
-    <t>Táto praktická aktivita predstavuje žiakom 3D modelovanie v programe Tinkercad prostredníctvom tvorby personalizovaného prívesku na kľúče. Ideálna na 60-minútovú hodinu, rozvíja kreativitu, dizajnové myslenie a digitálne zručnosti – bez potreby predchádzajúcich skúseností. Vhodná do triedy, krúžku alebo makerspace.</t>
+    <t>Uploaded 4 September 2025
+Táto praktická aktivita predstavuje žiakom 3D modelovanie v programe Tinkercad prostredníctvom tvorby personalizovaného prívesku na kľúče. Ideálna na 60-minútovú hodinu, rozvíja kreativitu, dizajnové myslenie a digitálne zručnosti – bez potreby predchádzajúcich skúseností. Vhodná do triedy, krúžku alebo makerspace.</t>
   </si>
   <si>
     <t>Ustvari svoj obesek za ključe -  za učitelje</t>
   </si>
   <si>
-    <t>Ta praktična aktivnost  uvaja učence v 3D modeliranje z orodjem Tinkercad, vodi jih skozi izdelavo personaliziranega obeska. Aktivnost traja eno uro. Spodbuja ustvarjalnost, oblikovalski način razmišljanja in digitalne spretnosti – predhodne izkušnje niso potrebne. Primerna je za učilnice, krožke ali makerspace prostore.</t>
+    <t>Uploaded 4 September 2025
+Ta praktična aktivnost  uvaja učence v 3D modeliranje z orodjem Tinkercad, vodi jih skozi izdelavo personaliziranega obeska. Aktivnost traja eno uro. Spodbuja ustvarjalnost, oblikovalski način razmišljanja in digitalne spretnosti – predhodne izkušnje niso potrebne. Primerna je za učilnice, krožke ali makerspace prostore.</t>
   </si>
   <si>
     <t>Crea tu llavero - para docentes</t>
   </si>
   <si>
-    <t>Esta actividad práctica introduce a los estudiantes al modelado 3D con Tinkercad guiándolos en la creación de un llavero personalizado. Ideal para una sesión de una hora, fomenta la creatividad, el pensamiento de diseño y las habilidades digitales – no se requiere experiencia previa. Perfecto para clases, clubes o espacios maker.</t>
+    <t>Uploaded 4 September 2025
+Esta actividad práctica introduce a los estudiantes al modelado 3D con Tinkercad guiándolos en la creación de un llavero personalizado. Ideal para una sesión de una hora, fomenta la creatividad, el pensamiento de diseño y las habilidades digitales – no se requiere experiencia previa. Perfecto para clases, clubes o espacios maker.</t>
   </si>
   <si>
     <t>Luo oma avaimenperä opettajille</t>
   </si>
   <si>
-    <t>Tämä käytännönläheinen tehtävä tutustuttaa oppilaat 3D-mallinnukseen Tinkercadin avulla ohjaamalla heidät oman personoidun avaimenperän suunnitteluun. Sopii yhden oppitunnin mittaiseksi työksi ja kehittää luovuutta, suunnittelulähtöistä ajattelua ja digitaalisia taitoja – aiempaa kokemusta ei tarvita. Erinomainen luokkahuoneisiin, kerhoihin ja maker-tiloihin.</t>
+    <t>Uploaded 4 September 2025
+Tämä käytännönläheinen tehtävä tutustuttaa oppilaat 3D-mallinnukseen Tinkercadin avulla ohjaamalla heidät oman personoidun avaimenperän suunnitteluun. Sopii yhden oppitunnin mittaiseksi työksi ja kehittää luovuutta, suunnittelulähtöistä ajattelua ja digitaalisia taitoja – aiempaa kokemusta ei tarvita. Erinomainen luokkahuoneisiin, kerhoihin ja maker-tiloihin.</t>
   </si>
   <si>
     <t>Skapa din nyckelring för lärare</t>
   </si>
   <si>
-    <t>Denna praktiska aktivitet introducerar elever till 3D-modellering i Tinkercad genom att vägleda dem i att skapa en personlig nyckelring. Perfekt för en lektion på en timme – den utvecklar kreativitet, design thinking och digitala färdigheter. Ingen tidigare erfarenhet krävs. Perfekt för klassrum, klubbar eller makerspaces.</t>
+    <t>Uploaded 4 September 2025
+Denna praktiska aktivitet introducerar elever till 3D-modellering i Tinkercad genom att vägleda dem i att skapa en personlig nyckelring. Perfekt för en lektion på en timme – den utvecklar kreativitet, design thinking och digitala färdigheter. Ingen tidigare erfarenhet krävs. Perfekt för klassrum, klubbar eller makerspaces.</t>
   </si>
   <si>
     <t>Eğitimciler için anahtarlığınızı yaratın</t>
   </si>
   <si>
-    <t>Bu uygulamalı etkinlik, öğrencilere kişiselleştirilmiş bir anahtarlık oluşturma konusunda rehberlik ederek Tinkercad kullanarak 3D modellemeyi öğretir. Bir saatlik bir oturum için idealdir ve yaratıcılık, tasarım odaklı düşünme ve dijital becerileri geliştirir; önceden deneyim gerektirmez. Sınıflar, kulüpler veya üretim alanları için idealdir.</t>
+    <t>Uploaded 4 September 2025
+Bu uygulamalı etkinlik, öğrencilere kişiselleştirilmiş bir anahtarlık oluşturma konusunda rehberlik ederek Tinkercad kullanarak 3D modellemeyi öğretir. Bir saatlik bir oturum için idealdir ve yaratıcılık, tasarım odaklı düşünme ve dijital becerileri geliştirir; önceden deneyim gerektirmez. Sınıflar, kulüpler veya üretim alanları için idealdir.</t>
   </si>
   <si>
     <t>Створи свій брелок для вчителів</t>
   </si>
   <si>
-    <t>Ця практична діяльність знайомить здобувачів освіти з 3D-моделюванням у Tinkercad, крок за кроком навчаючи створювати персоналізований брелок. Ідеально підходить для одногодинного заняття, розвиває креативність, дизайнерське мислення та цифрові навички — попередній досвід не потрібен. Чудово підходить для класних занять, гуртків або майстерень.</t>
-  </si>
-  <si>
-    <t>Krijo çelësin tënd për nxënësit</t>
-  </si>
-  <si>
-    <t>Një udhëzues vizual hap pas hapi që ndihmon nxënësit të krijojnë çelësin e tyre personal duke përdorur Tinkercad. Nga zgjedhja e shkronjave deri te personalizimi dhe eksportimi për printim 3D, ky aktivitet nxit krijimtarinë dhe punën praktike digjitale – perfekte për përdorim në klasë apo në hapësira krijuese.</t>
+    <t>Uploaded 4 September 2025
+Ця практична діяльність знайомить здобувачів освіти з 3D-моделюванням у Tinkercad, крок за кроком навчаючи створювати персоналізований брелок. Ідеально підходить для одногодинного заняття, розвиває креативність, дизайнерське мислення та цифрові навички — попередній досвід не потрібен. Чудово підходить для класних занять, гуртків або майстерень.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Krijo çelësin tënd për nxënësit </t>
+  </si>
+  <si>
+    <t>Uploaded 4 September 2025
+Një udhëzues vizual hap pas hapi që ndihmon nxënësit të krijojnë çelësin e tyre personal duke përdorur Tinkercad. Nga zgjedhja e shkronjave deri te personalizimi dhe eksportimi për printim 3D, ky aktivitet nxit krijimtarinë dhe punën praktike digjitale – perfekte për përdorim në klasë apo në hapësira krijuese.</t>
   </si>
   <si>
     <t>Създай свой ключодържател за ученици</t>
   </si>
   <si>
-    <t>Визуално ръководство, стъпка по стъпка, което помага на учениците да създадат свой персонализиран ключодържател чрез Tinkercad. От избора на букви до персонализиране и експортиране за 3D печат, тази дейност насърчава креативността и практическото цифрово създаване – идеална за класна стая или „maker space“.</t>
+    <t>Uploaded 4 September 2025
+Визуално ръководство, стъпка по стъпка, което помага на учениците да създадат свой персонализиран ключодържател чрез Tinkercad. От избора на букви до персонализиране и експортиране за 3D печат, тази дейност насърчава креативността и практическото цифрово създаване – идеална за класна стая или „maker space“.</t>
   </si>
   <si>
     <t>Izradi svoj privjesak za ključeve – za učenike</t>
   </si>
   <si>
-    <t>Vizualni vodič koji pomaže učenicima izraditi vlastiti personalizirani privjesak koristeći Tinkercad. Od odabira slova do prilagodbe i izvoza za 3D ispis, ova aktivnost potiče kreativnost i praktičan digitalni rad – prikladno za učionice ili „maker space“ prostore.</t>
+    <t>Uploaded 4 September 2025
+Vizualni vodič koji pomaže učenicima izraditi vlastiti personalizirani privjesak koristeći Tinkercad. Od odabira slova do prilagodbe i izvoza za 3D ispis, ova aktivnost potiče kreativnost i praktičan digitalni rad – prikladno za učionice ili „maker space“ prostore.</t>
   </si>
   <si>
     <t>Vytvoř si klíčenku – pro studenty</t>
   </si>
   <si>
-    <t>Krok za krokem vizuální průvodce, který studentům pomáhá vytvořit si vlastní personalizovanou klíčenku v Tinkercadu. Od výběru písmen až po přizpůsobení a export pro 3D tisk – aktivita podporuje kreativitu a digitální tvořivost. Ideální do výuky nebo makerspace.</t>
+    <t>Uploaded 4 September 2025
+Krok za krokem vizuální průvodce, který studentům pomáhá vytvořit si vlastní personalizovanou klíčenku v Tinkercadu. Od výběru písmen až po přizpůsobení a export pro 3D tisk – aktivita podporuje kreativitu a digitální tvořivost. Ideální do výuky nebo makerspace.</t>
   </si>
   <si>
     <t>Lav din egen nøglering – for elever</t>
   </si>
   <si>
-    <t>En trin-for-trin visuel guide, der hjælper elever med at skabe deres egen personlige nøglering med Tinkercad. Fra valg af bogstaver til tilpasning og eksport til 3D-print, opmuntrer denne aktivitet til kreativitet og praktisk digitalt arbejde – perfekt til klasseværelser eller makerspaces.</t>
+    <t>Uploaded 4 September 2025
+En trin-for-trin visuel guide, der hjælper elever med at skabe deres egen personlige nøglering med Tinkercad. Fra valg af bogstaver til tilpasning og eksport til 3D-print, opmuntrer denne aktivitet til kreativitet og praktisk digitalt arbejde – perfekt til klasseværelser eller makerspaces.</t>
   </si>
   <si>
     <t>Maak je eigen sleutelhanger – voor leerlingen</t>
   </si>
   <si>
-    <t>Een visuele stapsgewijze handleiding die leerlingen helpt om een gepersonaliseerde sleutelhanger te maken met Tinkercad. Van het kiezen van letters tot aanpassen en exporteren voor 3D-printen, deze activiteit stimuleert creativiteit en digitaal maakplezier – ideaal voor in de klas of makerspace.</t>
+    <t>Uploaded 4 September 2025
+Een visuele stapsgewijze handleiding die leerlingen helpt om een gepersonaliseerde sleutelhanger te maken met Tinkercad. Van het kiezen van letters tot aanpassen en exporteren voor 3D-printen, deze activiteit stimuleert creativiteit en digitaal maakplezier – ideaal voor in de klas of makerspace.</t>
   </si>
   <si>
     <t>Create your keychain for students</t>
   </si>
   <si>
-    <t>A step-by-step visual guide that helps students create their own personalized keychain using Tinkercad. From choosing letters to customizing and exporting for 3D printing, this activity encourages creativity and hands-on digital making—perfect for classroom or maker space use.</t>
-  </si>
-  <si>
-    <t>Crée ton porte-clés personnalisé</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Un guide visuel étape par étape pour aider les élèves à créer leur propre porte-clés personnalisé avec Tinkercad. Du choix des lettres à la personnalisation et à l’exportation pour l’impression 3D, cette activité stimule la créativité et la fabrication numérique – idéale en classe ou en fablab. </t>
+    <t>Uploaded 4 September 2025
+A step-by-step visual guide that helps students create their own personalized keychain using Tinkercad. From choosing letters to customizing and exporting for 3D printing, this activity encourages creativity and hands-on digital making—perfect for classroom or maker space use.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crée ton porte-clés personnalisé </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uploaded 4 September 2025
+Un guide visuel étape par étape pour aider les élèves à créer leur propre porte-clés personnalisé avec Tinkercad. Du choix des lettres à la personnalisation et à l’exportation pour l’impression 3D, cette activité stimule la créativité et la fabrication numérique – idéale en classe ou en fablab. </t>
   </si>
   <si>
     <t>Gestalte deinen eigenen Schlüsselanhänger – für Schüler*innen</t>
   </si>
   <si>
-    <t>Eine schrittweise visuelle Anleitung, die Schüler*innen dabei hilft, ihren eigenen personalisierten Schlüsselanhänger mit Tinkercad zu gestalten. Von der Auswahl der Buchstaben bis hin zur Anpassung und dem Export für den 3D-Druck fördert diese Aktivität Kreativität und praktisches digitales Arbeiten – perfekt für den Einsatz im Klassenzimmer oder im Makerspace.</t>
+    <t>Uploaded 4 September 2025
+Eine schrittweise visuelle Anleitung, die Schüler*innen dabei hilft, ihren eigenen personalisierten Schlüsselanhänger mit Tinkercad zu gestalten. Von der Auswahl der Buchstaben bis hin zur Anpassung und dem Export für den 3D-Druck fördert diese Aktivität Kreativität und praktisches digitales Arbeiten – perfekt für den Einsatz im Klassenzimmer oder im Makerspace.</t>
   </si>
   <si>
     <t>Δημιούργησε το μπρελόκ σου – για μαθητές</t>
   </si>
   <si>
-    <t>Ένας εικονικός οδηγός βήμα προς βήμα που βοηθά τους μαθητές να δημιουργήσουν το δικό τους μπρελόκ μέσω Tinkercad. Από την επιλογή _x000b_γραμμάτων έως την παραμετροποίηση και εξαγωγή για 3D εκτύπωση, η_x000b_δραστηριότητα ενισχύει τη δημιουργικότητα και την πρακτική ψηφιακή _x000b_κατασκευή – ιδανική για τάξεις ή makers paces.</t>
+    <t>Uploaded 4 September 2025
+Ένας εικονικός οδηγός βήμα προς βήμα που βοηθά τους μαθητές να δημιουργήσουν το δικό τους μπρελόκ μέσω Tinkercad. Από την επιλογή _x000b_γραμμάτων έως την παραμετροποίηση και εξαγωγή για 3D εκτύπωση, η_x000b_δραστηριότητα ενισχύει τη δημιουργικότητα και την πρακτική ψηφιακή _x000b_κατασκευή – ιδανική για τάξεις ή makers paces.</t>
   </si>
   <si>
     <t>Crea il tuo portachiavi – per studenti</t>
   </si>
   <si>
-    <t>Una guida visiva passo dopo passo che aiuta gli studenti a creare il proprio portachiavi personalizzato con Tinkercad. Dalla scelta delle lettere alla personalizzazione e all’esportazione per la stampa 3D, questa attività stimola la creatività e il digital making pratico – perfetta per l’uso in classe o nei makerspace.</t>
+    <t>Uploaded 4 September 2025
+Una guida visiva passo dopo passo che aiuta gli studenti a creare il proprio portachiavi personalizzato con Tinkercad. Dalla scelta delle lettere alla personalizzazione e all’esportazione per la stampa 3D, questa attività stimola la creatività e il digital making pratico – perfetta per l’uso in classe o nei makerspace.</t>
   </si>
   <si>
     <t>Izveido savu atslēgu piekariņu – skolēniem</t>
   </si>
   <si>
-    <t>Soli pa solim vizuāla pamācība, kas palīdz skolēniem izveidot savu personalizēto piekariņu ar Tinkercad. No burtu izvēles līdz pielāgošanai un eksportēšanai 3D drukai – šī aktivitāte veicina radošumu un praktisku digitālo darbu. Lieliski piemērota klasei vai radošajai darbnīcai.</t>
+    <t>Uploaded 4 September 2025
+Soli pa solim vizuāla pamācība, kas palīdz skolēniem izveidot savu personalizēto piekariņu ar Tinkercad. No burtu izvēles līdz pielāgošanai un eksportēšanai 3D drukai – šī aktivitāte veicina radošumu un praktisku digitālo darbu. Lieliski piemērota klasei vai radošajai darbnīcai.</t>
   </si>
   <si>
     <t>Sukurk savo raktų pakabuką (mokiniams)</t>
   </si>
   <si>
-    <t>Vaizdus nuoseklus vadovas, padedantis mokiniams susikurti savo asmeninį raktų pakabuką naudojant „Tinkercad“. Ši veikla skatina kūrybiškumą ir savarankišką skaitmeninį darbą - nuo raidžių pasirinkimo iki suasmeninimo ir parengimo trimačiam spausdinimui. Puikiai tinka pamokoms ar praktiniams užsiėmimams.</t>
+    <t>Uploaded 4 September 2025
+Vaizdus nuoseklus vadovas, padedantis mokiniams susikurti savo asmeninį raktų pakabuką naudojant „Tinkercad“. Ši veikla skatina kūrybiškumą ir savarankišką skaitmeninį darbą - nuo raidžių pasirinkimo iki suasmeninimo ir parengimo trimačiam spausdinimui. Puikiai tinka pamokoms ar praktiniams užsiėmimams.</t>
   </si>
   <si>
     <t>Oħloq il-keychain tiegħek – għal studenti</t>
   </si>
   <si>
-    <t>Gwida viżiva pass pass li tgħin lill-istudenti joħolqu keychain personalizzat tagħhom stess permezz ta’ Tinkercad. Mill-għażla tal-ittri sal-personalizzazzjoni u esportazzjoni għall-istampar 3D, din l-attività tħeġġeġ il-kreattività u l-ħiliet diġitali prattiċi – perfetta għall-klassijiet jew makerspaces.</t>
+    <t>Uploaded 4 September 2025
+Gwida viżiva pass pass li tgħin lill-istudenti joħolqu keychain personalizzat tagħhom stess permezz ta’ Tinkercad. Mill-għażla tal-ittri sal-personalizzazzjoni u esportazzjoni għall-istampar 3D, din l-attività tħeġġeġ il-kreattività u l-ħiliet diġitali prattiċi – perfetta għall-klassijiet jew makerspaces.</t>
   </si>
   <si>
     <t>Stwórz swój brelok – dla uczniów</t>
   </si>
   <si>
-    <t>Ilustrowana instrukcja krok po kroku, która pomaga uczniom stworzyć spersonalizowany brelok w programie Tinkercad. Od wyboru liter, przez personalizację, aż po eksport do druku 3D – ta aktywność rozwija kreatywność i praktyczne umiejętności cyfrowe. Idealna do klasy lub pracowni technicznej.</t>
+    <t>Uploaded 4 September 2025
+Ilustrowana instrukcja krok po kroku, która pomaga uczniom stworzyć spersonalizowany brelok w programie Tinkercad. Od wyboru liter, przez personalizację, aż po eksport do druku 3D – ta aktywność rozwija kreatywność i praktyczne umiejętności cyfrowe. Idealna do klasy lub pracowni technicznej.</t>
   </si>
   <si>
     <t>Cria o teu porta-chaves – para alunos</t>
   </si>
   <si>
-    <t>Um guia visual passo a passo que ajuda os alunos a criarem o seu próprio porta-chaves personalizado com o Tinkercad. Desde a escolha das letras até à personalização e exportação para impressão 3D, esta atividade promove a criatividade e o trabalho digital prático – perfeita para a sala de aula ou espaços criativos.</t>
+    <t>Uploaded 4 September 2025
+Um guia visual passo a passo que ajuda os alunos a criarem o seu próprio porta-chaves personalizado com o Tinkercad. Desde a escolha das letras até à personalização e exportação para impressão 3D, esta atividade promove a criatividade e o trabalho digital prático – perfeita para a sala de aula ou espaços criativos.</t>
   </si>
   <si>
     <t>Vytvor si vlastný prívesok – pre žiakov</t>
   </si>
   <si>
-    <t>Vizuálny sprievodca krok za krokom, ktorý žiakom pomáha vytvoriť si svoj vlastný personalizovaný prívesok v Tinkercade. Od výberu písmen po prispôsobenie a export na 3D tlač – aktivita podporuje kreativitu a praktické digitálne zručnosti. Ideálne pre triedy alebo tvorivé dielne.</t>
+    <t>Uploaded 4 September 2025
+Vizuálny sprievodca krok za krokom, ktorý žiakom pomáha vytvoriť si svoj vlastný personalizovaný prívesok v Tinkercade. Od výberu písmen po prispôsobenie a export na 3D tlač – aktivita podporuje kreativitu a praktické digitálne zručnosti. Ideálne pre triedy alebo tvorivé dielne.</t>
   </si>
   <si>
     <t>Ustvari svoj obesek za ključe – za učence</t>
   </si>
   <si>
-    <t>Vizualni vodnik, ki učencem pomaga ustvariti lasten personaliziran obesek z uporabo Tinkercada. Od izbire črk do prilagajanja in izvoza za 3D tiskanje ta aktivnost spodbuja ustvarjalnost in praktično digitalno delo – primerno za učilnice ali „maker space“ prostore.</t>
+    <t>Uploaded 4 September 2025
+Vizualni vodnik, ki učencem pomaga ustvariti lasten personaliziran obesek z uporabo Tinkercada. Od izbire črk do prilagajanja in izvoza za 3D tiskanje ta aktivnost spodbuja ustvarjalnost in praktično digitalno delo – primerno za učilnice ali „maker space“ prostore.</t>
   </si>
   <si>
     <t>Crea tu llavero - para estudiantes</t>
   </si>
   <si>
-    <t>Una guía visual paso a paso que ayuda a los estudiantes a crear su propio llavero personalizado usando Tinkercad. Desde elegir letras hasta personalizar y exportar para impresión 3D, esta actividad fomenta la creatividad y la creación digital práctica – ideal para el aula o espacios maker.</t>
+    <t>Uploaded 4 September 2025
+Una guía visual paso a paso que ayuda a los estudiantes a crear su propio llavero personalizado usando Tinkercad. Desde elegir letras hasta personalizar y exportar para impresión 3D, esta actividad fomenta la creatividad y la creación digital práctica – ideal para el aula o espacios maker.</t>
   </si>
   <si>
     <t>Luo oma avaimenperäsi – oppilaille</t>
   </si>
   <si>
-    <t>Visuaalinen vaihe vaiheelta -opas, joka auttaa oppilaita luomaan oman yksilöllisen avaimenperän Tinkercadin avulla. Kirjainten valinnasta muokkaamiseen ja vientiin 3D-tulostusta varten – tehtävä kehittää luovuutta ja käytännön digitaalisia taitoja. Sopii täydellisesti luokkahuoneisiin ja makerspace-tiloihin.</t>
+    <t>Uploaded 4 September 2025
+Visuaalinen vaihe vaiheelta -opas, joka auttaa oppilaita luomaan oman yksilöllisen avaimenperän Tinkercadin avulla. Kirjainten valinnasta muokkaamiseen ja vientiin 3D-tulostusta varten – tehtävä kehittää luovuutta ja käytännön digitaalisia taitoja. Sopii täydellisesti luokkahuoneisiin ja makerspace-tiloihin.</t>
   </si>
   <si>
     <t>Skapa din nyckelring – för elever</t>
   </si>
   <si>
-    <t>En visuell steg-för-steg-guide som hjälper elever att skapa sin egen personliga nyckelring med Tinkercad. Från att välja bokstäver till att anpassa och exportera för 3D-utskrift – aktiviteten uppmuntrar kreativitet och praktiskt digitalt skapande. Perfekt för klassrum eller makerspaces.</t>
+    <t>Uploaded 4 September 2025
+En visuell steg-för-steg-guide som hjälper elever att skapa sin egen personliga nyckelring med Tinkercad. Från att välja bokstäver till att anpassa och exportera för 3D-utskrift – aktiviteten uppmuntrar kreativitet och praktiskt digitalt skapande. Perfekt för klassrum eller makerspaces.</t>
   </si>
   <si>
     <t>Öğrenciler için anahtarlığınızı oluşturun</t>
   </si>
   <si>
-    <t>Öğrencilerin Tinkercad kullanarak kendi kişiselleştirilmiş anahtarlığını oluşturmalarına yardımcı olan adım adım görsel bir kılavuz. Harfleri seçmekten özelleştirmeye ve 3D baskı için dışa aktarmaya kadar bu etkinlik, yaratıcılığı ve uygulamalı dijital üretimi teşvik eder; sınıf veya üretim alanı kullanımı için mükemmeldir.</t>
-  </si>
-  <si>
-    <t>Створи свій брелок – для здобувачів освіти</t>
-  </si>
-  <si>
-    <t>Покроковий візуальний посібник, що допомагає здобувачам освіти створити персоналізований брелок у Tinkercad. Від вибору літер до налаштувань і підготовки до 3D-друку — ця активність стимулює креативність і розвиток практичних цифрових навичок. Ідеально підходить для навчальних класів та makerspace-просторів.</t>
+    <t>Uploaded 4 September 2025
+Öğrencilerin Tinkercad kullanarak kendi kişiselleştirilmiş anahtarlığını oluşturmalarına yardımcı olan adım adım görsel bir kılavuz. Harfleri seçmekten özelleştirmeye ve 3D baskı için dışa aktarmaya kadar bu etkinlik, yaratıcılığı ve uygulamalı dijital üretimi teşvik eder; sınıf veya üretim alanı kullanımı için mükemmeldir.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Створи свій брелок – для здобувачів освіти </t>
+  </si>
+  <si>
+    <t>Uploaded 4 September 2025
+Покроковий візуальний посібник, що допомагає здобувачам освіти створити персоналізований брелок у Tinkercad. Від вибору літер до налаштувань і підготовки до 3D-друку — ця активність стимулює креативність і розвиток практичних цифрових навичок. Ідеально підходить для навчальних класів та makerspace-просторів.</t>
   </si>
   <si>
     <t>Gratë në STEAM: Gratë që ndryshuan botën e teknologjisë</t>
   </si>
   <si>
-    <t>Një hyrje frymëzuese për gratë me ndikim në STEAM dhe pse larmia ka rëndësi në teknologji dhe shkencë. Nxënësit zbulojnë modele kyçe dhe eksplorojnë pse duhen më shumë vajza në fushat STEAM. Një burim i shkëlqyer për të nxitur kureshtjen dhe fuqizuar novatorët e rinj.</t>
+    <t>Uploaded 4 September 2025
+Një hyrje frymëzuese për gratë me ndikim në STEAM dhe pse larmia ka rëndësi në teknologji dhe shkencë. Nxënësit zbulojnë modele kyçe dhe eksplorojnë pse duhen më shumë vajza në fushat STEAM. Një burim i shkëlqyer për të nxitur kureshtjen dhe fuqizuar novatorët e rinj.</t>
   </si>
   <si>
     <t>Жените в STEAM: Жените, които промениха света на технологиите</t>
   </si>
   <si>
-    <t>Вдъхновяващо въведение за влиятелни жени в STEAM и защо разнообразието е важно в технологиите и науката. Учениците откриват ключови ролеви модели и изследват защо са нужни повече момичета в областите на STEAM. Перфектен ресурс за събуждане на любопитството и овластяване на младите новатори.</t>
+    <t>Uploaded 4 September 2025
+Вдъхновяващо въведение за влиятелни жени в STEAM и защо разнообразието е важно в технологиите и науката. Учениците откриват ключови ролеви модели и изследват защо са нужни повече момичета в областите на STEAM. Перфектен ресурс за събуждане на любопитството и овластяване на младите новатори.</t>
   </si>
   <si>
     <t>Žene u STEAM-u: Žene koje su promijenile svijet tehnologije</t>
   </si>
   <si>
-    <t xml:space="preserve">Inspirativan uvod u razloge zašto je raznolikost važna u tehnologiji i znanosti. Učenici otkrivaju ključne ženske figure u STEAM-u i istražuju zašto je potrebno više djevojaka u STEAM područjima. </t>
+    <t xml:space="preserve">Uploaded 4 September 2025
+Inspirativan uvod u razloge zašto je raznolikost važna u tehnologiji i znanosti. Učenici otkrivaju ključne ženske figure u STEAM-u i istražuju zašto je potrebno više djevojaka u STEAM područjima. </t>
   </si>
   <si>
     <t>Ženy v STEAM: Ženy, které změnily svět technologií</t>
   </si>
   <si>
-    <t>Inspirativní úvod ke vlivným ženám v oblasti STEAM a k důležitosti diverzity v technologiích a vědě. Studenti objevují klíčové vzory a zkoumají, proč je potřeba více dívek v oborech STEAM. Skvělý zdroj pro probuzení zvědavosti a podporu mladých inovátorek.</t>
+    <t>Uploaded 4 September 2025
+Inspirativní úvod ke vlivným ženám v oblasti STEAM a k důležitosti diverzity v technologiích a vědě. Studenti objevují klíčové vzory a zkoumají, proč je potřeba více dívek v oborech STEAM. Skvělý zdroj pro probuzení zvědavosti a podporu mladých inovátorek.</t>
   </si>
   <si>
     <t>Kvinder i STEAM: Kvinder der ændrede tech-verdenen</t>
   </si>
   <si>
-    <t>En inspirerende introduktion til indflydelsesrige kvinder i STEAM og hvorfor diversitet betyder noget i teknologi og videnskab. Eleverne opdager vigtige rollemodeller og undersøger, hvorfor flere piger er nødvendige i STEAM-felterne. En perfekt ressource til at vække nysgerrighed og styrke unge innovatorer.</t>
+    <t>Uploaded 4 September 2025
+En inspirerende introduktion til indflydelsesrige kvinder i STEAM og hvorfor diversitet betyder noget i teknologi og videnskab. Eleverne opdager vigtige rollemodeller og undersøger, hvorfor flere piger er nødvendige i STEAM-felterne. En perfekt ressource til at vække nysgerrighed og styrke unge innovatorer.</t>
   </si>
   <si>
     <t>Vrouwen in STEAM: Vrouwen die de tech-wereld veranderden</t>
   </si>
   <si>
-    <t>Een inspirerende introductie tot invloedrijke vrouwen in STEAM en waarom diversiteit belangrijk is in technologie en wetenschap. Leerlingen ontdekken belangrijke rolmodellen en verkennen waarom er meer meisjes nodig zijn in STEAM-gebieden. Een perfecte bron om nieuwsgierigheid te wekken en jonge vernieuwers te versterken.</t>
+    <t>Uploaded 4 September 2025
+Een inspirerende introductie tot invloedrijke vrouwen in STEAM en waarom diversiteit belangrijk is in technologie en wetenschap. Leerlingen ontdekken belangrijke rolmodellen en verkennen waarom er meer meisjes nodig zijn in STEAM-gebieden. Een perfecte bron om nieuwsgierigheid te wekken en jonge vernieuwers te versterken.</t>
   </si>
   <si>
     <t>Women in STEAM: Women Who Changed the Tech</t>
   </si>
   <si>
-    <t>An inspiring introduction to influential women in STEAM and why diversity matters in tech and science. Learners discover key role models, and explore why more girls are needed in STEAM fields. A perfect resource to spark curiosity and empower young innovators.</t>
+    <t>Uploaded 4 September 2025
+An inspiring introduction to influential women in STEAM and why diversity matters in tech and science. Learners discover key role models, and explore why more girls are needed in STEAM fields. A perfect resource to spark curiosity and empower young innovators.</t>
   </si>
   <si>
     <t>Femmes dans les STEAM : Femmes qui ont changé le monde de la technologie</t>
   </si>
   <si>
-    <t>Une introduction inspirante aux femmes influentes dans les STEAM et à l'importance de la diversité dans les technologies et les sciences. Les élèves découvrent des modèles clés et explorent pourquoi davantage de filles sont nécessaires dans les domaines STEAM. Une ressource parfaite pour éveiller la curiosité et encourager les jeunes innovatrices.</t>
+    <t>Uploaded 4 September 2025
+Une introduction inspirante aux femmes influentes dans les STEAM et à l'importance de la diversité dans les technologies et les sciences. Les élèves découvrent des modèles clés et explorent pourquoi davantage de filles sont nécessaires dans les domaines STEAM. Une ressource parfaite pour éveiller la curiosité et encourager les jeunes innovatrices.</t>
   </si>
   <si>
     <t>Frauen, die die Tech-Welt verändert haben</t>
   </si>
   <si>
-    <t>Eine inspirierende Einführung zu Pionierinnen der Wissenschaft und Technik und warum Vielfalt in der Tech-Welt wichtig ist. Die Lernenden entdecken Vorbilder und erfahren, warum mehr Mädchen im MINT-Bereich gebraucht werden. Eine ideale Ressource, um Neugier zu wecken und junge Innovatorinnen zu stärken.</t>
+    <t>Uploaded 4 September 2025
+Eine inspirierende Einführung zu Pionierinnen der Wissenschaft und Technik und warum Vielfalt in der Tech-Welt wichtig ist. Die Lernenden entdecken Vorbilder und erfahren, warum mehr Mädchen im MINT-Bereich gebraucht werden. Eine ideale Ressource, um Neugier zu wecken und junge Innovatorinnen zu stärken.</t>
   </si>
   <si>
     <t>Γυναίκες στο STEAM: Γυναίκες που άλλαξαν τον κόσμο της τεχνολογίας</t>
   </si>
   <si>
-    <t>Μια εμπνευσμένη εισαγωγή για τις γυναίκες με επιρροή στον χώρο του STEAM και γιατί η ποικιλομορφία είναι ζωτικής σημασίας στην  τεχνολογία και την επιστήμη. Οι μαθητές/τριες θα ανακαλύπψουν πρότυπα και θα εξερευνήσουν γιατί απαραίτητο να συμμετάσχουν περισσότερα κορίτσια στους  τομείς STEAM.
+    <t>Uploaded 4 September 2025
+Μια εμπνευσμένη εισαγωγή για τις γυναίκες με επιρροή στον χώρο του STEAM και γιατί η ποικιλομορφία είναι ζωτικής σημασίας στην  τεχνολογία και την επιστήμη. Οι μαθητές/τριες θα ανακαλύπψουν πρότυπα και θα εξερευνήσουν γιατί απαραίτητο να συμμετάσχουν περισσότερα κορίτσια στους  τομείς STEAM.
  Ένα ιδανικό υλικό για να ενισχυθεί η περιέργεια και να ενδυναμωθούν οι αυριανοί καινοτόμοι.</t>
   </si>
   <si>
     <t>Donne nelle STEAM: Donne che hanno cambiato il mondo della tecnologia</t>
   </si>
   <si>
-    <t>Un’introduzione ispiratrice alle donne influenti nelle STEAM e all'importanza della diversità nella tecnologia e nella scienza. Gli studenti scoprono modelli di riferimento chiave e approfondiscono perché servono più ragazze nei campi STEAM. Una risorsa perfetta per stimolare la curiosità e rafforzare le giovani innovatrici.</t>
+    <t>Uploaded 4 September 2025
+Un’introduzione ispiratrice alle donne influenti nelle STEAM e all'importanza della diversità nella tecnologia e nella scienza. Gli studenti scoprono modelli di riferimento chiave e approfondiscono perché servono più ragazze nei campi STEAM. Una risorsa perfetta per stimolare la curiosità e rafforzare le giovani innovatrici.</t>
   </si>
   <si>
     <t>Sievietes STEAM jomā: Sievietes, kuras mainīja tehnoloģiju pasauli</t>
   </si>
   <si>
-    <t>Iedvesmojošs ievads par ietekmīgām sievietēm STEAM jomā un par to, kāpēc daudzveidība ir svarīga tehnoloģijā un zinātnē. Skolēni iepazīst svarīgus paraugus un pēta, kāpēc STEAM jomās ir vajadzīgas vairāk meitenes. Lielisks resurss, lai rosinātu zinātkāri un iedrošinātu jaunos inovatorus.</t>
+    <t>Uploaded 4 September 2025
+Iedvesmojošs ievads par ietekmīgām sievietēm STEAM jomā un par to, kāpēc daudzveidība ir svarīga tehnoloģijā un zinātnē. Skolēni iepazīst svarīgus paraugus un pēta, kāpēc STEAM jomās ir vajadzīgas vairāk meitenes. Lielisks resurss, lai rosinātu zinātkāri un iedrošinātu jaunos inovatorus.</t>
   </si>
   <si>
     <t>Moterys STEAM srityje: moterys, kurios pakeitė technologijų pasaulį</t>
   </si>
   <si>
-    <t>įkvepiantis pasakojimas apie įtakingas moteris STEAM srityje ir kodėl įvairovė yra svarbi technologijose ir moksle. Mokiniai atranda svarbius pavyzdžius ir nagrinėja, kodėl STEAM srityse reikia daugiau merginų. Puikus išteklius žingeidumui skatinti ir jaunoms novatorėms įgalinti.</t>
+    <t>Uploaded 4 September 2025
+įkvepiantis pasakojimas apie įtakingas moteris STEAM srityje ir kodėl įvairovė yra svarbi technologijose ir moksle. Mokiniai atranda svarbius pavyzdžius ir nagrinėja, kodėl STEAM srityse reikia daugiau merginų. Puikus išteklius žingeidumui skatinti ir jaunoms novatorėms įgalinti.</t>
   </si>
   <si>
     <t>Nisa fil-STEAM: Nisa li biddlu d-dinja tat-teknoloġija</t>
   </si>
   <si>
-    <t>Introduzzjoni ispirata għal nisa influwenti fil-STEAM u għaliex id-diversità hija importanti fit-teknoloġija u x-xjenza. L-istudenti jiskopru mudelli ta’ ispirazzjoni u jesploraw għaliex għandna bżonn aktar bniet fil-qasam tal-STEAM. Riżorsa perfetta biex tqajjem il-kurżità u ssaħħaħ lill-inventuri żgħażagħ.</t>
+    <t>Uploaded 4 September 2025
+Introduzzjoni ispirata għal nisa influwenti fil-STEAM u għaliex id-diversità hija importanti fit-teknoloġija u x-xjenza. L-istudenti jiskopru mudelli ta’ ispirazzjoni u jesploraw għaliex għandna bżonn aktar bniet fil-qasam tal-STEAM. Riżorsa perfetta biex tqajjem il-kurżità u ssaħħaħ lill-inventuri żgħażagħ.</t>
   </si>
   <si>
     <t>Kobiety w STEAM: Kobiety, które zmieniły świat technologii</t>
   </si>
   <si>
-    <t>Inspirujące wprowadzenie do wpływowych kobiet w STEAM oraz znaczenia różnorodności w technologii i nauce. Uczniowie poznają kluczowe wzorce do naśladowania i dowiadują się, dlaczego w dziedzinach STEAM potrzeba więcej dziewcząt. Doskonałe źródło do rozbudzania ciekawości i wzmacniania młodych innowatorek.</t>
+    <t>Uploaded 4 September 2025
+Inspirujące wprowadzenie do wpływowych kobiet w STEAM oraz znaczenia różnorodności w technologii i nauce. Uczniowie poznają kluczowe wzorce do naśladowania i dowiadują się, dlaczego w dziedzinach STEAM potrzeba więcej dziewcząt. Doskonałe źródło do rozbudzania ciekawości i wzmacniania młodych innowatorek.</t>
   </si>
   <si>
     <t>Mulheres no STEAM: Mulheres que mudaram o mundo da tecnologia</t>
   </si>
   <si>
-    <t>Uma introdução inspiradora a mulheres influentes no STEAM e à importância da diversidade na tecnologia e na ciência. Os alunos descobrem modelos de referência e exploram por que precisamos de mais meninas nas áreas de STEAM. Um recurso perfeito para despertar a curiosidade e capacitar jovens inovadoras.</t>
+    <t>Uploaded 4 September 2025
+Uma introdução inspiradora a mulheres influentes no STEAM e à importância da diversidade na tecnologia e na ciência. Os alunos descobrem modelos de referência e exploram por que precisamos de mais meninas nas áreas de STEAM. Um recurso perfeito para despertar a curiosidade e capacitar jovens inovadoras.</t>
   </si>
   <si>
     <t>Femei în STEAM: Femei care au schimbat lumea tehnologiei</t>
   </si>
   <si>
-    <t>O introducere inspirațională despre femei influente din domeniul STEAM și despre importanța diversității în tehnologie și știință. Elevii descoperă modele de urmat și explorează de ce este nevoie de mai multe fete în domeniile STEAM. O resursă perfectă pentru a stimula curiozitatea și a încuraja tinerele inovatoare.</t>
+    <t>Uploaded 4 September 2025
+O introducere inspirațională despre femei influente din domeniul STEAM și despre importanța diversității în tehnologie și știință. Elevii descoperă modele de urmat și explorează de ce este nevoie de mai multe fete în domeniile STEAM. O resursă perfectă pentru a stimula curiozitatea și a încuraja tinerele inovatoare.</t>
   </si>
   <si>
     <t>Ženy v STEAM: Ženy, ktoré zmenili svet technológií</t>
   </si>
   <si>
-    <t>Inšpiratívny úvod k významným ženám v oblasti STEAM a vysvetlenie, prečo je rozmanitosť v technológiách a vede dôležitá. Žiaci spoznajú kľúčové vzory a zistia, prečo potrebujeme viac dievčat v STEAM oblastiach. Skvelý zdroj na podporu zvedavosti a posilnenie mladých inovátoriek.</t>
+    <t>Uploaded 4 September 2025
+Inšpiratívny úvod k významným ženám v oblasti STEAM a vysvetlenie, prečo je rozmanitosť v technológiách a vede dôležitá. Žiaci spoznajú kľúčové vzory a zistia, prečo potrebujeme viac dievčat v STEAM oblastiach. Skvelý zdroj na podporu zvedavosti a posilnenie mladých inovátoriek.</t>
   </si>
   <si>
     <t>Ženske v STEAM-u: Ženske, ki so spremenile tehnološki svet</t>
   </si>
   <si>
-    <t>Navdihujoč uvod v vplivne ženske na področju STEAM ter zakaj je raznolikost pomembna v tehnologiji in znanosti. Učenci spoznajo ključne vzornice in raziskujejo, zakaj je na področjih STEAM potrebnih več deklet. Odličen vir za spodbujanje radovednosti in opolnomočenje mladih inovatoric.</t>
+    <t>Uploaded 4 September 2025
+Navdihujoč uvod v vplivne ženske na področju STEAM ter zakaj je raznolikost pomembna v tehnologiji in znanosti. Učenci spoznajo ključne vzornice in raziskujejo, zakaj je na področjih STEAM potrebnih več deklet. Odličen vir za spodbujanje radovednosti in opolnomočenje mladih inovatoric.</t>
   </si>
   <si>
     <t>Mujeres en STEAM: Mujeres que cambiaron el mundo de la tecnología</t>
   </si>
   <si>
-    <t>Una introducción inspiradora a mujeres influyentes en STEAM y la importancia de la diversidad en la tecnología y la ciencia. Los estudiantes descubren modelos clave y exploran por qué se necesitan más niñas en los campos STEAM. Un recurso perfecto para despertar la curiosidad y empoderar a las jóvenes innovadoras.</t>
+    <t>Uploaded 4 September 2025
+Una introducción inspiradora a mujeres influyentes en STEAM y la importancia de la diversidad en la tecnología y la ciencia. Los estudiantes descubren modelos clave y exploran por qué se necesitan más niñas en los campos STEAM. Un recurso perfecto para despertar la curiosidad y empoderar a las jóvenes innovadoras.</t>
   </si>
   <si>
     <t>Naiset STEAM-aloilla: Naiset, jotka muuttivat teknologia-alan</t>
   </si>
   <si>
-    <t>Inspiroiva johdatus vaikutusvaltaisiin naisiin STEAM-aloilla ja siihen, miksi monimuotoisuus on tärkeää teknologiassa ja tieteessä. Oppilaat tutustuvat tärkeisiin roolimalleihin ja tutkivat, miksi STEAM-aloille tarvitaan lisää tyttöjä. Täydellinen resurssi uteliaisuuden herättämiseen ja nuorten innovaattoreiden rohkaisemiseen.</t>
+    <t>Uploaded 4 September 2025
+Inspiroiva johdatus vaikutusvaltaisiin naisiin STEAM-aloilla ja siihen, miksi monimuotoisuus on tärkeää teknologiassa ja tieteessä. Oppilaat tutustuvat tärkeisiin roolimalleihin ja tutkivat, miksi STEAM-aloille tarvitaan lisää tyttöjä. Täydellinen resurssi uteliaisuuden herättämiseen ja nuorten innovaattoreiden rohkaisemiseen.</t>
   </si>
   <si>
     <t>Kvinnor i STEAM: Kvinnor som förändrade teknikvärlden</t>
   </si>
   <si>
-    <t>En inspirerande introduktion till inflytelserika kvinnor inom STEAM och varför mångfald är viktigt inom teknik och vetenskap. Eleverna upptäcker viktiga förebilder och utforskar varför fler flickor behövs inom STEAM-områdena. En perfekt resurs för att väcka nyfikenhet och stärka unga innovatörer.</t>
-  </si>
-  <si>
-    <t>STEAM'deki Kadınlar: Teknoloji Dünyasını Değiştiren</t>
-  </si>
-  <si>
-    <t>STEAM'deki etkili kadınlara ve teknoloji ve bilimde çeşitliliğin neden önemli olduğuna dair ilham verici bir giriş. Öğrenciler önemli rol modelleri keşfediyor ve STEAM alanlarında neden daha fazla kız çocuğuna ihtiyaç duyulduğunu inceliyor. Merak uyandırmak ve genç yenilikçileri güçlendirmek için mükemmel bir kaynak.</t>
+    <t>Uploaded 4 September 2025
+En inspirerande introduktion till inflytelserika kvinnor inom STEAM och varför mångfald är viktigt inom teknik och vetenskap. Eleverna upptäcker viktiga förebilder och utforskar varför fler flickor behövs inom STEAM-områdena. En perfekt resurs för att väcka nyfikenhet och stärka unga innovatörer.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> STEAM'deki Kadınlar: Teknoloji Dünyasını Değiştiren</t>
+  </si>
+  <si>
+    <t>Uploaded 4 September 2025
+STEAM'deki etkili kadınlara ve teknoloji ve bilimde çeşitliliğin neden önemli olduğuna dair ilham verici bir giriş. Öğrenciler önemli rol modelleri keşfediyor ve STEAM alanlarında neden daha fazla kız çocuğuna ihtiyaç duyulduğunu inceliyor. Merak uyandırmak ve genç yenilikçileri güçlendirmek için mükemmel bir kaynak.</t>
   </si>
   <si>
     <t>Жінки у STEAM: Жінки, які змінили світ технологій</t>
   </si>
   <si>
-    <t>Надихаючий вступ до впливових жінок у STEAM і важливість різноманіття в технологіях та науці. Здобувачі освіти знайомляться з ключовими рольовими моделями та досліджують, чому у STEAM необхідно більше дівчат. Ідеальний ресурс для пробудження цікавості та розширення можливостей молодих новаторок.</t>
+    <t>Uploaded 4 September 2025
+Надихаючий вступ до впливових жінок у STEAM і важливість різноманіття в технологіях та науці. Здобувачі освіти знайомляться з ключовими рольовими моделями та досліджують, чому у STEAM необхідно більше дівчат. Ідеальний ресурс для пробудження цікавості та розширення можливостей молодих новаторок.</t>
   </si>
   <si>
     <t>Zbulo tipin tënd digjital</t>
   </si>
   <si>
-    <t>Kjo aktivitet fton nxënësit të eksplorojnë pikat e tyre të forta dhe interesat përmes kuizeve online tërheqëse që i lidhin me karriera digjitale. Nxënësit reflektojnë mbi rezultatet, diskutojnë në grupe dhe ndajnë përvojat e tyre në një mur bashkëpunues. Një mënyrë e shkëlqyer për të nxitur kuriozitetin dhe për të personalizuar eksplorimin e karrierës – ideale si në klasë ashtu edhe në mësimin online.</t>
+    <t>Uploaded 4 September 2025
+Kjo aktivitet fton nxënësit të eksplorojnë pikat e tyre të forta dhe interesat përmes kuizeve online tërheqëse që i lidhin me karriera digjitale. Nxënësit reflektojnë mbi rezultatet, diskutojnë në grupe dhe ndajnë përvojat e tyre në një mur bashkëpunues. Një mënyrë e shkëlqyer për të nxitur kuriozitetin dhe për të personalizuar eksplorimin e karrierës – ideale si në klasë ashtu edhe në mësimin online.</t>
   </si>
   <si>
     <t>Открий своя дигитален тип</t>
   </si>
   <si>
-    <t>Тази дейност приканва учениците да изследват своите силни страни и интереси чрез забавни онлайн тестове, които ги свързват с дигитални кариери. Учениците разсъждават върху резултатите си, обсъждат в групи и споделят впечатленията си на обща стена. Отличен начин за събуждане на любопитство и персонализирано кариерно ориентиране – подходящо както за присъствено, така и за дистанционно обучение.</t>
+    <t>Uploaded 4 September 2025
+Тази дейност приканва учениците да изследват своите силни страни и интереси чрез забавни онлайн тестове, които ги свързват с дигитални кариери. Учениците разсъждават върху резултатите си, обсъждат в групи и споделят впечатленията си на обща стена. Отличен начин за събуждане на любопитство и персонализирано кариерно ориентиране – подходящо както за присъствено, така и за дистанционно обучение.</t>
   </si>
   <si>
     <t>Otkrij svoju digitalnu karijeru</t>
   </si>
   <si>
-    <t>Aktivnost poziva učenike da istraže svoje jake strane i interese putem zanimljivih online kvizova koji ih povezuju s digitalnim karijerama. Učenici razmišljaju o rezultatima, raspravljaju u grupama i dijele svoja zapažanja. Aktivnost je odličan način za poticanje znatiželje i individualnog istraživanje karijera – prikladna je za nastavu uživo i na daljinu.</t>
+    <t>Uploaded 4 September 2025
+Aktivnost poziva učenike da istraže svoje jake strane i interese putem zanimljivih online kvizova koji ih povezuju s digitalnim karijerama. Učenici razmišljaju o rezultatima, raspravljaju u grupama i dijele svoja zapažanja. Aktivnost je odličan način za poticanje znatiželje i individualnog istraživanje karijera – prikladna je za nastavu uživo i na daljinu.</t>
   </si>
   <si>
     <t>Objevte svůj digitální typ</t>
   </si>
   <si>
-    <t>Tato aktivita vybízí studenty, aby prozkoumali své silné stránky a zájmy pomocí poutavých online kvízů, které je spojí s digitálními kariérami. Studenti reflektují výsledky, diskutují ve skupinách a sdílejí své poznatky na společné nástěnce. Skvělý způsob, jak vzbudit zvědavost a přizpůsobit objevování kariéry – ideální pro výuku ve třídě i na dálku.</t>
+    <t>Uploaded 4 September 2025
+Tato aktivita vybízí studenty, aby prozkoumali své silné stránky a zájmy pomocí poutavých online kvízů, které je spojí s digitálními kariérami. Studenti reflektují výsledky, diskutují ve skupinách a sdílejí své poznatky na společné nástěnce. Skvělý způsob, jak vzbudit zvědavost a přizpůsobit objevování kariéry – ideální pro výuku ve třídě i na dálku.</t>
   </si>
   <si>
     <t>Opdag din digitale type</t>
   </si>
   <si>
-    <t>Denne aktivitet inviterer eleverne til at udforske deres styrker og interesser gennem engagerende online quizzer, der matcher dem med digitale karrierer. Eleverne reflekterer over resultaterne, diskuterer i grupper og deler deres indsigter på en fælles væg. En fantastisk måde at vække nysgerrighed og tilpasse karriereudforskning – perfekt til både klasselokalet og fjernundervisning.</t>
+    <t>Uploaded 4 September 2025
+Denne aktivitet inviterer eleverne til at udforske deres styrker og interesser gennem engagerende online quizzer, der matcher dem med digitale karrierer. Eleverne reflekterer over resultaterne, diskuterer i grupper og deler deres indsigter på en fælles væg. En fantastisk måde at vække nysgerrighed og tilpasse karriereudforskning – perfekt til både klasselokalet og fjernundervisning.</t>
   </si>
   <si>
     <t>Ontdek jouw digitale type</t>
   </si>
   <si>
-    <t>Deze activiteit nodigt leerlingen uit om hun sterke punten en interesses te ontdekken via leuke online quizzen die hen koppelen aan digitale carrières. Leerlingen reflecteren op hun resultaten, bespreken deze in groepen en delen hun inzichten op een gezamenlijke muur. Een geweldige manier om nieuwsgierigheid op te wekken en loopbaanoriëntatie te personaliseren – ideaal voor klassikaal en afstandsonderwijs.</t>
+    <t>Uploaded 4 September 2025
+Deze activiteit nodigt leerlingen uit om hun sterke punten en interesses te ontdekken via leuke online quizzen die hen koppelen aan digitale carrières. Leerlingen reflecteren op hun resultaten, bespreken deze in groepen en delen hun inzichten op een gezamenlijke muur. Een geweldige manier om nieuwsgierigheid op te wekken en loopbaanoriëntatie te personaliseren – ideaal voor klassikaal en afstandsonderwijs.</t>
   </si>
   <si>
     <t>Discover Your Digital Type</t>
   </si>
   <si>
-    <t>This activity invites students to explore their strengths and interests through engaging online quizzes that match them with digital careers. Learners reflect on their results, discuss in groups, and share their insights on a collaborative wall. A great way to spark curiosity and personalize career exploration—ideal for both in-class and remote settings.</t>
+    <t>Uploaded 4 September 2025
+This activity invites students to explore their strengths and interests through engaging online quizzes that match them with digital careers. Learners reflect on their results, discuss in groups, and share their insights on a collaborative wall. A great way to spark curiosity and personalize career exploration—ideal for both in-class and remote settings.</t>
   </si>
   <si>
     <t>Découvre ton profil numérique</t>
   </si>
   <si>
-    <t>Cette activité invite les élèves à explorer leurs forces et centres d’intérêt à travers des quiz en ligne qui leur proposent des carrières dans le numérique. Les apprenants réfléchissent à leurs résultats, discutent en groupe et partagent leurs idées sur un tableau interactif. Un excellent moyen de susciter la curiosité et de rendre l'orientation professionnelle plus personnelle – idéal en classe comme à distance.</t>
+    <t>Uploaded 4 September 2025
+Cette activité invite les élèves à explorer leurs forces et centres d’intérêt à travers des quiz en ligne qui leur proposent des carrières dans le numérique. Les apprenants réfléchissent à leurs résultats, discutent en groupe et partagent leurs idées sur un tableau interactif. Un excellent moyen de susciter la curiosité et de rendre l'orientation professionnelle plus personnelle – idéal en classe comme à distance.</t>
   </si>
   <si>
     <t>Welcher Digitaltyp bist du?</t>
   </si>
   <si>
-    <t>Diese Aktivität lädt Schüler*innen ein, mit spannenden Online-Quizzes ihre Stärken und Interessen zu erkunden, die sie mit digitalen Berufen in Verbindung bringen. Die Lernenden reflektieren ihre Ergebnisse, diskutieren in Gruppen und teilen ihre Erkenntnisse auf einer gemeinsamen Pinnwand. Eine gute Möglichkeit, Neugier zu wecken und die Berufsorientierung zu individualisieren – ideal für Präsenz- und Fernunterricht.</t>
+    <t>Uploaded 4 September 2025
+Diese Aktivität lädt Schüler*innen ein, mit spannenden Online-Quizzes ihre Stärken und Interessen zu erkunden, die sie mit digitalen Berufen in Verbindung bringen. Die Lernenden reflektieren ihre Ergebnisse, diskutieren in Gruppen und teilen ihre Erkenntnisse auf einer gemeinsamen Pinnwand. Eine gute Möglichkeit, Neugier zu wecken und die Berufsorientierung zu individualisieren – ideal für Präsenz- und Fernunterricht.</t>
   </si>
   <si>
     <t>Ανακάλυψε τον ψηφιακό σου τύπο</t>
   </si>
   <si>
-    <t>Αυτή η δραστηριότητα προσκαλεί τους μαθητές να διερευνήσουν τις δυνάμεις και τα ενδιαφέροντά τους μέσω διαδραστικών διαδικτυακών quiz που τους συνδέουν με ψηφιακές καριέρες. Οι μαθητές αναλύουν τα αποτελέσματά τους, συζητούν σε ομάδες και μοιράζονται τα ευρήματά τους σε έναν τοίχο συνεργασίας. Μια εξαιρετική μέθοδος για την ενίσχυση της περιέργειας και την εξατομικευμένη διερεύνηση σταδιοδρομίας– ιδανική για φυσική ή εξ αποστάσεως διδασκαλία.</t>
+    <t>Uploaded 4 September 2025
+Αυτή η δραστηριότητα προσκαλεί τους μαθητές να διερευνήσουν τις δυνάμεις και τα ενδιαφέροντά τους μέσω διαδραστικών διαδικτυακών quiz που τους συνδέουν με ψηφιακές καριέρες. Οι μαθητές αναλύουν τα αποτελέσματά τους, συζητούν σε ομάδες και μοιράζονται τα ευρήματά τους σε έναν τοίχο συνεργασίας. Μια εξαιρετική μέθοδος για την ενίσχυση της περιέργειας και την εξατομικευμένη διερεύνηση σταδιοδρομίας– ιδανική για φυσική ή εξ αποστάσεως διδασκαλία.</t>
   </si>
   <si>
     <t>Scopri il tuo tipo digitale</t>
   </si>
   <si>
-    <t>Questa attività invita gli studenti a esplorare i propri punti di forza e interessi attraverso quiz online coinvolgenti che li collegano a carriere digitali. Gli studenti riflettono sui risultati, discutono in gruppo e condividono le loro intuizioni su una bacheca collaborativa. Un ottimo modo per stimolare la curiosità e personalizzare l’esplorazione della carriera – ideale sia in classe che a distanza.</t>
+    <t>Uploaded 4 September 2025
+Questa attività invita gli studenti a esplorare i propri punti di forza e interessi attraverso quiz online coinvolgenti che li collegano a carriere digitali. Gli studenti riflettono sui risultati, discutono in gruppo e condividono le loro intuizioni su una bacheca collaborativa. Un ottimo modo per stimolare la curiosità e personalizzare l’esplorazione della carriera – ideale sia in classe che a distanza.</t>
   </si>
   <si>
     <t>Atklāj savu digitālo tipu</t>
   </si>
   <si>
-    <t>Šī aktivitāte aicina skolēnus izpētīt savas stiprās puses un intereses, izmantojot saistošus tiešsaistes testus, kas tos sasaista ar digitālajām karjerām. Skolēni pārdomā rezultātus, diskutē grupās un dalās iespaidos kopīgā sienā. Lielisks veids, kā rosināt zinātkāri un personalizēt karjeras izpēti – piemērots gan klātienes, gan attālinātām nodarbībām.</t>
+    <t>Uploaded 4 September 2025
+Šī aktivitāte aicina skolēnus izpētīt savas stiprās puses un intereses, izmantojot saistošus tiešsaistes testus, kas tos sasaista ar digitālajām karjerām. Skolēni pārdomā rezultātus, diskutē grupās un dalās iespaidos kopīgā sienā. Lielisks veids, kā rosināt zinātkāri un personalizēt karjeras izpēti – piemērots gan klātienes, gan attālinātām nodarbībām.</t>
   </si>
   <si>
     <t>Atraskite savo skaitmeninį tipą</t>
   </si>
   <si>
-    <t>Šioje veikloje mokiniai kviečiami ištirti savo stipriąsias puses ir pomėgius atliekant įdomius internetinius testus, kurie padeda susieti juos su skaitmenine karjera. Mokiniai aptaria rezultatus, diskutuoja grupėse ir dalijasi savo įžvalgomis bendroje lentoje. Puikus būdas skatinti smalsumą ir suasmeninti karjeros galimybių tyrinėjimą – tinkantis ir klasėje, ir nuotoliniu būdu.</t>
+    <t>Uploaded 4 September 2025
+Šioje veikloje mokiniai kviečiami ištirti savo stipriąsias puses ir pomėgius atliekant įdomius internetinius testus, kurie padeda susieti juos su skaitmenine karjera. Mokiniai aptaria rezultatus, diskutuoja grupėse ir dalijasi savo įžvalgomis bendroje lentoje. Puikus būdas skatinti smalsumą ir suasmeninti karjeros galimybių tyrinėjimą – tinkantis ir klasėje, ir nuotoliniu būdu.</t>
   </si>
   <si>
     <t>Skopri t-tip diġitali tiegħek</t>
   </si>
   <si>
-    <t>Din l-attività tistieden lill-istudenti jesploraw is-saħħiet u l-interessi tagħhom permezz ta’ kwizzijiet online interattivi li jqabbduhom ma’ karrieri diġitali. L-istudenti jirriflettu fuq ir-riżultati, jiddiskutu f’gruppi u jaqsmu l-ħsibijiet tagħhom fuq ħajt kollaborattiv. Mod mill-aqwa biex tqanqal il-kurżità u tippersonalizza l-esplorazzjoni tal-karriera – ideali kemm fil-klassi kif ukoll f’ambjent remoti.</t>
+    <t>Uploaded 4 September 2025
+Din l-attività tistieden lill-istudenti jesploraw is-saħħiet u l-interessi tagħhom permezz ta’ kwizzijiet online interattivi li jqabbduhom ma’ karrieri diġitali. L-istudenti jirriflettu fuq ir-riżultati, jiddiskutu f’gruppi u jaqsmu l-ħsibijiet tagħhom fuq ħajt kollaborattiv. Mod mill-aqwa biex tqanqal il-kurżità u tippersonalizza l-esplorazzjoni tal-karriera – ideali kemm fil-klassi kif ukoll f’ambjent remoti.</t>
   </si>
   <si>
     <t>Odkryj swój cyfrowy typ</t>
   </si>
   <si>
-    <t>To ćwiczenie zachęca uczniów do poznawania swoich mocnych stron i zainteresowań za pomocą angażujących quizów online, które dopasowują ich do cyfrowych ścieżek kariery. Uczniowie analizują wyniki, dyskutują w grupach i dzielą się przemyśleniami na wspólnej tablicy. Świetny sposób na rozbudzenie ciekawości i spersonalizowanie eksploracji kariery – idealny do pracy w klasie i zdalnie.</t>
+    <t>Uploaded 4 September 2025
+To ćwiczenie zachęca uczniów do poznawania swoich mocnych stron i zainteresowań za pomocą angażujących quizów online, które dopasowują ich do cyfrowych ścieżek kariery. Uczniowie analizują wyniki, dyskutują w grupach i dzielą się przemyśleniami na wspólnej tablicy. Świetny sposób na rozbudzenie ciekawości i spersonalizowanie eksploracji kariery – idealny do pracy w klasie i zdalnie.</t>
   </si>
   <si>
     <t>Descubra o seu tipo digital</t>
   </si>
   <si>
-    <t>Esta atividade convida os alunos a explorarem os seus pontos fortes e interesses através de questionários online envolventes que os associam a carreiras digitais. Os alunos refletem sobre os resultados, discutem em grupo e partilham as suas ideias numa parede colaborativa. Uma excelente forma de despertar a curiosidade e personalizar a exploração de carreiras – ideal tanto para o ensino presencial como à distância.</t>
+    <t>Uploaded 4 September 2025
+Esta atividade convida os alunos a explorarem os seus pontos fortes e interesses através de questionários online envolventes que os associam a carreiras digitais. Os alunos refletem sobre os resultados, discutem em grupo e partilham as suas ideias numa parede colaborativa. Uma excelente forma de despertar a curiosidade e personalizar a exploração de carreiras – ideal tanto para o ensino presencial como à distância.</t>
   </si>
   <si>
     <t>Descoperă-ți stilul digital</t>
   </si>
   <si>
-    <t>Această activitate îi invită pe elevi să își exploreze punctele forte și interesele prin quizuri online captivante care îi asociază cu cariere digitale. Elevii reflectează asupra rezultatelor, discută în grupuri și își împărtășesc ideile pe un perete colaborativ. O modalitate excelentă de a stârni curiozitatea și de a personaliza explorarea carierei – ideală atât pentru lecții față în față, cât și la distanță.</t>
+    <t>Uploaded 4 September 2025
+Această activitate îi invită pe elevi să își exploreze punctele forte și interesele prin quizuri online captivante care îi asociază cu cariere digitale. Elevii reflectează asupra rezultatelor, discută în grupuri și își împărtășesc ideile pe un perete colaborativ. O modalitate excelentă de a stârni curiozitatea și de a personaliza explorarea carierei – ideală atât pentru lecții față în față, cât și la distanță.</t>
   </si>
   <si>
     <t>Objavte svoj digitálny typ</t>
   </si>
   <si>
-    <t>Ova aktivita pozýva študentov, aby preskúmali svoje silné stránky a záujmy prostredníctvom zábavných online kvízov, ktoré ich spájajú s digitálnymi kariérami. Žiaci sa zamýšľajú nad svojimi výsledkami, diskutujú v skupinách a zdieľajú svoje postrehy na spoločnej nástenke. Skvelý spôsob, ako prebudiť zvedavosť a prispôsobiť objavovanie kariéry – ideálne pre výučbu v triede aj na diaľku.</t>
+    <t>Uploaded 4 September 2025
+Ova aktivita pozýva študentov, aby preskúmali svoje silné stránky a záujmy prostredníctvom zábavných online kvízov, ktoré ich spájajú s digitálnymi kariérami. Žiaci sa zamýšľajú nad svojimi výsledkami, diskutujú v skupinách a zdieľajú svoje postrehy na spoločnej nástenke. Skvelý spôsob, ako prebudiť zvedavosť a prispôsobiť objavovanie kariéry – ideálne pre výučbu v triede aj na diaľku.</t>
   </si>
   <si>
     <t>Odkrij svojo digitalno kariero</t>
   </si>
   <si>
-    <t>Aktivnost spodbuja učence, da raziskujejo svoje močne strani in interese s pomočjo zanimivih spletnih kvizov, ki jih povezujejo z digitalnimi karierami. Učenci razmišljajo o rezultatih, razpravljajo v skupinah in delijo svoja opažanja. Aktivnost je odličen način za spodbujanje radovednosti in individualnega raziskovanja karier – primerna je za izvajanje v učilnici ali na daljavo.</t>
+    <t>Uploaded 4 September 2025
+Aktivnost spodbuja učence, da raziskujejo svoje močne strani in interese s pomočjo zanimivih spletnih kvizov, ki jih povezujejo z digitalnimi karierami. Učenci razmišljajo o rezultatih, razpravljajo v skupinah in delijo svoja opažanja. Aktivnost je odličen način za spodbujanje radovednosti in individualnega raziskovanja karier – primerna je za izvajanje v učilnici ali na daljavo.</t>
   </si>
   <si>
     <t>Descubre tu tipo digital</t>
   </si>
   <si>
-    <t>Esta actividad invita al alumnado a explorar sus fortalezas e intereses a través de cuestionarios en línea atractivos que los conectan con distintas carreras digitales. Después, reflexionan sobre sus resultados, debaten en grupo y comparten sus ideas en un mural colaborativo. Es una forma excelente de despertar la curiosidad y personalizar la orientación profesional, ideal tanto para clases presenciales como a distancia.</t>
+    <t>Uploaded 4 September 2025
+Esta actividad invita al alumnado a explorar sus fortalezas e intereses a través de cuestionarios en línea atractivos que los conectan con distintas carreras digitales. Después, reflexionan sobre sus resultados, debaten en grupo y comparten sus ideas en un mural colaborativo. Es una forma excelente de despertar la curiosidad y personalizar la orientación profesional, ideal tanto para clases presenciales como a distancia.</t>
   </si>
   <si>
     <t>Löydä digityyppisi</t>
   </si>
   <si>
-    <t>Tämä tehtävä kannustaa oppilaita tutkimaan omia vahvuuksiaan ja kiinnostuksen kohteitaan mukaansatempaavien verkkotestien avulla, jotka yhdistävät heidät digitaalisiin urapolkuihin. Oppilaat pohtivat tuloksiaan, keskustelevat ryhmissä ja jakavat oivalluksiaan yhteisellä seinällä. Loistava tapa herättää uteliaisuutta ja tehdä uratutkimuksesta henkilökohtaisempaa – sopii sekä lähi- että etäopetukseen.</t>
+    <t>Uploaded 4 September 2025
+Tämä tehtävä kannustaa oppilaita tutkimaan omia vahvuuksiaan ja kiinnostuksen kohteitaan mukaansatempaavien verkkotestien avulla, jotka yhdistävät heidät digitaalisiin urapolkuihin. Oppilaat pohtivat tuloksiaan, keskustelevat ryhmissä ja jakavat oivalluksiaan yhteisellä seinällä. Loistava tapa herättää uteliaisuutta ja tehdä uratutkimuksesta henkilökohtaisempaa – sopii sekä lähi- että etäopetukseen.</t>
   </si>
   <si>
     <t>Upptäck din digitala typ</t>
   </si>
   <si>
-    <t xml:space="preserve">Den här aktiviteten uppmuntrar elever att utforska sina styrkor och intressen genom engagerande onlinequiz som matchar dem med digitala yrken. Eleverna reflekterar över sina resultat, diskuterar i grupper och delar sina insikter på en gemensam vägg. Ett utmärkt sätt att väcka nyfikenhet och göra karriärutforskning mer personlig – perfekt för både klassrummet och distansundervisning. </t>
+    <t xml:space="preserve">Uploaded 4 September 2025
+Den här aktiviteten uppmuntrar elever att utforska sina styrkor och intressen genom engagerande onlinequiz som matchar dem med digitala yrken. Eleverna reflekterar över sina resultat, diskuterar i grupper och delar sina insikter på en gemensam vägg. Ett utmärkt sätt att väcka nyfikenhet och göra karriärutforskning mer personlig – perfekt för både klassrummet och distansundervisning. </t>
   </si>
   <si>
     <t>Dijital Tipinizi Keşfedin</t>
   </si>
   <si>
-    <t>Bu etkinlik, öğrencileri dijital kariyerlerle eşleştiren ilgi çekici çevrimiçi testler aracılığıyla güçlü yönlerini ve ilgi alanlarını keşfetmeye davet eder. Öğrenciler sonuçları üzerinde düşünür, gruplar halinde tartışır ve fikirlerini ortak bir duvarda paylaşır. Merak uyandırmanın ve kariyer keşfini kişiselleştirmenin harika bir yolu; hem sınıf içi hem de uzaktan eğitim için idealdir</t>
+    <t>Uploaded 4 September 2025
+Bu etkinlik, öğrencileri dijital kariyerlerle eşleştiren ilgi çekici çevrimiçi testler aracılığıyla güçlü yönlerini ve ilgi alanlarını keşfetmeye davet eder. Öğrenciler sonuçları üzerinde düşünür, gruplar halinde tartışır ve fikirlerini ortak bir duvarda paylaşır. Merak uyandırmanın ve kariyer keşfini kişiselleştirmenin harika bir yolu; hem sınıf içi hem de uzaktan eğitim için idealdir</t>
   </si>
   <si>
     <t>Визнач свій цифровий тип</t>
   </si>
   <si>
-    <t>Ця активність пропонує здобувачам освіти дослідити свої сильні сторони та інтереси за допомогою інтерактивних онлайн-тестів, що допомагають зв’язати їх з цифровими професіями. Здобувачі освіти аналізують результати, обговорюють їх у групах і діляться думками на спільній онлайн-стіні. Це чудовий спосіб пробудити інтерес і персоналізувати профорієнтацію. Активність підходить як для очного, так і дистанційного навчання.</t>
-  </si>
-  <si>
-    <t>Prezanto punën tuaj të ëndrrave në botën digjitale</t>
-  </si>
-  <si>
-    <t>Nxënësit eksplorojnë karriera digjitale duke hulumtuar dhe prezantuar një rol që i frymëzon. Duke përdorur një listë të përzgjedhur dhe një model të thjeshtë, ata theksojnë aftësitë kryesore, detyrat e punës dhe ekspertët e industrisë. Kjo aktivitet zhvillon aftësi kërkimore, mendim kritik dhe aftësi prezantimi – ideale për klasat që fokusohen në përgatitjen për karrierë dhe zërin e nxënësve.</t>
+    <t>Uploaded 4 September 2025
+Ця активність пропонує здобувачам освіти дослідити свої сильні сторони та інтереси за допомогою інтерактивних онлайн-тестів, що допомагають зв’язати їх з цифровими професіями. Здобувачі освіти аналізують результати, обговорюють їх у групах і діляться думками на спільній онлайн-стіні. Це чудовий спосіб пробудити інтерес і персоналізувати профорієнтацію. Активність підходить як для очного, так і дистанційного навчання.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prezanto punën tuaj të ëndrrave në botën digjitale </t>
+  </si>
+  <si>
+    <t>Uploaded 4 September 2025
+Nxënësit eksplorojnë karriera digjitale duke hulumtuar dhe prezantuar një rol që i frymëzon. Duke përdorur një listë të përzgjedhur dhe një model të thjeshtë, ata theksojnë aftësitë kryesore, detyrat e punës dhe ekspertët e industrisë. Kjo aktivitet zhvillon aftësi kërkimore, mendim kritik dhe aftësi prezantimi – ideale për klasat që fokusohen në përgatitjen për karrierë dhe zërin e nxënësve.</t>
   </si>
   <si>
     <t>Представи мечтаната си дигитална професия</t>
   </si>
   <si>
-    <t>Учениците разглеждат дигитални кариери, като проучват и представят роля, която ги вдъхновява. Използвайки подбрани списъци и опростен шаблон, те подчертават ключови умения, задачи и експерти в индустрията. Тази дейност развива умения за проучване, критично мислене и презентация – идеална за класни стаи, ориентирани към професионално развитие и ученически глас.</t>
+    <t>Uploaded 4 September 2025
+Учениците разглеждат дигитални кариери, като проучват и представят роля, която ги вдъхновява. Използвайки подбрани списъци и опростен шаблон, те подчертават ключови умения, задачи и експерти в индустрията. Тази дейност развива умения за проучване, критично мислене и презентация – идеална за класни стаи, ориентирани към професионално развитие и ученически глас.</t>
   </si>
   <si>
     <t>Predstavi svoj posao iz snova u digitalnom svijetu</t>
   </si>
   <si>
-    <t>Učenici istražuju digitalne karijere tako da prouče i predstave zanimanje koje ih inspirira. Koristeći unaprijed pripremljen popis i upute, učenici ističu ključne vještine, odgovornosti, zadatke i stručnjake iz industrije. Ova aktivnost razvija istraživačke sposobnosti, kritičko razmišljanje i prezentacijske vještine - prikladna je za nastavu uživo ili na daljinu.</t>
+    <t>Uploaded 4 September 2025
+Učenici istražuju digitalne karijere tako da prouče i predstave zanimanje koje ih inspirira. Koristeći unaprijed pripremljen popis i upute, učenici ističu ključne vještine, odgovornosti, zadatke i stručnjake iz industrije. Ova aktivnost razvija istraživačke sposobnosti, kritičko razmišljanje i prezentacijske vještine - prikladna je za nastavu uživo ili na daljinu.</t>
   </si>
   <si>
     <t xml:space="preserve">Představte si svou vysněnou digitální práci 
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Studenti zkoumají digitální kariéry prostřednictvím výzkumu a prezentace role, která je inspiruje. Pomocí vybraného seznamu a jednoduché šablony zdůrazňují klíčové dovednosti, pracovní úkoly a odborníky z oboru. Tato aktivita rozvíjí výzkumné, kritické a prezentační dovednosti – ideální pro třídy zaměřené na kariérní připravenost a hlas studentů. </t>
+    <t xml:space="preserve">Uploaded 4 September 2025
+Studenti zkoumají digitální kariéry prostřednictvím výzkumu a prezentace role, která je inspiruje. Pomocí vybraného seznamu a jednoduché šablony zdůrazňují klíčové dovednosti, pracovní úkoly a odborníky z oboru. Tato aktivita rozvíjí výzkumné, kritické a prezentační dovednosti – ideální pro třídy zaměřené na kariérní připravenost a hlas studentů. </t>
   </si>
   <si>
     <t>Præsenter dit digitale drømmejob</t>
   </si>
   <si>
-    <t>Eleverne udforsker digitale karrierer ved at undersøge og præsentere en rolle, der inspirerer dem. Ved hjælp af en udvalgt liste og en enkel skabelon fremhæver de nøglefærdigheder, jobopgaver og brancheeksperter. Denne aktivitet styrker research, kritisk tænkning og præsentationsevner – ideel til klasselokaler med fokus på karriereparathed og elevstemme.</t>
+    <t>Uploaded 4 September 2025
+Eleverne udforsker digitale karrierer ved at undersøge og præsentere en rolle, der inspirerer dem. Ved hjælp af en udvalgt liste og en enkel skabelon fremhæver de nøglefærdigheder, jobopgaver og brancheeksperter. Denne aktivitet styrker research, kritisk tænkning og præsentationsevner – ideel til klasselokaler med fokus på karriereparathed og elevstemme.</t>
   </si>
   <si>
     <t>Presenteer je digitale droombaan</t>
   </si>
   <si>
-    <t>Leerlingen verkennen digitale carrières door een functie te onderzoeken en te presenteren die hen inspireert. Met behulp van een samengestelde lijst en een eenvoudig sjabloon belichten ze kernvaardigheden, taken en experts uit de sector. Deze activiteit versterkt onderzoeks-, kritisch denk- en presentatievaardigheden – ideaal voor klaslokalen die gericht zijn op loopbaanvoorbereiding en leerlingbetrokkenheid.</t>
+    <t>Uploaded 4 September 2025
+Leerlingen verkennen digitale carrières door een functie te onderzoeken en te presenteren die hen inspireert. Met behulp van een samengestelde lijst en een eenvoudig sjabloon belichten ze kernvaardigheden, taken en experts uit de sector. Deze activiteit versterkt onderzoeks-, kritisch denk- en presentatievaardigheden – ideaal voor klaslokalen die gericht zijn op loopbaanvoorbereiding en leerlingbetrokkenheid.</t>
   </si>
   <si>
     <t>Present Your Dream Digital Job</t>
   </si>
   <si>
-    <t xml:space="preserve">Students explore digital careers by researching and presenting a role that inspires them. Using a curated list and a simple template, they highlight key skills, job tasks, and industry experts. This activity builds research, critical thinking, and presentation skills - ideal for classrooms focused on career readiness and student voice. </t>
+    <t xml:space="preserve">Uploaded 4 September 2025
+Students explore digital careers by researching and presenting a role that inspires them. Using a curated list and a simple template, they highlight key skills, job tasks, and industry experts. This activity builds research, critical thinking, and presentation skills - ideal for classrooms focused on career readiness and student voice. </t>
   </si>
   <si>
     <t>Présente ton métier numérique de rêve</t>
   </si>
   <si>
-    <t>Les élèves explorent les carrières du secteur numérique en recherchant et présentant un métier qui les inspire. À l’aide d’une liste de métiers et d’un modèle simple à remplir, ils mettent en avant les compétences clés, les missions et les experts du métier choisi. Cette activité permet aux élèves de développer leurs compétences en recherche, en pensée critique et en expression orale. Elle est particulièrement adaptée aux classes travaillant sur l’orientation professionnelle et la prise de parole.</t>
+    <t>Uploaded 4 September 2025
+Les élèves explorent les carrières du secteur numérique en recherchant et présentant un métier qui les inspire. À l’aide d’une liste de métiers et d’un modèle simple à remplir, ils mettent en avant les compétences clés, les missions et les experts du métier choisi. Cette activité permet aux élèves de développer leurs compétences en recherche, en pensée critique et en expression orale. Elle est particulièrement adaptée aux classes travaillant sur l’orientation professionnelle et la prise de parole.</t>
   </si>
   <si>
     <t>Stelle deinen digitalen Traumberuf vor</t>
   </si>
   <si>
-    <t>Schüler*innen erkunden digitale Berufe, indem sie zu einem Berufsfeld, das sie inspiriert, recherchieren und referieren. Mit einer kuratierten Liste von Berufen und einer einfachen Vorlage arbeiten sie wichtige Fähigkeiten und Aufgaben heraus und stellen Branchenexpert*innen vor. Diese Aktivität fördert Recherchefähigkeiten, kritisches Denken und Präsentationskompetenz – ideal für Berufsorientierung im Unterricht und die Förderung von Mitbestimmungsmöglichkeiten.</t>
+    <t>Uploaded 4 September 2025
+Schüler*innen erkunden digitale Berufe, indem sie zu einem Berufsfeld, das sie inspiriert, recherchieren und referieren. Mit einer kuratierten Liste von Berufen und einer einfachen Vorlage arbeiten sie wichtige Fähigkeiten und Aufgaben heraus und stellen Branchenexpert*innen vor. Diese Aktivität fördert Recherchefähigkeiten, kritisches Denken und Präsentationskompetenz – ideal für Berufsorientierung im Unterricht und die Förderung von Mitbestimmungsmöglichkeiten.</t>
   </si>
   <si>
     <t>Παρουσίασε το ψηφιακό επάγγελμα των ονείρων σου</t>
   </si>
   <si>
-    <t>Οι μαθητές εξερευνούν τα ψηφιακά επαγγέλματα, ερευνώντας και παρουσιάζοντας έναν ρόλο που τους εμπνέει. Χρησιμοποιώντας μία επιλεγμένη λίστα και ένα απλό πρότυπο έντυπο, αναδεικνύουν βασικές δεξιότητες, εργασιακά καθήκοντα και ειδικούς του κλάδου. Η δραστηριότητα αναπτύσσει δεξιότητες έρευνας, κριτικής σκέψης και παρουσίασης – ιδανική για τάξεις με έμφαση στην επαγγελματική προετοιμασία και την έκφραση των μαθητών.</t>
+    <t>Uploaded 4 September 2025
+Οι μαθητές εξερευνούν τα ψηφιακά επαγγέλματα, ερευνώντας και παρουσιάζοντας έναν ρόλο που τους εμπνέει. Χρησιμοποιώντας μία επιλεγμένη λίστα και ένα απλό πρότυπο έντυπο, αναδεικνύουν βασικές δεξιότητες, εργασιακά καθήκοντα και ειδικούς του κλάδου. Η δραστηριότητα αναπτύσσει δεξιότητες έρευνας, κριτικής σκέψης και παρουσίασης – ιδανική για τάξεις με έμφαση στην επαγγελματική προετοιμασία και την έκφραση των μαθητών.</t>
   </si>
   <si>
     <t>Presenta il tuo lavoro digital dei sogni</t>
   </si>
   <si>
-    <t>Gli studenti esplorano le carriere digitali ricercando e presentando un ruolo che li ispira. Usando un elenco selezionato e un modello semplice, evidenziano competenze chiave, mansioni ed esperti del settore. Questa attività sviluppa capacità di ricerca, pensiero critico e competenze sulle presentazioni – ideale per le classi orientate alla carriera e a dare voce agli studenti.</t>
+    <t>Uploaded 4 September 2025
+Gli studenti esplorano le carriere digitali ricercando e presentando un ruolo che li ispira. Usando un elenco selezionato e un modello semplice, evidenziano competenze chiave, mansioni ed esperti del settore. Questa attività sviluppa capacità di ricerca, pensiero critico e competenze sulle presentazioni – ideale per le classi orientate alla carriera e a dare voce agli studenti.</t>
   </si>
   <si>
     <t>Prezentē savu sapņu digitālo profesiju</t>
   </si>
   <si>
-    <t>Skolēni pēta digitālās karjeras, izpētot un prezentējot lomu, kas viņus iedvesmo. Izmantojot atlasītu sarakstu un vienkāršu veidni, viņi izceļ galvenās prasmes, darba uzdevumus un nozares ekspertus. Šī aktivitāte attīsta pētniecības, kritiskās domāšanas un prezentēšanas prasmes – lieliski piemērota klasēm, kas fokusējas uz karjeras sagatavotību un skolēnu balsi.</t>
+    <t>Uploaded 4 September 2025
+Skolēni pēta digitālās karjeras, izpētot un prezentējot lomu, kas viņus iedvesmo. Izmantojot atlasītu sarakstu un vienkāršu veidni, viņi izceļ galvenās prasmes, darba uzdevumus un nozares ekspertus. Šī aktivitāte attīsta pētniecības, kritiskās domāšanas un prezentēšanas prasmes – lieliski piemērota klasēm, kas fokusējas uz karjeras sagatavotību un skolēnu balsi.</t>
   </si>
   <si>
     <t>Pristatykite savo svajonių skaitmeninį darbą</t>
   </si>
   <si>
-    <t>Mokiniai nagrinėja skaitmeninės karjeros galimybes ieškodami ir pristatydami įdomias profesijas. Naudodamiesi sudarytu sąrašu ir paprastu šablonu, jie įvardija pagrindinius įgūdžius, darbo užduotis ir šios srities ekspertus. Ši veikla lavina tyrinėjimo, kritinio mąstymo ir pristatymo įgūdžius - puikiai tinka į karjerą orientuotoms pamokoms ir mokinių saviraiškai.</t>
+    <t>Uploaded 4 September 2025
+Mokiniai nagrinėja skaitmeninės karjeros galimybes ieškodami ir pristatydami įdomias profesijas. Naudodamiesi sudarytu sąrašu ir paprastu šablonu, jie įvardija pagrindinius įgūdžius, darbo užduotis ir šios srities ekspertus. Ši veikla lavina tyrinėjimo, kritinio mąstymo ir pristatymo įgūdžius - puikiai tinka į karjerą orientuotoms pamokoms ir mokinių saviraiškai.</t>
   </si>
   <si>
     <t>Ippreżenta l-impjieg diġitali tal-ħolm tiegħek</t>
   </si>
   <si>
-    <t>L-istudenti jesploraw karrieri diġitali billi jagħmlu riċerka u jippreżentaw rwol li jispirahom. Bl-użu ta’ lista magħżula u mudell sempliċi, juru ħiliet ewlenin, kompiti tax-xogħol u esperti tal-industrija. Din l-attività tibni ħiliet ta’ riċerka, ħsieb kritiku u ta’ preżentazzjoni – ideali għal klassijiet iffokati fuq il-karrieri u l-vuċi tal-istudenti.</t>
+    <t>Uploaded 4 September 2025
+L-istudenti jesploraw karrieri diġitali billi jagħmlu riċerka u jippreżentaw rwol li jispirahom. Bl-użu ta’ lista magħżula u mudell sempliċi, juru ħiliet ewlenin, kompiti tax-xogħol u esperti tal-industrija. Din l-attività tibni ħiliet ta’ riċerka, ħsieb kritiku u ta’ preżentazzjoni – ideali għal klassijiet iffokati fuq il-karrieri u l-vuċi tal-istudenti.</t>
   </si>
   <si>
     <t>Przedstaw swoją wymarzoną cyfrową pracę</t>
   </si>
   <si>
-    <t>Uczniowie poznają cyfrowe ścieżki kariery, badając i prezentując zawód, który ich inspiruje. Korzystając z wybranej listy i prostego szablonu, przedstawiają kluczowe umiejętności, zadania zawodowe i ekspertów branżowych. Ta aktywność rozwija umiejętności badawcze, krytyczne myślenie i prezentację – idealna dla klas przygotowujących do kariery i wspierających głos ucznia.</t>
+    <t>Uploaded 4 September 2025
+Uczniowie poznają cyfrowe ścieżki kariery, badając i prezentując zawód, który ich inspiruje. Korzystając z wybranej listy i prostego szablonu, przedstawiają kluczowe umiejętności, zadania zawodowe i ekspertów branżowych. Ta aktywność rozwija umiejętności badawcze, krytyczne myślenie i prezentację – idealna dla klas przygotowujących do kariery i wspierających głos ucznia.</t>
   </si>
   <si>
     <t>Apresenta o teu emprego digital de sonh</t>
   </si>
   <si>
-    <t>Os alunos exploram carreiras digitais investigando e apresentando uma função que os inspira. Usando uma lista selecionada e um modelo simples, destacam competências-chave, tarefas e especialistas da indústria. Esta atividade desenvolve competências de pesquisa, pensamento crítico e apresentação – ideal para salas de aula focadas em preparação para a carreira e na voz do aluno.</t>
+    <t>Uploaded 4 September 2025
+Os alunos exploram carreiras digitais investigando e apresentando uma função que os inspira. Usando uma lista selecionada e um modelo simples, destacam competências-chave, tarefas e especialistas da indústria. Esta atividade desenvolve competências de pesquisa, pensamento crítico e apresentação – ideal para salas de aula focadas em preparação para a carreira e na voz do aluno.</t>
   </si>
   <si>
     <t>Prezintă-ți jobul digital de vis</t>
   </si>
   <si>
-    <t>Elevii explorează cariere digitale cercetând și prezentând un rol care îi inspiră. Folosind o listă selectată și un șablon simplu, evidențiază abilități cheie, sarcini specifice și experți din industrie. Activitatea dezvoltă abilități de cercetare, gândire critică și prezentare – ideală pentru clase axate pe orientare profesională și implicarea elevilor.</t>
+    <t>Uploaded 4 September 2025
+Elevii explorează cariere digitale cercetând și prezentând un rol care îi inspiră. Folosind o listă selectată și un șablon simplu, evidențiază abilități cheie, sarcini specifice și experți din industrie. Activitatea dezvoltă abilități de cercetare, gândire critică și prezentare – ideală pentru clase axate pe orientare profesională și implicarea elevilor.</t>
   </si>
   <si>
     <t>Predstav si svoju vysnívanú digitálnu prácu</t>
   </si>
   <si>
-    <t xml:space="preserve">Žiaci skúmajú digitálne povolania prostredníctvom výskumu a prezentácie roly, ktorá ich inšpiruje. Pomocou vybraného zoznamu a jednoduchej šablóny zvýraznia kľúčové zručnosti, pracovné úlohy a odborníkov z odvetvia. Aktivita rozvíja výskumné, kritické a prezentačné zručnosti – ideálna pre triedy zamerané na kariérnu pripravenosť a hlas žiakov. </t>
+    <t xml:space="preserve">Uploaded 4 September 2025
+Žiaci skúmajú digitálne povolania prostredníctvom výskumu a prezentácie roly, ktorá ich inšpiruje. Pomocou vybraného zoznamu a jednoduchej šablóny zvýraznia kľúčové zručnosti, pracovné úlohy a odborníkov z odvetvia. Aktivita rozvíja výskumné, kritické a prezentačné zručnosti – ideálna pre triedy zamerané na kariérnu pripravenosť a hlas žiakov. </t>
   </si>
   <si>
     <t>Predstavi svojo sanjsko službo v digitalnem svetu</t>
   </si>
   <si>
-    <t>Učenci raziskujejo digitalne kariere tako, da preučijo in predstavijo poklic, ki jih navdihuje. S pomočjo vnaprej pripravljenega seznama in navodil učenci izpostavijo ključne veščine, odgovornosti, naloge in strokovnjake iz industrije. Aktivnost razvija raziskovalne sposobnosti, kritično razmišljanje in predstavitvene veščine – primerna je za izvajanje pri pouku v živo ali na daljavo.</t>
-  </si>
-  <si>
-    <t>Presenta el trabajo digital de tus sueños</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Los estudiantes exploran carreras digitales investigando y presentando un rol que los inspire. Usan una lista seleccionada y una plantilla sencilla para resaltar habilidades clave, tareas del puesto y expertos del sector. Esta actividad desarrolla habilidades de investigación, pensamiento crítico y presentación – ideal para aulas centradas en la orientación profesional y la voz estudiantil. </t>
+    <t>Uploaded 4 September 2025
+Učenci raziskujejo digitalne kariere tako, da preučijo in predstavijo poklic, ki jih navdihuje. S pomočjo vnaprej pripravljenega seznama in navodil učenci izpostavijo ključne veščine, odgovornosti, naloge in strokovnjake iz industrije. Aktivnost razvija raziskovalne sposobnosti, kritično razmišljanje in predstavitvene veščine – primerna je za izvajanje pri pouku v živo ali na daljavo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Presenta el trabajo digital de tus sueños </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uploaded 4 September 2025
+Los estudiantes exploran carreras digitales investigando y presentando un rol que los inspire. Usan una lista seleccionada y una plantilla sencilla para resaltar habilidades clave, tareas del puesto y expertos del sector. Esta actividad desarrolla habilidades de investigación, pensamiento crítico y presentación – ideal para aulas centradas en la orientación profesional y la voz estudiantil. </t>
   </si>
   <si>
     <t>Esittele unelmiesi digitaalinen työ</t>
   </si>
   <si>
-    <t>Oppilaat tutkivat digitaalisia urapolkuja tutkimalla ja esittelemällä roolin, joka inspiroi heitä. He käyttävät valikoitua listaa ja yksinkertaista mallia korostaakseen keskeisiä taitoja, työtehtäviä ja alan asiantuntijoita. Tämä tehtävä kehittää tutkimus-, kriittisen ajattelun ja esitystaitoja – ihanteellinen uravalmiuksiin ja oppilaslähtöisyyteen keskittyville oppitunneille.</t>
+    <t>Uploaded 4 September 2025
+Oppilaat tutkivat digitaalisia urapolkuja tutkimalla ja esittelemällä roolin, joka inspiroi heitä. He käyttävät valikoitua listaa ja yksinkertaista mallia korostaakseen keskeisiä taitoja, työtehtäviä ja alan asiantuntijoita. Tämä tehtävä kehittää tutkimus-, kriittisen ajattelun ja esitystaitoja – ihanteellinen uravalmiuksiin ja oppilaslähtöisyyteen keskittyville oppitunneille.</t>
   </si>
   <si>
     <t>Presentera ditt digitala drömjobb</t>
   </si>
   <si>
-    <t>Elever utforskar digitala karriärer genom att undersöka och presentera en roll som inspirerar dem. Med hjälp av en utvald lista och en enkel mall lyfter de fram viktiga färdigheter, arbetsuppgifter och branschexperter. Denna aktivitet utvecklar forskningsförmåga, kritiskt tänkande och presentationsfärdigheter – perfekt för klassrum med fokus på karriärförberedelse och elevröst.</t>
+    <t>Uploaded 4 September 2025
+Elever utforskar digitala karriärer genom att undersöka och presentera en roll som inspirerar dem. Med hjälp av en utvald lista och en enkel mall lyfter de fram viktiga färdigheter, arbetsuppgifter och branschexperter. Denna aktivitet utvecklar forskningsförmåga, kritiskt tänkande och presentationsfärdigheter – perfekt för klassrum med fokus på karriärförberedelse och elevröst.</t>
   </si>
   <si>
     <t>Hayalinizdeki Dijital İşi Sunun</t>
   </si>
   <si>
-    <t xml:space="preserve">Öğrenciler, kendilerine ilham veren bir rolü araştırıp sunarak dijital kariyerleri keşfederler. Özenle hazırlanmış bir liste ve basit bir şablon kullanarak temel becerileri, iş görevlerini ve sektör uzmanlarını vurgularlar. Bu etkinlik, araştırma, eleştirel düşünme ve sunum becerilerini geliştirir; kariyer hazırlığına ve öğrenci sesine odaklanan sınıflar için idealdir. </t>
+    <t xml:space="preserve">Uploaded 4 September 2025
+Öğrenciler, kendilerine ilham veren bir rolü araştırıp sunarak dijital kariyerleri keşfederler. Özenle hazırlanmış bir liste ve basit bir şablon kullanarak temel becerileri, iş görevlerini ve sektör uzmanlarını vurgularlar. Bu etkinlik, araştırma, eleştirel düşünme ve sunum becerilerini geliştirir; kariyer hazırlığına ve öğrenci sesine odaklanan sınıflar için idealdir. </t>
   </si>
   <si>
     <t>Презентуй свою цифрову роботу мрії</t>
   </si>
   <si>
-    <t>Здобувачі освіти досліджують цифрові професії, обираючи й презентуючи роль, яка їх надихає. Використовуючи підготовлений список і простий шаблон, вони висвітлюють ключові навички, основні обов’язки та відомих експертів у галузі. Ця активність розвиває навички дослідження, критичного мислення і презентації — ідеально підходить для класів із орієнтацією на кар’єрний розвиток та активну участь здобувачів освіти.</t>
-  </si>
-  <si>
-    <t>“Meitenes kodē labāk” sprints</t>
-  </si>
-  <si>
-    <t>Dinamiska 3–4 stundu darbnīca, kurā meitenes risina radošus tehnoloģiju izaicinājumus un izstrādā oriģinālus digitālos produktus. Ar praktisku vadību viņas jautrā un atbalstošā vidē iepazīstina ar kodēšanu, digitālo veidošanu un problēmu risināšanu. Lieliski piemērots zinātkāres rosināšanai un pārliecības veidošanai par tehnoloģijām — tiešsaistē vai klātienē.</t>
-  </si>
-  <si>
-    <t>„Girls Code It Better“ dirbtuvės</t>
-  </si>
-  <si>
-    <t>Dinamiškos 3–4 valandų dirbtuvės, kurioje merginos sprendžia kūrybinius technologijų iššūkius ir kuria originalius skaitmeninius produktus. Pagal praktinius nurodymus, jos smagioje ir palankioje aplinkoje susipažįsta su programavimu, skaitmenine kūryba ir problemų sprendimu. Puikiai tinka smalsumui sužadinti ir pasitikėjimui technologijomis ugdyti – internetu arba gyvai</t>
-  </si>
-  <si>
-    <t>Šprint “Girls Code It Better”</t>
-  </si>
-  <si>
-    <t>Dynamický 3–4 hodinový workshop, kde dievčatá riešia kreatívne technologické výzvy a navrhujú originálne digitálne produkty. S praktickým vedením skúmajú programovanie, digitálnu tvorbu a riešenie problémov v zábavnom a podpornom prostredí. Ideálne na prebudenie zvedavosti a budovanie sebadôvery v oblasti technológií—online alebo prezenčne.</t>
-  </si>
-  <si>
-    <t>Girls Code It Better Sprintti</t>
-  </si>
-  <si>
-    <t>Dynaaminen 3–4 tunnin työpaja, jossa tytöt ratkaisevat luovia teknologiahaasteita ja suunnittelevat omaperäisiä digitaalisia tuotteita. Käytännön ohjauksessa he tutustuvat ohjelmointiin, digitaaliseen luomiseen ja ongelmanratkaisuun hauskassa ja kannustavassa ympäristössä. Täydellinen tapa herättää uteliaisuutta ja vahvistaa itsevarmuutta teknologiassa—verkossa tai paikan päällä.</t>
-  </si>
-  <si>
-    <t>Kızlar Daha İyi Kod Yazıyor Sprinti</t>
-  </si>
-  <si>
-    <t>Kızların yaratıcı teknoloji zorluklarıyla mücadele edip özgün dijital ürünler tasarladıkları dinamik 3-4 saatlik bir atölye çalışması. Uygulamalı rehberlik eşliğinde, eğlenceli ve destekleyici bir ortamda kodlama, dijital üretim ve problem çözme becerilerini keşfediyorlar. Merak uyandırmak ve teknolojiye olan güveni artırmak için mükemmel bir seçenek - çevrimiçi veya yüz yüze.</t>
+    <t>Uploaded 4 September 2025
+Здобувачі освіти досліджують цифрові професії, обираючи й презентуючи роль, яка їх надихає. Використовуючи підготовлений список і простий шаблон, вони висвітлюють ключові навички, основні обов’язки та відомих експертів у галузі. Ця активність розвиває навички дослідження, критичного мислення і презентації — ідеально підходить для класів із орієнтацією на кар’єрний розвиток та активну участь здобувачів освіти.</t>
   </si>
   <si>
     <t>Aktiviteti Magic 8 Ball</t>
   </si>
   <si>
-    <t xml:space="preserve">Nxënësit eksplorojnë konceptet bazë të programimit duke krijuar një “Magic 8 Ball” digjital duke përdorur micro:bit dhe MakeCode. Në grupe, ata krijojnë një program që përdor sensorë dhe numra të rastësishëm për të gjeneruar përgjigje kur pajisja tundet. Ky aktivitet argëtues dhe praktik ndërton punën në ekip, prezanton mekatronikën dhe zhvillon aftësitë e programimit dhe zgjidhjes së problemeve. </t>
+    <t xml:space="preserve">Uploaded 4 September 2025
+Nxënësit eksplorojnë konceptet bazë të programimit duke krijuar një “Magic 8 Ball” digjital duke përdorur micro:bit dhe MakeCode. Në grupe, ata krijojnë një program që përdor sensorë dhe numra të rastësishëm për të gjeneruar përgjigje kur pajisja tundet. Ky aktivitet argëtues dhe praktik ndërton punën në ekip, prezanton mekatronikën dhe zhvillon aftësitë e programimit dhe zgjidhjes së problemeve. </t>
   </si>
   <si>
     <t>Дейност "Магическа топка 8"</t>
   </si>
   <si>
-    <t>Учениците изследват основни концепции за програмиране, като създават дигитална Магическа топка 8 с помощта на micro:bit и MakeCode. В екипи те проектират програма, която използва сензори и случайни числа за генериране на отговори при разклащане на устройството. Това забавно и практическо занимание изгражда умения за работа в екип, въвежда в мехатрониката и развива умения за програмиране и решаване на проблеми.</t>
+    <t>Uploaded 4 September 2025
+Учениците изследват основни концепции за програмиране, като създават дигитална Магическа топка 8 с помощта на micro:bit и MakeCode. В екипи те проектират програма, която използва сензори и случайни числа за генериране на отговори при разклащане на устройството. Това забавно и практическо занимание изгражда умения за работа в екип, въвежда в мехатрониката и развива умения за програмиране и решаване на проблеми.</t>
   </si>
   <si>
     <t>Aktivnost: Čarobna kugla broj 8 (Magic 8 Ball)</t>
   </si>
   <si>
-    <t xml:space="preserve">Učenici istražuju osnovne koncepte programiranja izrađujući čarobnu kuglu broj 8 (Magic 8 Ball) koristeći micro:bit i MakeCode. U timovima osmišljavaju program koji koristi senzore i nasumične brojeve za generiranje odgovora kada se uređaj protrese. Ova zabavna, praktična aktivnost potiče timski rad, uvodi u mehatroniku i razvija vještine programiranja i rješavanja problema. </t>
+    <t xml:space="preserve">Uploaded 4 September 2025
+Učenici istražuju osnovne koncepte programiranja izrađujući čarobnu kuglu broj 8 (Magic 8 Ball) koristeći micro:bit i MakeCode. U timovima osmišljavaju program koji koristi senzore i nasumične brojeve za generiranje odgovora kada se uređaj protrese. Ova zabavna, praktična aktivnost potiče timski rad, uvodi u mehatroniku i razvija vještine programiranja i rješavanja problema. </t>
   </si>
   <si>
     <t>Aktivita Magic 8 Ball</t>
   </si>
   <si>
-    <t>Studenti prozkoumávají základní koncepty programování vytvořením digitální Magic 8 Ball pomocí micro:bitu a MakeCode. V týmech navrhují program, který využívá senzory a náhodná čísla k generování odpovědí při zatřesení zařízení. Tato zábavná, praktická aktivita podporuje týmovou práci, seznamuje s mechatronikou a rozvíjí programátorské a řešitelské dovednosti.</t>
+    <t>Uploaded 4 September 2025
+Studenti prozkoumávají základní koncepty programování vytvořením digitální Magic 8 Ball pomocí micro:bitu a MakeCode. V týmech navrhují program, který využívá senzory a náhodná čísla k generování odpovědí při zatřesení zařízení. Tato zábavná, praktická aktivita podporuje týmovou práci, seznamuje s mechatronikou a rozvíjí programátorské a řešitelské dovednosti.</t>
   </si>
   <si>
     <t>Magic 8 Ball-aktivitet</t>
   </si>
   <si>
-    <t>Eleverne udforsker grundlæggende programmeringskoncepter ved at skabe en digital Magic 8 Ball med micro:bit og MakeCode. I teams designer de et program, der bruger sensorer og tilfældige tal til at generere svar, når enheden rystes. Denne sjove, praktiske aktivitet styrker teamwork, introducerer mekatronik og udvikler kodnings- og problemløsningskompetencer.</t>
-  </si>
-  <si>
-    <t>Magic 8 ball Activiteit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Studenten verkennen basisprincipes van programmeren door een digitale Magic 8 Ball te maken met behulp van micro:bit en MakeCode. In teams ontwerpen ze een programma dat sensoren en willekeurige getallen gebruikt om antwoorden te genereren wanneer het apparaat wordt geschud. Deze leuke, praktische activiteit bevordert teamwork, introduceert mechatronica en ontwikkelt programmeer- en probleemoplossende vaardigheden. </t>
-  </si>
-  <si>
-    <t>Magic 8 Ball Activity</t>
-  </si>
-  <si>
-    <t>Students explore basic programming concepts by creating a digital Magic 8 Ball using micro:bit and MakeCode. In teams, they design a program that uses sensors and random numbers to generate answers when the device is shaken. This fun, hands-on activity builds teamwork, introduces mechatronics, and develops coding and problem-solving skills.</t>
+    <t>Uploaded 4 September 2025
+Eleverne udforsker grundlæggende programmeringskoncepter ved at skabe en digital Magic 8 Ball med micro:bit og MakeCode. I teams designer de et program, der bruger sensorer og tilfældige tal til at generere svar, når enheden rystes. Denne sjove, praktiske aktivitet styrker teamwork, introducerer mekatronik og udvikler kodnings- og problemløsningskompetencer.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magic 8 ball Activiteit </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uploaded 4 September 2025
+Studenten verkennen basisprincipes van programmeren door een digitale Magic 8 Ball te maken met behulp van micro:bit en MakeCode. In teams ontwerpen ze een programma dat sensoren en willekeurige getallen gebruikt om antwoorden te genereren wanneer het apparaat wordt geschud. Deze leuke, praktische activiteit bevordert teamwork, introduceert mechatronica en ontwikkelt programmeer- en probleemoplossende vaardigheden. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magic 8 Ball Activity </t>
+  </si>
+  <si>
+    <t>Uploaded 4 September 2025
+Students explore basic programming concepts by creating a digital Magic 8 Ball using micro:bit and MakeCode. In teams, they design a program that uses sensors and random numbers to generate answers when the device is shaken. This fun, hands-on activity builds teamwork, introduces mechatronics, and develops coding and problem-solving skills.</t>
   </si>
   <si>
     <t xml:space="preserve">Activité Boule magique numéro 8 
 </t>
   </si>
   <si>
-    <t>Les élèves explorent les concepts de base de la programmation en créant une Boule magique numéro 8 numérique avec micro:bit et MakeCode. En équipes, ils conçoivent un programme utilisant des capteurs et des nombres aléatoires pour générer des réponses lorsque l'appareil est secoué. Cette activité ludique et pratique favorise le travail d'équipe, introduit la mécatronique et développe des compétences en codage et en résolution de problèmes.</t>
+    <t>Uploaded 4 September 2025
+Les élèves explorent les concepts de base de la programmation en créant une Boule magique numéro 8 numérique avec micro:bit et MakeCode. En équipes, ils conçoivent un programme utilisant des capteurs et des nombres aléatoires pour générer des réponses lorsque l'appareil est secoué. Cette activité ludique et pratique favorise le travail d'équipe, introduit la mécatronique et développe des compétences en codage et en résolution de problèmes.</t>
   </si>
   <si>
     <t>Einen Magic 8 Ball programmieren</t>
   </si>
   <si>
-    <t>Die Schüler*innen erkunden grundlegende Programmierkonzepte, indem sie mit micro:bit und MakeCode einen digitalen Magic 8 Ball erstellen. In Teamarbeit entwerfen sie ein Programm, das mithilfe von Sensoren und Zufallszahlen Antworten generiert, wenn das Gerät geschüttelt wird. Diese unterhaltsame, praktische Aktivität fördert Team-, Programmier- und Problemlösungsfähigkeiten und führt in die Mechatronik ein.</t>
+    <t>Uploaded 4 September 2025
+Die Schüler*innen erkunden grundlegende Programmierkonzepte, indem sie mit micro:bit und MakeCode einen digitalen Magic 8 Ball erstellen. In Teamarbeit entwerfen sie ein Programm, das mithilfe von Sensoren und Zufallszahlen Antworten generiert, wenn das Gerät geschüttelt wird. Diese unterhaltsame, praktische Aktivität fördert Team-, Programmier- und Problemlösungsfähigkeiten und führt in die Mechatronik ein.</t>
   </si>
   <si>
     <t>Δραστηριότητα Magic 8 Ball</t>
   </si>
   <si>
-    <t>Οι μαθητές εξερευνούν βασικές έννοιες προγραμματισμού δημιουργώντας μία ψηφιακή Magic 8 Ball με χρήση micro:bit και MakeCode. Σε ομάδες, σχεδιάζουν ένα πρόγραμμα που χρησιμοποιεί αισθητήρες και τυχαίους αριθμούς για να παράγει απαντήσεις όταν η συσκευή ανακινείται. Αυτή η διασκεδαστική, πρακτική δραστηριότητα ενισχύει τη συνεργασία, εισάγει τη μεκατρονική και αναπτύσσει δεξιότητες προγραμματισμού και επίλυσης προβλημάτων.</t>
+    <t>Uploaded 4 September 2025
+Οι μαθητές εξερευνούν βασικές έννοιες προγραμματισμού δημιουργώντας μία ψηφιακή Magic 8 Ball με χρήση micro:bit και MakeCode. Σε ομάδες, σχεδιάζουν ένα πρόγραμμα που χρησιμοποιεί αισθητήρες και τυχαίους αριθμούς για να παράγει απαντήσεις όταν η συσκευή ανακινείται. Αυτή η διασκεδαστική, πρακτική δραστηριότητα ενισχύει τη συνεργασία, εισάγει τη μεκατρονική και αναπτύσσει δεξιότητες προγραμματισμού και επίλυσης προβλημάτων.</t>
   </si>
   <si>
     <t>Attività Magic 8 ball</t>
   </si>
   <si>
-    <t>Gli studenti esplorano i concetti base della programmazione creando una Magic 8 Ball digitale con micro:bit e MakeCode. In gruppi, progettano un programma che utilizza sensori e numeri casuali per generare risposte quando il dispositivo viene scosso. Questa attività divertente e pratica promuove il lavoro di squadra, introduce la meccatronica e sviluppa competenze di programmazione e problem-solving.</t>
+    <t>Uploaded 4 September 2025
+Gli studenti esplorano i concetti base della programmazione creando una Magic 8 Ball digitale con micro:bit e MakeCode. In gruppi, progettano un programma che utilizza sensori e numeri casuali per generare risposte quando il dispositivo viene scosso. Questa attività divertente e pratica promuove il lavoro di squadra, introduce la meccatronica e sviluppa competenze di programmazione e problem-solving.</t>
   </si>
   <si>
     <t>Magic 8 Ball aktivitāte</t>
   </si>
   <si>
-    <t xml:space="preserve">Skolēni izzina programmēšanas pamata koncepcijas, veidojot digitālu Magic 8 Ball, izmantojot micro:bit un MakeCode. Komandās viņi izstrādā programmu, kas izmanto sensorus un nejaušus skaitļus, lai radītu atbildes, kad ierīce tiek sakratīta. Šī jautrā un praktiskā aktivitāte veicina komandas darbu, iepazīstina ar mehatroniku un attīsta programmēšanas un problēmu risināšanas prasmes. </t>
+    <t xml:space="preserve">Uploaded 4 September 2025
+Skolēni izzina programmēšanas pamata koncepcijas, veidojot digitālu Magic 8 Ball, izmantojot micro:bit un MakeCode. Komandās viņi izstrādā programmu, kas izmanto sensorus un nejaušus skaitļus, lai radītu atbildes, kad ierīce tiek sakratīta. Šī jautrā un praktiskā aktivitāte veicina komandas darbu, iepazīstina ar mehatroniku un attīsta programmēšanas un problēmu risināšanas prasmes. </t>
   </si>
   <si>
     <t>Magiškojo rutulio veikla</t>
   </si>
   <si>
-    <t>mokiniai nagrinėja pagrindines programavimo sąvokas, kurdami skaitmeninį magiškąjį rutulį, naudodami „micro:bit“ ir „MakeCode“. Susibūrę į komandas, jie kuria programą, kuri, naudodama jutiklius ir atsitiktinius skaičius, generuoja atsakymus, kai prietaisas pakratomas. Šis smagus praktinis užsiėmimas skatina komandinį darbą, supažindina su mechatronika, lavina programavimo ir problemų sprendimo įgūdžius.</t>
+    <t>Uploaded 4 September 2025
+mokiniai nagrinėja pagrindines programavimo sąvokas, kurdami skaitmeninį magiškąjį rutulį, naudodami „micro:bit“ ir „MakeCode“. Susibūrę į komandas, jie kuria programą, kuri, naudodama jutiklius ir atsitiktinius skaičius, generuoja atsakymus, kai prietaisas pakratomas. Šis smagus praktinis užsiėmimas skatina komandinį darbą, supažindina su mechatronika, lavina programavimo ir problemų sprendimo įgūdžius.</t>
   </si>
   <si>
     <t>Attività Magic 8 Ball</t>
   </si>
   <si>
-    <t>L-istudenti jesploraw kunċetti bażiċi tal-ipprogrammar billi joħolqu Magic 8 Ball diġitali bl-użu ta' micro:bit u MakeCode. F'timijiet, jiddisinjaw programm li juża sensors u numri każwali biex jiġġeneraw tweġibiet meta l-apparat jitħawwad. Din l-attività divertenti u prattika tibni ħiliet ta’ xogħol f’tim, tintroduċi l-mekatronika u tiżviluppa ħiliet ta’ coding u ta’ soluzzjoni tal-problemi.</t>
+    <t>Uploaded 4 September 2025
+L-istudenti jesploraw kunċetti bażiċi tal-ipprogrammar billi joħolqu Magic 8 Ball diġitali bl-użu ta' micro:bit u MakeCode. F'timijiet, jiddisinjaw programm li juża sensors u numri każwali biex jiġġeneraw tweġibiet meta l-apparat jitħawwad. Din l-attività divertenti u prattika tibni ħiliet ta’ xogħol f’tim, tintroduċi l-mekatronika u tiżviluppa ħiliet ta’ coding u ta’ soluzzjoni tal-problemi.</t>
   </si>
   <si>
     <t>Aktywność Magic 8 Ball</t>
   </si>
   <si>
-    <t>Uczniowie poznają podstawowe pojęcia programowania, tworząc cyfrową Magic 8 Ball za pomocą micro:bit i MakeCode. W zespołach projektują program, który wykorzystuje czujniki i liczby losowe do generowania odpowiedzi, gdy urządzenie jest potrząsane. Ta zabawna, praktyczna aktywność rozwija pracę zespołową, wprowadza do mechatroniki oraz rozwija umiejętności programowania i rozwiązywania problemów.</t>
+    <r>
+      <rPr>
+        <rFont val="Aptos Narrow"/>
+        <color theme="1"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>Uploaded 4 September 2025
+Uczniowie poznają podstawowe</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Aptos Narrow"/>
+        <color theme="1"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t xml:space="preserve"> pojęcia programowania, tworząc cyfrową Magic 8 Ball za pomocą micro:bit i MakeCode. W zespołach projektują program, który wykorzystuje czujniki i liczby losowe do generowania odpowiedzi, gdy urządzenie jest potrząsane. Ta zabawna, praktyczna aktywność rozwija pracę zespołową, wprowadza do mechatroniki oraz rozwija umiejętności programowania i rozwiązywania problemów.</t>
+    </r>
   </si>
   <si>
     <t>Atividade Magic 8 Ball</t>
   </si>
   <si>
-    <t>Os alunos exploram conceitos básicos de programação criando uma Magic 8 Ball digital com micro:bit e MakeCode. Em equipes, projetam um programa que usa sensores e números aleatórios para gerar respostas quando o dispositivo é agitado. Esta atividade divertida e prática promove o trabalho em equipe, introduz a mecatrónica e desenvolve habilidades de programação e resolução de problemas.</t>
+    <t>Uploaded 4 September 2025
+Os alunos exploram conceitos básicos de programação criando uma Magic 8 Ball digital com micro:bit e MakeCode. Em equipes, projetam um programa que usa sensores e números aleatórios para gerar respostas quando o dispositivo é agitado. Esta atividade divertida e prática promove o trabalho em equipe, introduz a mecatrónica e desenvolve habilidades de programação e resolução de problemas.</t>
   </si>
   <si>
     <t>Activitate Magic 8 Ball</t>
   </si>
   <si>
-    <t xml:space="preserve">Elevii explorează conceptele de bază ale programării, creând o Magic 8 Ball digitală folosind micro:bit și MakeCode. În echipe, proiectează un program care utilizează senzori și numere aleatorii pentru a genera răspunsuri atunci când dispozitivul este scuturat. Această activitate practică și distractivă dezvoltă munca în echipă, introduce mecatronica și dezvoltă abilități de programare și rezolvare de probleme. </t>
-  </si>
-  <si>
-    <t>Žiaci skúmajú základné koncepty programovania vytvorením digitálnej Magic 8 Ball pomocou micro:bitu a MakeCode. V tímoch navrhujú program, ktorý využíva senzory a náhodné čísla na generovanie odpovedí pri zatrasení zariadenia. Táto zábavná a praktická aktivita podporuje tímovú prácu, zoznamuje s mechatronikou a rozvíja programátorské a riešiteľské zručnosti.</t>
+    <t xml:space="preserve">Uploaded 4 September 2025
+Elevii explorează conceptele de bază ale programării, creând o Magic 8 Ball digitală folosind micro:bit și MakeCode. În echipe, proiectează un program care utilizează senzori și numere aleatorii pentru a genera răspunsuri atunci când dispozitivul este scuturat. Această activitate practică și distractivă dezvoltă munca în echipă, introduce mecatronica și dezvoltă abilități de programare și rezolvare de probleme. </t>
+  </si>
+  <si>
+    <t>Uploaded 4 September 2025
+Žiaci skúmajú základné koncepty programovania vytvorením digitálnej Magic 8 Ball pomocou micro:bitu a MakeCode. V tímoch navrhujú program, ktorý využíva senzory a náhodné čísla na generovanie odpovedí pri zatrasení zariadenia. Táto zábavná a praktická aktivita podporuje tímovú prácu, zoznamuje s mechatronikou a rozvíja programátorské a riešiteľské zručnosti.</t>
   </si>
   <si>
     <t>Aktivnost: Čarobna 8-krogla (Magic 8-ball)</t>
   </si>
   <si>
-    <t>Učenci raziskujejo osnovne koncepte programiranja z ustvarjanjem digitalne čarobne krogle številka 8 (Magic 8 Ball) z uporabo micro:bita in MakeCode. V skupinah načrtujejo program, ki uporablja senzorje in naključna števila za generiranje odgovorov, ko napravo pretresejo. Ta zabavna in praktična dejavnost spodbuja timsko delo, uvaja mehatroniko in razvija veščine programiranja ter reševanja problemov.</t>
+    <t>Uploaded 4 September 2025
+Učenci raziskujejo osnovne koncepte programiranja z ustvarjanjem digitalne čarobne krogle številka 8 (Magic 8 Ball) z uporabo micro:bita in MakeCode. V skupinah načrtujejo program, ki uporablja senzorje in naključna števila za generiranje odgovorov, ko napravo pretresejo. Ta zabavna in praktična dejavnost spodbuja timsko delo, uvaja mehatroniko in razvija veščine programiranja ter reševanja problemov.</t>
   </si>
   <si>
     <t>Actividad de la Bola 8 Mágica</t>
   </si>
   <si>
-    <t>Los estudiantes exploran conceptos básicos de programación mediante la creación de una Magic 8 Ball digital utilizando micro:bit y MakeCode. En equipos, diseñan un programa que utiliza sensores y números aleatorios para generar respuestas cuando se agita el dispositivo. Esta actividad divertida y práctica fomenta el trabajo en equipo, introduce la mecatrónica y desarrolla habilidades de codificación y resolución de problemas.</t>
-  </si>
-  <si>
-    <t>Oppilaat tutkivat ohjelmoinnin peruskäsitteitä luomalla digitaalisen Magic 8 Ballin micro:bitin ja MakeCoden avulla. Ryhmissä he suunnittelevat ohjelman, joka käyttää antureita ja satunnaislukuja vastausten luomiseen, kun laitetta ravistetaan. Tämä hauska, käytännönläheinen toiminta rakentaa tiimityötä, esittelee mekatroniikkaa ja kehittää koodaus- ja ongelmanratkaisutaitoja.</t>
-  </si>
-  <si>
-    <t>Magic 8 boll Aktivitet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eleverna utforskar grundläggande programmeringskoncept genom att skapa en digital Magic 8 Ball med micro:bit och MakeCode. I team designar de ett program som använder sensorer och slumpmässiga tal för att generera svar när enheten skakas. Denna roliga och praktiska aktivitet bygger lagarbete, introducerar mekatronik och utvecklar färdigheter i programmering och problemlösning. </t>
-  </si>
-  <si>
-    <t>Magic 8 Ball Etkinliği</t>
-  </si>
-  <si>
-    <t>Öğrenciler, micro:bit ve MakeCode kullanarak dijital bir Magic 8 Ball oluşturarak temel programlama kavramlarını keşfederler. Takımlar halinde, cihaz sallandığında yanıtlar üretmek için sensörler ve rastgele sayılar kullanan bir program tasarlarlar. Bu eğlenceli ve uygulamalı etkinlik, takım çalışmasını geliştirir, mekatronik bilimini tanıtır ve kodlama ve problem çözme becerilerini geliştirir.</t>
+    <t>Uploaded 4 September 2025
+Los estudiantes exploran conceptos básicos de programación mediante la creación de una Magic 8 Ball digital utilizando micro:bit y MakeCode. En equipos, diseñan un programa que utiliza sensores y números aleatorios para generar respuestas cuando se agita el dispositivo. Esta actividad divertida y práctica fomenta el trabajo en equipo, introduce la mecatrónica y desarrolla habilidades de codificación y resolución de problemas.</t>
+  </si>
+  <si>
+    <t>Uploaded 4 September 2025
+Oppilaat tutkivat ohjelmoinnin peruskäsitteitä luomalla digitaalisen Magic 8 Ballin micro:bitin ja MakeCoden avulla. Ryhmissä he suunnittelevat ohjelman, joka käyttää antureita ja satunnaislukuja vastausten luomiseen, kun laitetta ravistetaan. Tämä hauska, käytännönläheinen toiminta rakentaa tiimityötä, esittelee mekatroniikkaa ja kehittää koodaus- ja ongelmanratkaisutaitoja.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magic 8 boll Aktivitet </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uploaded 4 September 2025
+Eleverna utforskar grundläggande programmeringskoncept genom att skapa en digital Magic 8 Ball med micro:bit och MakeCode. I team designar de ett program som använder sensorer och slumpmässiga tal för att generera svar när enheten skakas. Denna roliga och praktiska aktivitet bygger lagarbete, introducerar mekatronik och utvecklar färdigheter i programmering och problemlösning. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magic 8 Ball Etkinliği </t>
+  </si>
+  <si>
+    <t>Uploaded 4 September 2025
+Öğrenciler, micro:bit ve MakeCode kullanarak dijital bir Magic 8 Ball oluşturarak temel programlama kavramlarını keşfederler. Takımlar halinde, cihaz sallandığında yanıtlar üretmek için sensörler ve rastgele sayılar kullanan bir program tasarlarlar. Bu eğlenceli ve uygulamalı etkinlik, takım çalışmasını geliştirir, mekatronik bilimini tanıtır ve kodlama ve problem çözme becerilerini geliştirir.</t>
   </si>
   <si>
     <t>Активність з Magic 8 Ball</t>
   </si>
   <si>
-    <t>Учні досліджують базові концепції програмування, створюючи цифрову «Чарівну кулю передбачень» за допомогою micro:bit та MakeCode. Працюючи в командах, вони розробляють програму, яка використовує сенсори та випадкові числа для генерації відповідей, коли пристрій струшують. Ця весела практична активність сприяє командній роботі, знайомить із мехатронікою та розвиває навички кодування й розв’язання проблем.</t>
+    <t>Uploaded 4 September 2025
+Учні досліджують базові концепції програмування, створюючи цифрову «Чарівну кулю передбачень» за допомогою micro:bit та MakeCode. Працюючи в командах, вони розробляють програму, яка використовує сенсори та випадкові числа для генерації відповідей, коли пристрій струшують. Ця весела практична активність сприяє командній роботі, знайомить із мехатронікою та розвиває навички кодування й розв’язання проблем.</t>
   </si>
   <si>
     <t>Aktiviteti me micro:bit</t>
   </si>
   <si>
-    <t xml:space="preserve">Nxënësit zbulojnë micro:bit-in dhe mjedisin e tij të programimit, duke eksploruar sesi sensorët dhe kodi krijojnë përgjigje interaktive. Ata eksperimentojnë me kodimin me blloqe, Python ose JavaScript—një hyrje praktike ideale në kompjuterikën fizike dhe programimin kreativ. </t>
+    <t xml:space="preserve">Uploaded 4 September 2025
+Nxënësit zbulojnë micro:bit-in dhe mjedisin e tij të programimit, duke eksploruar sesi sensorët dhe kodi krijojnë përgjigje interaktive. Ata eksperimentojnë me kodimin me blloqe, Python ose JavaScript—një hyrje praktike ideale në kompjuterikën fizike dhe programimin kreativ. </t>
   </si>
   <si>
     <t>Дейност с micro:bit</t>
   </si>
   <si>
-    <t>Учениците откриват micro:bit и неговата среда за програмиране, като изследват как сензорите и кодът създават интерактивни отговори. Те експериментират с блоково програмиране, Python или JavaScript—идеално практическо въведение в хардуерното програмиране и креативното кодиране.</t>
+    <t>Uploaded 4 September 2025
+Учениците откриват micro:bit и неговата среда за програмиране, като изследват как сензорите и кодът създават интерактивни отговори. Те експериментират с блоково програмиране, Python или JavaScript—идеално практическо въведение в хардуерното програмиране и креативното кодиране.</t>
   </si>
   <si>
     <t>Aktivnosti s micro:bitom</t>
   </si>
   <si>
-    <t xml:space="preserve">Učenici otkrivaju micro:bit i njegovo programsko okruženje, istražujući kako senzori i kod stvaraju interaktivne odgovore. Eksperimentiraju s programiranjem pomoću blokova, Pythonom ili JavaScriptom. Aktivnost je praktičan uvod u fizičko računarstvo i kreativno programiranje. </t>
+    <t xml:space="preserve">Uploaded 4 September 2025
+Učenici otkrivaju micro:bit i njegovo programsko okruženje, istražujući kako senzori i kod stvaraju interaktivne odgovore. Eksperimentiraju s programiranjem pomoću blokova, Pythonom ili JavaScriptom. Aktivnost je praktičan uvod u fizičko računarstvo i kreativno programiranje. </t>
   </si>
   <si>
     <t>Aktivita s micro:bitem</t>
   </si>
   <si>
-    <t>Studenti objevují micro:bit a jeho programovací prostředí, zkoumají, jak senzory a kód vytvářejí interaktivní odezvy. Experimentují s blokovým programováním, Pythonem nebo JavaScriptem—ideální praktický úvod do fyzického počítačového světa a kreativního programování.</t>
+    <t>Uploaded 4 September 2025
+Studenti objevují micro:bit a jeho programovací prostředí, zkoumají, jak senzory a kód vytvářejí interaktivní odezvy. Experimentují s blokovým programováním, Pythonem nebo JavaScriptem—ideální praktický úvod do fyzického počítačového světa a kreativního programování.</t>
   </si>
   <si>
     <t>micro:bit-aktivitet</t>
   </si>
   <si>
-    <t>Eleverne opdager micro:bit og dets programmeringsmiljø og udforsker, hvordan sensorer og kode skaber interaktive svar. De eksperimenterer med blokprogrammering, Python eller JavaScript—en ideel praktisk introduktion til fysisk computing og kreativ programmering.</t>
-  </si>
-  <si>
-    <t>micro:bit Activiteit</t>
-  </si>
-  <si>
-    <t>Studenten ontdekken de micro:bit en zijn programmeeromgeving en verkennen hoe sensoren en code interactieve reacties creëren. Ze experimenteren met blokprogrammeren, Python of JavaScript - een ideale praktische kennismaking met fysieke computing en creatief programmeren.</t>
-  </si>
-  <si>
-    <t>Activities with micro:bit</t>
-  </si>
-  <si>
-    <t>Students discover the micro:bit and its coding environment, exploring how sensors and code create interactive responses. They experiment with block coding, Python, or JavaScript - an ideal hands-on introduction to physical computing and creative programming.</t>
+    <t>Uploaded 4 September 2025
+Eleverne opdager micro:bit og dets programmeringsmiljø og udforsker, hvordan sensorer og kode skaber interaktive svar. De eksperimenterer med blokprogrammering, Python eller JavaScript—en ideel praktisk introduktion til fysisk computing og kreativ programmering.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">micro:bit Activiteit </t>
+  </si>
+  <si>
+    <t>Uploaded 4 September 2025
+Studenten ontdekken de micro:bit en zijn programmeeromgeving en verkennen hoe sensoren en code interactieve reacties creëren. Ze experimenteren met blokprogrammeren, Python of JavaScript - een ideale praktische kennismaking met fysieke computing en creatief programmeren.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Activities with micro:bit </t>
+  </si>
+  <si>
+    <t>Uploaded 4 September 2025
+Students discover the micro:bit and its coding environment, exploring how sensors and code create interactive responses. They experiment with block coding, Python, or JavaScript - an ideal hands-on introduction to physical computing and creative programming.</t>
   </si>
   <si>
     <t>Activité micro:bit</t>
   </si>
   <si>
-    <t xml:space="preserve">Les élèves découvrent le micro:bit et son environnement de programmation, explorant comment capteurs et code créent des réponses interactives. Ils expérimentent la programmation par blocs, en Python ou en JavaScript—une introduction pratique idéale à l’informatique physique et à la programmation créative. </t>
+    <t xml:space="preserve">Uploaded 4 September 2025
+Les élèves découvrent le micro:bit et son environnement de programmation, explorant comment capteurs et code créent des réponses interactives. Ils expérimentent la programmation par blocs, en Python ou en JavaScript—une introduction pratique idéale à l’informatique physique et à la programmation créative. </t>
   </si>
   <si>
     <t>micro:bit-Aktivität</t>
   </si>
   <si>
-    <t>Die Schüler*innen lernen den micro:bit und seine Programmierumgebung kennen und erforschen, wie Sensoren und Code interaktive Reaktionen erzeugen. Sie experimentieren mit visueller Programmierung, Python oder JavaScript – ein idealer Einstieg in Physical Computing und kreatives Programmieren.</t>
+    <t>Uploaded 4 September 2025
+Die Schüler*innen lernen den micro:bit und seine Programmierumgebung kennen und erforschen, wie Sensoren und Code interaktive Reaktionen erzeugen. Sie experimentieren mit visueller Programmierung, Python oder JavaScript – ein idealer Einstieg in Physical Computing und kreatives Programmieren.</t>
   </si>
   <si>
     <t>Δραστηριότητα με micro:bit</t>
   </si>
   <si>
-    <t>Οι μαθητές ανακαλύπτουν το micro:bit και το περιβάλλον προγραμματισμού του, εξερευνώντας πώς οι αισθητήρες και ο κώδικας δημιουργούν διαδραστικές αποκρίσεις. Πειραματίζονται με προγραμματισμό με μπλοκ, Python ή JavaScript—μια ιδανική πρακτική εισαγωγή στη φυσική πληροφορική και τον δημιουργικό προγραμματισμό.</t>
+    <t>Uploaded 4 September 2025
+Οι μαθητές ανακαλύπτουν το micro:bit και το περιβάλλον προγραμματισμού του, εξερευνώντας πώς οι αισθητήρες και ο κώδικας δημιουργούν διαδραστικές αποκρίσεις. Πειραματίζονται με προγραμματισμό με μπλοκ, Python ή JavaScript—μια ιδανική πρακτική εισαγωγή στη φυσική πληροφορική και τον δημιουργικό προγραμματισμό.</t>
   </si>
   <si>
     <t>Attività con micro:bit</t>
   </si>
   <si>
-    <t xml:space="preserve">Gli studenti e le studentesse scoprono micro:bit e il suo ambiente di programmazione, esplorando come i sensori e il codice creano risposte interattive. Sperimentano con la programmazione a blocchi, in Python o JavaScript - un'introduzione pratica ideale al physical computing e alla programmazione creativa. </t>
+    <t xml:space="preserve">Uploaded 4 September 2025
+Gli studenti e le studentesse scoprono micro:bit e il suo ambiente di programmazione, esplorando come i sensori e il codice creano risposte interattive. Sperimentano con la programmazione a blocchi, in Python o JavaScript - un'introduzione pratica ideale al physical computing e alla programmazione creativa. </t>
   </si>
   <si>
     <t>micro:bit aktivitāte</t>
   </si>
   <si>
-    <t>Skolēni iepazīst micro:bit un tā programmēšanas vidi, pētot, kā sensori un kods rada interaktīvas atbildes. Viņi eksperimentē ar bloku programmēšanu, Python vai JavaScript—ideāls praktisks ievads fiziskajā datorikā un radošajā programmēšanā.</t>
+    <t>Uploaded 4 September 2025
+Skolēni iepazīst micro:bit un tā programmēšanas vidi, pētot, kā sensori un kods rada interaktīvas atbildes. Viņi eksperimentē ar bloku programmēšanu, Python vai JavaScript—ideāls praktisks ievads fiziskajā datorikā un radošajā programmēšanā.</t>
   </si>
   <si>
     <t>„micro:bit“ veikla</t>
   </si>
   <si>
-    <t>Mokiniai susipažįsta su „micro:bit“ ir jo programavimo aplinka, tyrinėja, kaip jutikliai ir kodas kuria interaktyvius atsakus. Jie eksperimentuoja su blokine programavimo kalba, „Python“ arba „JavaScript“ – tai ideali praktinė įžanga į fizinę kompiuteriją ir kūrybišką programavimą.</t>
+    <t>Uploaded 4 September 2025
+Mokiniai susipažįsta su „micro:bit“ ir jo programavimo aplinka, tyrinėja, kaip jutikliai ir kodas kuria interaktyvius atsakus. Jie eksperimentuoja su blokine programavimo kalba, „Python“ arba „JavaScript“ – tai ideali praktinė įžanga į fizinę kompiuteriją ir kūrybišką programavimą.</t>
   </si>
   <si>
     <t>Attività micro:bit</t>
   </si>
   <si>
-    <t>L-istudenti jsibu l-micro:bit u l-ambjent tal-ipprogrammar tiegħu, jesploraw kif is-sensers u l-code joħolqu risposti interattivi. Jippruvaw programmar bil-blokki, Python jew JavaScript—introduzzjoni prattika ideali għall-computing fiżiku u l-ipprogrammar kreattiv.</t>
+    <t>Uploaded 4 September 2025
+L-istudenti jsibu l-micro:bit u l-ambjent tal-ipprogrammar tiegħu, jesploraw kif is-sensers u l-code joħolqu risposti interattivi. Jippruvaw programmar bil-blokki, Python jew JavaScript—introduzzjoni prattika ideali għall-computing fiżiku u l-ipprogrammar kreattiv.</t>
   </si>
   <si>
     <t>Aktywność z micro:bitem</t>
   </si>
   <si>
-    <t>Uczniowie poznają micro:bit i jego środowisko programistyczne, badając, jak czujniki i kod tworzą interaktywne odpowiedzi. Eksperymentują z programowaniem blokowym, Pythonem lub JavaScriptem—idealny praktyczny wstęp do informatyki fizycznej i kreatywnego programowania.</t>
+    <t>Uploaded 4 September 2025
+Uczniowie poznają micro:bit i jego środowisko programistyczne, badając, jak czujniki i kod tworzą interaktywne odpowiedzi. Eksperymentują z programowaniem blokowym, Pythonem lub JavaScriptem—idealny praktyczny wstęp do informatyki fizycznej i kreatywnego programowania.</t>
   </si>
   <si>
     <t>Atividade com micro:bit</t>
   </si>
   <si>
-    <t>Os alunos descobrem o micro:bit e o seu ambiente de programação, explorando como sensores e código criam respostas interativas. Experimentam programação em blocos, Python ou JavaScript—uma introdução prática ideal à computação física e à programação criativa.</t>
+    <t>Uploaded 4 September 2025
+Os alunos descobrem o micro:bit e o seu ambiente de programação, explorando como sensores e código criam respostas interativas. Experimentam programação em blocos, Python ou JavaScript—uma introdução prática ideal à computação física e à programação criativa.</t>
   </si>
   <si>
     <t>Activitate cu micro:bit</t>
   </si>
   <si>
-    <t>Elevii descoperă micro:bit-ul și mediul său de programare, explorând cum senzorii și codul creează răspunsuri interactive. Ei experimentează cu programarea pe blocuri, în Python sau JavaScript—o introducere practică ideală în informatica fizică și programarea creativă.</t>
+    <t>Uploaded 4 September 2025
+Elevii descoperă micro:bit-ul și mediul său de programare, explorând cum senzorii și codul creează răspunsuri interactive. Ei experimentează cu programarea pe blocuri, în Python sau JavaScript—o introducere practică ideală în informatica fizică și programarea creativă.</t>
   </si>
   <si>
     <t>Aktivita s micro:bitom</t>
   </si>
   <si>
-    <t>Žiaci objavujú micro:bit a jeho programovacie prostredie, skúmajú, ako senzory a kód vytvárajú interaktívne odozvy. Experimentujú s blokovým programovaním, Pythonom alebo JavaScriptom—ideálny praktický úvod do fyzického počítačového sveta a kreatívneho programovania.</t>
+    <t>Uploaded 4 September 2025
+Žiaci objavujú micro:bit a jeho programovacie prostredie, skúmajú, ako senzory a kód vytvárajú interaktívne odozvy. Experimentujú s blokovým programovaním, Pythonom alebo JavaScriptom—ideálny praktický úvod do fyzického počítačového sveta a kreatívneho programovania.</t>
   </si>
   <si>
     <t>Aktivnosti z micro:bitom</t>
   </si>
   <si>
-    <t>Učenci spoznajo micro:bit in njegovo programsko okolje ter raziskujejo, kako senzorji in koda ustvarjajo interaktivne odzive. Preizkušajo blokovno programiranje, Python ali JavaScript. Aktivnost je odličen praktičen uvod v fizično računalništvo in ustvarjalno programiranje.</t>
+    <t>Uploaded 4 September 2025
+Učenci spoznajo micro:bit in njegovo programsko okolje ter raziskujejo, kako senzorji in koda ustvarjajo interaktivne odzive. Preizkušajo blokovno programiranje, Python ali JavaScript. Aktivnost je odličen praktičen uvod v fizično računalništvo in ustvarjalno programiranje.</t>
   </si>
   <si>
     <t>Actividad con micro:bit</t>
   </si>
   <si>
-    <t>Los estudiantes descubren el micro:bit y su entorno de programación, explorando cómo los sensores y el código crean respuestas interactivas. Experimentan con programación por bloques, Python o JavaScript—una introducción práctica ideal a la informática física y a la programación creativa.</t>
+    <t>Uploaded 4 September 2025
+Los estudiantes descubren el micro:bit y su entorno de programación, explorando cómo los sensores y el código crean respuestas interactivas. Experimentan con programación por bloques, Python o JavaScript—una introducción práctica ideal a la informática física y a la programación creativa.</t>
   </si>
   <si>
     <t>micro:bit-harjoitus</t>
   </si>
   <si>
-    <t xml:space="preserve">Oppilaat tutustuvat micro:bit-laitteeseen ja sen ohjelmointiympäristöön, tutkien kuinka sensorit ja koodi luovat interaktiivisia vastauksia. He kokeilevat lohko-ohjelmointia, Pythonia tai JavaScriptiä—ihanteellinen käytännön johdanto fyysiseen tietojenkäsittelyyn ja luovaan ohjelmointiin. </t>
-  </si>
-  <si>
-    <t>Eleverna upptäcker micro:bit och dess programmeringsmiljö, och utforskar hur sensorer och kod skapar interaktiva svar. De experimenterar med blockprogrammering, Python eller JavaScript—en idealisk praktisk introduktion till fysisk datoranvändning och kreativ programmering.</t>
+    <t xml:space="preserve">Uploaded 4 September 2025
+Oppilaat tutustuvat micro:bit-laitteeseen ja sen ohjelmointiympäristöön, tutkien kuinka sensorit ja koodi luovat interaktiivisia vastauksia. He kokeilevat lohko-ohjelmointia, Pythonia tai JavaScriptiä—ihanteellinen käytännön johdanto fyysiseen tietojenkäsittelyyn ja luovaan ohjelmointiin. </t>
+  </si>
+  <si>
+    <t>Uploaded 4 September 2025
+Eleverna upptäcker micro:bit och dess programmeringsmiljö, och utforskar hur sensorer och kod skapar interaktiva svar. De experimenterar med blockprogrammering, Python eller JavaScript—en idealisk praktisk introduktion till fysisk datoranvändning och kreativ programmering.</t>
   </si>
   <si>
     <t>Micro:bit Etkinlik Açıklaması:</t>
   </si>
   <si>
-    <t>Öğrenciler, micro:bit'i ve kodlama ortamını keşfederek sensörlerin ve kodun etkileşimli tepkiler nasıl oluşturduğunu incelerler. Blok kodlama, Python veya JavaScript ile deneyler yaparlar; bu, fiziksel hesaplama ve yaratıcı programlamaya ideal bir uygulamalı giriştir.</t>
+    <t>Uploaded 4 September 2025
+Öğrenciler, micro:bit'i ve kodlama ortamını keşfederek sensörlerin ve kodun etkileşimli tepkiler nasıl oluşturduğunu incelerler. Blok kodlama, Python veya JavaScript ile deneyler yaparlar; bu, fiziksel hesaplama ve yaratıcı programlamaya ideal bir uygulamalı giriştir.</t>
   </si>
   <si>
     <t>Активність із micro:bit</t>
   </si>
   <si>
-    <t>Учні знайомляться з micro:bit та середовищем для програмування, досліджуючи, як датчики та код створюють інтерактивні реакції. Вони експериментують із блочним програмуванням, Python або JavaScript — це ідеальне практичне введення у фізичні обчислення та креативне програмування.</t>
+    <t>Uploaded 4 September 2025
+Учні знайомляться з micro:bit та середовищем для програмування, досліджуючи, як датчики та код створюють інтерактивні реакції. Вони експериментують із блочним програмуванням, Python або JavaScript — це ідеальне практичне введення у фізичні обчислення та креативне програмування.</t>
   </si>
   <si>
     <t>Aktiviteti Python</t>
   </si>
   <si>
-    <t xml:space="preserve">Nxënësit krijojnë një kuiz për gratë në shkencë duke përdorur Python. Duke punuar në ekipe, ata ushtrojnë të menduarit algoritmik, përdorin input/output, deklarata if/else dhe variabla. Një mënyrë praktike për të ndërtuar aftësi në programim ndërsa promovojnë punën në grup dhe ndërgjegjësimin për modele frymëzuese. </t>
+    <t xml:space="preserve">Uploaded 4 September 2025
+Nxënësit krijojnë një kuiz për gratë në shkencë duke përdorur Python. Duke punuar në ekipe, ata ushtrojnë të menduarit algoritmik, përdorin input/output, deklarata if/else dhe variabla. Një mënyrë praktike për të ndërtuar aftësi në programim ndërsa promovojnë punën në grup dhe ndërgjegjësimin për modele frymëzuese. </t>
   </si>
   <si>
     <t>Дейност с Python</t>
   </si>
   <si>
-    <t>Учениците създават тест за жените в науката, използвайки Python. Работейки в екипи, те упражняват алгоритмично мислене, използват вход/изход, условни конструкции if/else и променливи. Практически начин за развитие на умения по програмиране, като същевременно се насърчава работата в екип и повишава осведомеността за вдъхновяващи ролеви модели.</t>
+    <t>Uploaded 4 September 2025
+Учениците създават тест за жените в науката, използвайки Python. Работейки в екипи, те упражняват алгоритмично мислене, използват вход/изход, условни конструкции if/else и променливи. Практически начин за развитие на умения по програмиране, като същевременно се насърчава работата в екип и повишава осведомеността за вдъхновяващи ролеви модели.</t>
   </si>
   <si>
     <t>Aktivnost u Pythonu</t>
   </si>
   <si>
-    <t>Učenici izrađuju kviz o ženama u znanosti koristeći Python. Radeći u timovima, vježbaju algoritamsko razmišljanje, koriste input/print, if/else naredbe i varijable. Aktivnost je praktična za razvoj programerskih vještina uz poticanje timskog rada i podizanja svijesti o inspirativnim uzorima.</t>
+    <t>Uploaded 4 September 2025
+Učenici izrađuju kviz o ženama u znanosti koristeći Python. Radeći u timovima, vježbaju algoritamsko razmišljanje, koriste input/print, if/else naredbe i varijable. Aktivnost je praktična za razvoj programerskih vještina uz poticanje timskog rada i podizanja svijesti o inspirativnim uzorima.</t>
   </si>
   <si>
     <t>Aktivita s Pythone</t>
   </si>
   <si>
-    <t>Studenti vytvářejí kvíz o ženách ve vědě pomocí Pythonu. Pracují v týmech, procvičují algoritmické myšlení, používají vstup/výstup, podmínky if/else a proměnné. Praktický způsob, jak rozvíjet programovací dovednosti a podporovat týmovou spolupráci a povědomí o inspirativních vzorech.</t>
+    <t>Uploaded 4 September 2025
+Studenti vytvářejí kvíz o ženách ve vědě pomocí Pythonu. Pracují v týmech, procvičují algoritmické myšlení, používají vstup/výstup, podmínky if/else a proměnné. Praktický způsob, jak rozvíjet programovací dovednosti a podporovat týmovou spolupráci a povědomí o inspirativních vzorech.</t>
   </si>
   <si>
     <t>Python-aktivitet</t>
   </si>
   <si>
-    <t>Eleverne laver en quiz om kvinder i videnskab ved hjælp af Python. De arbejder i teams, øver algoritmisk tænkning, bruger input/output, if/else-sætninger og variabler. En praktisk måde at udvikle programmeringsevner på, samtidig med at samarbejde og bevidsthed om inspirerende rollemodeller fremmes.</t>
+    <t>Uploaded 4 September 2025
+Eleverne laver en quiz om kvinder i videnskab ved hjælp af Python. De arbejder i teams, øver algoritmisk tænkning, bruger input/output, if/else-sætninger og variabler. En praktisk måde at udvikle programmeringsevner på, samtidig med at samarbejde og bevidsthed om inspirerende rollemodeller fremmes.</t>
   </si>
   <si>
     <t>Python-activiteit</t>
   </si>
   <si>
-    <t>Studenten maken een quiz over vrouwen in de wetenschap met behulp van Python. In teams oefenen ze algoritmisch denken, gebruiken ze input/output, if/else-structuren en variabelen. Een praktische manier om programmeervaardigheden op te bouwen, terwijl samenwerking en bewustzijn over inspirerende rolmodellen worden gestimuleerd.</t>
-  </si>
-  <si>
-    <t>Python Activity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Students create a quiz about women in science using Python. Working in teams, they practice algorithmic thinking, use input/output, if/else statements, and variables. A hands-on way to build coding skills while promoting teamwork and awareness of inspiring role models. </t>
+    <t>Uploaded 4 September 2025
+Studenten maken een quiz over vrouwen in de wetenschap met behulp van Python. In teams oefenen ze algoritmisch denken, gebruiken ze input/output, if/else-structuren en variabelen. Een praktische manier om programmeervaardigheden op te bouwen, terwijl samenwerking en bewustzijn over inspirerende rolmodellen worden gestimuleerd.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Python Activity </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uploaded 4 September 2025
+Students create a quiz about women in science using Python. Working in teams, they practice algorithmic thinking, use input/output, if/else statements, and variables. A hands-on way to build coding skills while promoting teamwork and awareness of inspiring role models. </t>
   </si>
   <si>
     <t>Activité Python</t>
   </si>
   <si>
-    <t>Les élèves créent un quiz sur les femmes dans la science en utilisant Python. En équipes, ils pratiquent la pensée algorithmique, utilisent les entrées/sorties, les instructions si/sinon et les variables. Une approche pratique pour développer des compétences en programmation tout en encourageant le travail d'équipe et la sensibilisation à des modèles inspirants.</t>
+    <t>Uploaded 4 September 2025
+Les élèves créent un quiz sur les femmes dans la science en utilisant Python. En équipes, ils pratiquent la pensée algorithmique, utilisent les entrées/sorties, les instructions si/sinon et les variables. Une approche pratique pour développer des compétences en programmation tout en encourageant le travail d'équipe et la sensibilisation à des modèles inspirants.</t>
   </si>
   <si>
     <t>Aktivität: Mit Python ein Quiz programmieren</t>
   </si>
   <si>
-    <t>Die Schüler*innen erstellen mit Python ein Quiz über Frauen in der Wissenschaft. In Teamarbeit üben sie algorithmisches Denken, nutzen Ein-/Ausgabe, if-else-Anweisungen und Variablen. Diese praxisnahe Aktivität baut Programmierfähigkeiten auf, fördert Teamarbeit und schärft das Bewusstsein für inspirierende Vorbilder.</t>
+    <t>Uploaded 4 September 2025
+Die Schüler*innen erstellen mit Python ein Quiz über Frauen in der Wissenschaft. In Teamarbeit üben sie algorithmisches Denken, nutzen Ein-/Ausgabe, if-else-Anweisungen und Variablen. Diese praxisnahe Aktivität baut Programmierfähigkeiten auf, fördert Teamarbeit und schärft das Bewusstsein für inspirierende Vorbilder.</t>
   </si>
   <si>
     <t>Δραστηριότητα με Python</t>
   </si>
   <si>
-    <t>Οι μαθητές δημιουργούν ένα κουίζ για τις γυναίκες στην επιστήμη χρησιμοποιώντας Python. Εργαζόμενοι σε ομάδες, εξασκούν αλγοριθμική σκέψη, χρησιμοποιούν είσοδο/έξοδο, εντολές if/else και μεταβλητές. Ένας πρακτικός τρόπος για την ανάπτυξη δεξιοτήτων προγραμματισμού, ενώ παράλληλα ενισχύεται η ομαδική εργασία και η ευαισθητοποίηση για εμπνευσμένα πρότυπα.</t>
+    <t>Uploaded 4 September 2025
+Οι μαθητές δημιουργούν ένα κουίζ για τις γυναίκες στην επιστήμη χρησιμοποιώντας Python. Εργαζόμενοι σε ομάδες, εξασκούν αλγοριθμική σκέψη, χρησιμοποιούν είσοδο/έξοδο, εντολές if/else και μεταβλητές. Ένας πρακτικός τρόπος για την ανάπτυξη δεξιοτήτων προγραμματισμού, ενώ παράλληλα ενισχύεται η ομαδική εργασία και η ευαισθητοποίηση για εμπνευσμένα πρότυπα.</t>
   </si>
   <si>
     <t>Attività con Python</t>
   </si>
   <si>
-    <t>Gli studenti e le studentesse creano un quiz sulle donne nella scienza usando Python. Lavorando in gruppo, esercitano il pensiero algoritmico, utilizzano input/output, istruzioni if/then e variabili. Un approccio pratico per sviluppare competenze di programmazione, promuovere il lavoro di squadra e aumentare la consapevolezza di modelli ispiratori.</t>
+    <t>Uploaded 4 September 2025
+Gli studenti e le studentesse creano un quiz sulle donne nella scienza usando Python. Lavorando in gruppo, esercitano il pensiero algoritmico, utilizzano input/output, istruzioni if/then e variabili. Un approccio pratico per sviluppare competenze di programmazione, promuovere il lavoro di squadra e aumentare la consapevolezza di modelli ispiratori.</t>
   </si>
   <si>
     <t xml:space="preserve">Python aktivitāte 
 </t>
   </si>
   <si>
-    <t>Skolēni izveido viktorīnu par sievietēm zinātnē, izmantojot Python. Darbojoties komandās, viņi trenē algoritmisko domāšanu, izmanto ievadi/izvadi, if/else nosacījumus un mainīgos. Praktisks veids, kā attīstīt programmēšanas prasmes, vienlaikus veicinot sadarbību un izpratni par iedvesmojošām personībām.</t>
-  </si>
-  <si>
-    <t>„Python“ veikla</t>
-  </si>
-  <si>
-    <t>mokiniai, taikydami „Python“, sukuria testą apie moteris moksle. Dirbdami komandose jie lavina algoritminį mąstymą, taiko įvesties ir išvesties, „if-else“ sakinius ir kintamuosius. Tai patogus būdas ugdyti programavimo įgūdžius, kartu skatinant komandinį darbą ir supažindinant su įkvepiančiais pavyzdžiais.</t>
+    <t>Uploaded 4 September 2025
+Skolēni izveido viktorīnu par sievietēm zinātnē, izmantojot Python. Darbojoties komandās, viņi trenē algoritmisko domāšanu, izmanto ievadi/izvadi, if/else nosacījumus un mainīgos. Praktisks veids, kā attīstīt programmēšanas prasmes, vienlaikus veicinot sadarbību un izpratni par iedvesmojošām personībām.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">„Python“ veikla </t>
+  </si>
+  <si>
+    <t>Uploaded 4 September 2025
+mokiniai, taikydami „Python“, sukuria testą apie moteris moksle. Dirbdami komandose jie lavina algoritminį mąstymą, taiko įvesties ir išvesties, „if-else“ sakinius ir kintamuosius. Tai patogus būdas ugdyti programavimo įgūdžius, kartu skatinant komandinį darbą ir supažindinant su įkvepiančiais pavyzdžiais.</t>
   </si>
   <si>
     <t>Attività Python</t>
   </si>
   <si>
-    <t>L-istudenti joħolqu kwizz dwar in-nisa fix-xjenza bl-użu ta' Python. Jaħdmu fi gruppi, jipprattikaw ħsieb algoritmiku, jużaw input/output, statements if/else u varjabbli. Mod prattiku biex jibnu ħiliet fil-coding filwaqt li jippromwovu xogħol f’tim u għarfien ta’ mudelli ta’ ispirazzjoni.</t>
+    <t>Uploaded 4 September 2025
+L-istudenti joħolqu kwizz dwar in-nisa fix-xjenza bl-użu ta' Python. Jaħdmu fi gruppi, jipprattikaw ħsieb algoritmiku, jużaw input/output, statements if/else u varjabbli. Mod prattiku biex jibnu ħiliet fil-coding filwaqt li jippromwovu xogħol f’tim u għarfien ta’ mudelli ta’ ispirazzjoni.</t>
   </si>
   <si>
     <t>Aktywność z Pythonem</t>
   </si>
   <si>
-    <t>Uczniowie tworzą quiz o kobietach w nauce, używając Pythona. Pracując w zespołach, ćwiczą myślenie algorytmiczne, korzystają z wejścia/wyjścia, instrukcji if/else i zmiennych. Praktyczny sposób na rozwijanie umiejętności programowania, promowanie pracy zespołowej i budowanie świadomości o inspirujących wzorcach.</t>
+    <t>Uploaded 4 September 2025
+Uczniowie tworzą quiz o kobietach w nauce, używając Pythona. Pracując w zespołach, ćwiczą myślenie algorytmiczne, korzystają z wejścia/wyjścia, instrukcji if/else i zmiennych. Praktyczny sposób na rozwijanie umiejętności programowania, promowanie pracy zespołowej i budowanie świadomości o inspirujących wzorcach.</t>
   </si>
   <si>
     <t>Atividade com Python</t>
   </si>
   <si>
-    <t>Os alunos criam um quiz sobre mulheres na ciência usando Python. Trabalhando em equipes, praticam o pensamento algorítmico, usam entrada/saída, instruções if/else e variáveis. Uma abordagem prática para desenvolver habilidades de programação enquanto promovem o trabalho em equipe e a conscientização sobre modelos inspiradores.</t>
+    <t>Uploaded 4 September 2025
+Os alunos criam um quiz sobre mulheres na ciência usando Python. Trabalhando em equipes, praticam o pensamento algorítmico, usam entrada/saída, instruções if/else e variáveis. Uma abordagem prática para desenvolver habilidades de programação enquanto promovem o trabalho em equipe e a conscientização sobre modelos inspiradores.</t>
   </si>
   <si>
     <t xml:space="preserve">Activitate cu Python 
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Elevii creează un quiz despre femeile în știință folosind Python. Lucrând în echipe, exersează gândirea algoritmică, folosesc input/output, instrucțiuni if/else și variabile. O modalitate practică de a dezvolta abilități de programare, promovând totodată munca în echipă și conștientizarea modelelor inspiraționale. </t>
+    <t xml:space="preserve">Uploaded 4 September 2025
+Elevii creează un quiz despre femeile în știință folosind Python. Lucrând în echipe, exersează gândirea algoritmică, folosesc input/output, instrucțiuni if/else și variabile. O modalitate practică de a dezvolta abilități de programare, promovând totodată munca în echipă și conștientizarea modelelor inspiraționale. </t>
   </si>
   <si>
     <t>Aktivita s Pythonom</t>
   </si>
   <si>
-    <t>Žiaci vytvoria kvíz o ženách vo vede pomocou Pythonu. Pracujú v tímoch, precvičujú algoritmické myslenie, používajú vstup/výstup, príkazy if/else a premenné. Praktický spôsob, ako rozvíjať programátorské zručnosti, podporovať tímovú prácu a zvýšiť povedomie o inšpiratívnych vzoroch.</t>
+    <t>Uploaded 4 September 2025
+Žiaci vytvoria kvíz o ženách vo vede pomocou Pythonu. Pracujú v tímoch, precvičujú algoritmické myslenie, používajú vstup/výstup, príkazy if/else a premenné. Praktický spôsob, ako rozvíjať programátorské zručnosti, podporovať tímovú prácu a zvýšiť povedomie o inšpiratívnych vzoroch.</t>
   </si>
   <si>
     <t>Aktivnost v Pythonu</t>
   </si>
   <si>
-    <t>Učenci ustvarijo kviz o ženskah v znanosti z uporabo Pythona. V skupinah vadijo algoritmično razmišljanje, uporabljajo vnos/iznos, if/else stavke in spremenljivke. Praktičen način za razvoj programerskih veščin ter spodbujanje timskega dela in ozaveščanja o navdihujočih vzorih.</t>
+    <t>Uploaded 4 September 2025
+Učenci ustvarijo kviz o ženskah v znanosti z uporabo Pythona. V skupinah vadijo algoritmično razmišljanje, uporabljajo vnos/iznos, if/else stavke in spremenljivke. Praktičen način za razvoj programerskih veščin ter spodbujanje timskega dela in ozaveščanja o navdihujočih vzorih.</t>
   </si>
   <si>
     <t>Actividad con Python</t>
   </si>
   <si>
-    <t xml:space="preserve">Los estudiantes crean un quiz sobre mujeres en la ciencia usando Python. Trabajando en equipos, practican el pensamiento algorítmico, usan entrada/salida, sentencias if/else y variables. Una forma práctica de desarrollar habilidades de programación mientras se fomenta el trabajo en equipo y la concienciación sobre modelos a seguir inspiradores. </t>
+    <t xml:space="preserve">Uploaded 4 September 2025
+Los estudiantes crean un quiz sobre mujeres en la ciencia usando Python. Trabajando en equipos, practican el pensamiento algorítmico, usan entrada/salida, sentencias if/else y variables. Una forma práctica de desarrollar habilidades de programación mientras se fomenta el trabajo en equipo y la concienciación sobre modelos a seguir inspiradores. </t>
   </si>
   <si>
     <t>Python-harjoitus</t>
   </si>
   <si>
-    <t xml:space="preserve">Oppilaat tekevät tietovisan naisista tieteessä Pythonin avulla. Ryhmissä he harjoittelevat algoritmista ajattelua, käyttävät syötettä/tulostetta, if/else-lauseita ja muuttujia. Käytännöllinen tapa kehittää ohjelmointitaitoja ja edistää tiimityötä sekä tietoisuutta inspiroivista roolimalleista. </t>
-  </si>
-  <si>
-    <t>Eleverna skapar en quiz om kvinnor inom vetenskap med Python. I team tränar de algoritmiskt tänkande, använder input/output, if/else-satser och variabler. Ett praktiskt sätt att utveckla programmeringskunskaper och samtidigt främja lagarbete och medvetenhet om inspirerande förebilder.</t>
+    <t xml:space="preserve">Uploaded 4 September 2025
+Oppilaat tekevät tietovisan naisista tieteessä Pythonin avulla. Ryhmissä he harjoittelevat algoritmista ajattelua, käyttävät syötettä/tulostetta, if/else-lauseita ja muuttujia. Käytännöllinen tapa kehittää ohjelmointitaitoja ja edistää tiimityötä sekä tietoisuutta inspiroivista roolimalleista. </t>
+  </si>
+  <si>
+    <t>Uploaded 4 September 2025
+Eleverna skapar en quiz om kvinnor inom vetenskap med Python. I team tränar de algoritmiskt tänkande, använder input/output, if/else-satser och variabler. Ett praktiskt sätt att utveckla programmeringskunskaper och samtidigt främja lagarbete och medvetenhet om inspirerande förebilder.</t>
   </si>
   <si>
     <t>Python Etkinliği</t>
   </si>
   <si>
-    <t>Öğrenciler, Python kullanarak bilim dünyasındaki kadınlar hakkında bir sınav hazırlarlar. Takımlar halinde çalışarak algoritmik düşünmeyi, girdi/çıktı, if/else ifadeleri ve değişkenleri kullanmayı öğrenirler. Bu, ekip çalışmasını ve ilham verici rol modellerin farkındalığını teşvik ederken kodlama becerilerini geliştirmenin uygulamalı bir yoludur.</t>
+    <t>Uploaded 4 September 2025
+Öğrenciler, Python kullanarak bilim dünyasındaki kadınlar hakkında bir sınav hazırlarlar. Takımlar halinde çalışarak algoritmik düşünmeyi, girdi/çıktı, if/else ifadeleri ve değişkenleri kullanmayı öğrenirler. Bu, ekip çalışmasını ve ilham verici rol modellerin farkındalığını teşvik ederken kodlama becerilerini geliştirmenin uygulamalı bir yoludur.</t>
   </si>
   <si>
     <t>Активність із Python</t>
   </si>
   <si>
-    <t>Учні створюють вікторину про жінок у науці, використовуючи Python. Працюючи в командах, вони практикують алгоритмічне мислення, використовують введення/виведення даних, умовні оператори if/else та змінні. Це практичний спосіб розвивати навички програмування, водночас сприяючи командній роботі й підвищенню обізнаності про надихаючі приклади рольових моделей.</t>
+    <t>Uploaded 4 September 2025
+Учні створюють вікторину про жінок у науці, використовуючи Python. Працюючи в командах, вони практикують алгоритмічне мислення, використовують введення/виведення даних, умовні оператори if/else та змінні. Це практичний спосіб розвивати навички програмування, водночас сприяючи командній роботі й підвищенню обізнаності про надихаючі приклади рольових моделей.</t>
   </si>
   <si>
     <t>Aktiviteti me Scratch</t>
   </si>
   <si>
-    <t>Në këtë aktivitet, nxënësit krijojnë një histori interaktive për një grua në shkencë duke përdorur Scratch. Duke punuar në ekipe, ata eksplorojnë të menduarit algoritmik, dialogun dhe animacionin ndërsa hulumtojnë figura frymëzuese. Një mënyrë kreative dhe e qasshme për të ndërthurur programimin, tregimin dhe shkathtësitë digjitale.</t>
+    <t>Uploaded 4 September 2025
+Në këtë aktivitet, nxënësit krijojnë një histori interaktive për një grua në shkencë duke përdorur Scratch. Duke punuar në ekipe, ata eksplorojnë të menduarit algoritmik, dialogun dhe animacionin ndërsa hulumtojnë figura frymëzuese. Një mënyrë kreative dhe e qasshme për të ndërthurur programimin, tregimin dhe shkathtësitë digjitale.</t>
   </si>
   <si>
     <t>Дейност със Scratch</t>
   </si>
   <si>
-    <t>В тази дейност учениците създават интерактивна история за жена в науката, използвайки Scratch. Работейки в екипи, те изследват алгоритмичното мислене, диалога и анимацията, докато проучват вдъхновяващи личности. Креативен и достъпен начин да се комбинират програмиране, разказване на истории и дигитална грамотност.</t>
+    <t>Uploaded 4 September 2025
+В тази дейност учениците създават интерактивна история за жена в науката, използвайки Scratch. Работейки в екипи, те изследват алгоритмичното мислене, диалога и анимацията, докато проучват вдъхновяващи личности. Креативен и достъпен начин да се комбинират програмиране, разказване на истории и дигитална грамотност.</t>
   </si>
   <si>
     <t>Aktivnost u Scratchu</t>
   </si>
   <si>
-    <t xml:space="preserve">U ovoj aktivnosti učenici stvaraju interaktivnu priču o odabranoj znanstvenici koristeći Scratch. Radeći u timovima, istražuju algoritamsko razmišljanje, dijalog i animaciju, a pritom proučavaju inspirativne osobe. 	Aktivnost je kreativna i pristupačna za povezivanje programiranja, pripovijedanja i digitalne pismenosti. </t>
+    <t xml:space="preserve">Uploaded 4 September 2025
+U ovoj aktivnosti učenici stvaraju interaktivnu priču o odabranoj znanstvenici koristeći Scratch. Radeći u timovima, istražuju algoritamsko razmišljanje, dijalog i animaciju, a pritom proučavaju inspirativne osobe. 	Aktivnost je kreativna i pristupačna za povezivanje programiranja, pripovijedanja i digitalne pismenosti. </t>
   </si>
   <si>
     <t>Aktivita se Scratchem</t>
   </si>
   <si>
-    <t xml:space="preserve">V této aktivitě studenti vytvářejí interaktivní příběh o ženě ve vědě pomocí Scratch. Pracují v týmech, zkoumají algoritmické myšlení, dialog a animaci a zároveň se seznamují s inspirativními osobnostmi. Kreativní a přístupný způsob, jak propojit programování, vyprávění příběhů a digitální gramotnost. </t>
+    <t xml:space="preserve">Uploaded 4 September 2025
+V této aktivitě studenti vytvářejí interaktivní příběh o ženě ve vědě pomocí Scratch. Pracují v týmech, zkoumají algoritmické myšlení, dialog a animaci a zároveň se seznamují s inspirativními osobnostmi. Kreativní a přístupný způsob, jak propojit programování, vyprávění příběhů a digitální gramotnost. </t>
   </si>
   <si>
     <t>Scratch-aktivitet</t>
   </si>
   <si>
-    <t xml:space="preserve">I denne aktivitet skaber eleverne en interaktiv fortælling om en kvinde i videnskab ved hjælp af Scratch. De arbejder i teams og udforsker algoritmisk tænkning, dialog og animation, mens de undersøger inspirerende personer. En kreativ og tilgængelig måde at kombinere kodning, historiefortælling og digital dannelse. </t>
-  </si>
-  <si>
-    <t>Scratch activiteit</t>
-  </si>
-  <si>
-    <t>In deze activiteit creëren leerlingen een interactief verhaal over een vrouw in de wetenschap met behulp van Scratch. In teams verkennen ze algoritmisch denken, dialoog en animatie terwijl ze inspirerende figuren onderzoeken. Een creatieve en toegankelijke manier om coderen, verhalen vertellen en digitale geletterdheid te combineren.</t>
+    <t xml:space="preserve">Uploaded 4 September 2025
+I denne aktivitet skaber eleverne en interaktiv fortælling om en kvinde i videnskab ved hjælp af Scratch. De arbejder i teams og udforsker algoritmisk tænkning, dialog og animation, mens de undersøger inspirerende personer. En kreativ og tilgængelig måde at kombinere kodning, historiefortælling og digital dannelse. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scratch activiteit </t>
+  </si>
+  <si>
+    <t>Uploaded 4 September 2025
+In deze activiteit creëren leerlingen een interactief verhaal over een vrouw in de wetenschap met behulp van Scratch. In teams verkennen ze algoritmisch denken, dialoog en animatie terwijl ze inspirerende figuren onderzoeken. Een creatieve en toegankelijke manier om coderen, verhalen vertellen en digitale geletterdheid te combineren.</t>
   </si>
   <si>
     <t>Scratch Activity</t>
   </si>
   <si>
-    <t>In this activity, learners create an interactive story about a woman in science using Scratch. Working in teams, they explore algorithmic thinking, dialogue, and animation while researching inspiring figures. A creative and accessible way to blend coding, storytelling, and digital literacy.</t>
-  </si>
-  <si>
-    <t>Activité avec Scratch</t>
-  </si>
-  <si>
-    <t>Dans cette activité, les élèves créent une histoire interactive sur une femme scientifique en utilisant Scratch. En équipes, ils explorent la pensée algorithmique, le dialogue et l’animation tout en recherchant des figures inspirantes. Une manière créative et accessible de combiner programmation, narration et culture numérique.</t>
+    <t>Uploaded 4 September 2025
+In this activity, learners create an interactive story about a woman in science using Scratch. Working in teams, they explore algorithmic thinking, dialogue, and animation while researching inspiring figures. A creative and accessible way to blend coding, storytelling, and digital literacy.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Activité avec Scratch </t>
+  </si>
+  <si>
+    <t>Uploaded 4 September 2025
+Dans cette activité, les élèves créent une histoire interactive sur une femme scientifique en utilisant Scratch. En équipes, ils explorent la pensée algorithmique, le dialogue et l’animation tout en recherchant des figures inspirantes. Une manière créative et accessible de combiner programmation, narration et culture numérique.</t>
   </si>
   <si>
     <t>Aktivität: Storytelling mit Scratch</t>
   </si>
   <si>
-    <t>In dieser Aktivität kreieren die Lernenden mit Scratch eine interaktive Geschichte über eine berühmte Wissenschaftlerin. In Teamarbeit üben sie algorithmisches Denken und Kommunikation, recherchieren zu inspirierenden Persönlichkeiten und animieren die Ergebnisse. Ein kreativer und niedrigschwelliger Ansatz zur Verbindung von Programmieren, Geschichtenerzählen und digitalen Kompetenzen.</t>
+    <t>Uploaded 4 September 2025
+In dieser Aktivität kreieren die Lernenden mit Scratch eine interaktive Geschichte über eine berühmte Wissenschaftlerin. In Teamarbeit üben sie algorithmisches Denken und Kommunikation, recherchieren zu inspirierenden Persönlichkeiten und animieren die Ergebnisse. Ein kreativer und niedrigschwelliger Ansatz zur Verbindung von Programmieren, Geschichtenerzählen und digitalen Kompetenzen.</t>
   </si>
   <si>
     <t>Δραστηριότητα με Scratch</t>
   </si>
   <si>
-    <t>Σε αυτή τη δραστηριότητα, οι μαθητές δημιουργούν μια διαδραστική ιστορία για μια γυναίκα στην επιστήμη χρησιμοποιώντας τη Scratch. Εργαζόμενοι σε ομάδες, εξερευνούν τον αλγοριθμικό τρόπο σκέψης, την κίνηση των χαρακτήρων και τη δημιουργία διαλόγων, ενώ ερευνούν εμπνευσμένα πρότυπα. Ένας δημιουργικός και προσιτός τρόπος για να συνδυάσουν τον προγραμματισμό, την αφήγηση και τον ψηφιακό γραμματισμό.</t>
+    <t>Uploaded 4 September 2025
+Σε αυτή τη δραστηριότητα, οι μαθητές δημιουργούν μια διαδραστική ιστορία για μια γυναίκα στην επιστήμη χρησιμοποιώντας τη Scratch. Εργαζόμενοι σε ομάδες, εξερευνούν τον αλγοριθμικό τρόπο σκέψης, την κίνηση των χαρακτήρων και τη δημιουργία διαλόγων, ενώ ερευνούν εμπνευσμένα πρότυπα. Ένας δημιουργικός και προσιτός τρόπος για να συνδυάσουν τον προγραμματισμό, την αφήγηση και τον ψηφιακό γραμματισμό.</t>
   </si>
   <si>
     <t>Attività con Scratch</t>
   </si>
   <si>
-    <t>In questa attività, gli studenti creano una storia interattiva su una donna nella scienza usando Scratch. Lavorando in gruppo, esplorano il pensiero algoritmico, i dialoghi e l'animazione mentre ricercano figure ispiratrici. Un modo creativo e accessibile per unire programmazione, narrazione e alfabetizzazione digitale.</t>
+    <t>Uploaded 4 September 2025
+In questa attività, gli studenti creano una storia interattiva su una donna nella scienza usando Scratch. Lavorando in gruppo, esplorano il pensiero algoritmico, i dialoghi e l'animazione mentre ricercano figure ispiratrici. Un modo creativo e accessibile per unire programmazione, narrazione e alfabetizzazione digitale.</t>
   </si>
   <si>
     <t>Scratch aktivitāte</t>
   </si>
   <si>
-    <t>Šajā aktivitātē skolēni veido interaktīvu stāstu par sievieti zinātnē, izmantojot Scratch. Strādājot komandās, viņi pēta algoritmisko domāšanu, dialogu un animāciju, vienlaikus pētot iedvesmojošas personības. Radošs un pieejams veids, kā apvienot programmēšanu, stāstniecību un digitālo pratību.</t>
+    <t>Uploaded 4 September 2025
+Šajā aktivitātē skolēni veido interaktīvu stāstu par sievieti zinātnē, izmantojot Scratch. Strādājot komandās, viņi pēta algoritmisko domāšanu, dialogu un animāciju, vienlaikus pētot iedvesmojošas personības. Radošs un pieejams veids, kā apvienot programmēšanu, stāstniecību un digitālo pratību.</t>
   </si>
   <si>
     <t>„Scratch“ veikla</t>
   </si>
   <si>
-    <t>šiame užsiėmime mokiniai, pasitelkę „Scratch“, kuria interaktyvų pasakojimą apie moteris moksle. Dirbdami komandose, jie susipažįsta su algoritminiu mąstymu, dialogais ir animacija, kartu nagrinėdami įkvepiančias asmenybes. Kūrybiškas ir prieinamas būdas sujungti programavimą, pasakojimą ir skaitmeninį raštingumą.</t>
+    <t>Uploaded 4 September 2025
+šiame užsiėmime mokiniai, pasitelkę „Scratch“, kuria interaktyvų pasakojimą apie moteris moksle. Dirbdami komandose, jie susipažįsta su algoritminiu mąstymu, dialogais ir animacija, kartu nagrinėdami įkvepiančias asmenybes. Kūrybiškas ir prieinamas būdas sujungti programavimą, pasakojimą ir skaitmeninį raštingumą.</t>
   </si>
   <si>
     <t>Attività Scratch</t>
   </si>
   <si>
-    <t>F’din l-attività, l-istudenti joħolqu storja interattiva dwar mara fix-xjenza bl-użu ta’ Scratch. Jaħdmu fi gruppi, jesploraw ħsieb algoritmiku, djalogu u animazzjoni waqt li jirriċerkaw figuri ta’ ispirazzjoni. Mod kreattiv u aċċessibbli biex jgħaqqdu l-ipprogrammar, it-tgħid tal-istejjer u l-ħiliet diġitali.</t>
+    <t>Uploaded 4 September 2025
+F’din l-attività, l-istudenti joħolqu storja interattiva dwar mara fix-xjenza bl-użu ta’ Scratch. Jaħdmu fi gruppi, jesploraw ħsieb algoritmiku, djalogu u animazzjoni waqt li jirriċerkaw figuri ta’ ispirazzjoni. Mod kreattiv u aċċessibbli biex jgħaqqdu l-ipprogrammar, it-tgħid tal-istejjer u l-ħiliet diġitali.</t>
   </si>
   <si>
     <t>Aktywność ze Scratchem</t>
   </si>
   <si>
-    <t>W tej aktywności uczniowie tworzą interaktywną historię o kobiecie w nauce za pomocą Scratch. Pracując w zespołach, badają algorytmiczne myślenie, dialog i animację, jednocześnie poznając inspirujące postacie. Kreatywny i dostępny sposób na połączenie programowania, opowiadania historii i kompetencji cyfrowych.</t>
+    <t>Uploaded 4 September 2025
+W tej aktywności uczniowie tworzą interaktywną historię o kobiecie w nauce za pomocą Scratch. Pracując w zespołach, badają algorytmiczne myślenie, dialog i animację, jednocześnie poznając inspirujące postacie. Kreatywny i dostępny sposób na połączenie programowania, opowiadania historii i kompetencji cyfrowych.</t>
   </si>
   <si>
     <t xml:space="preserve">Atividade com Scratch 
 </t>
   </si>
   <si>
-    <t>Nesta atividade, os alunos criam uma história interativa sobre uma mulher na ciência usando o Scratch. Trabalhando em equipe, exploram o pensamento algorítmico, o diálogo e a animação enquanto pesquisam figuras inspiradoras. Uma forma criativa e acessível de combinar programação, narrativa e alfabetização digital.</t>
+    <t>Uploaded 4 September 2025
+Nesta atividade, os alunos criam uma história interativa sobre uma mulher na ciência usando o Scratch. Trabalhando em equipe, exploram o pensamento algorítmico, o diálogo e a animação enquanto pesquisam figuras inspiradoras. Uma forma criativa e acessível de combinar programação, narrativa e alfabetização digital.</t>
   </si>
   <si>
     <t>Activitate cu Scratch</t>
   </si>
   <si>
-    <t xml:space="preserve">În această activitate, elevii creează o poveste interactivă despre o femeie din știință folosind Scratch. Lucrând în echipe, explorează gândirea algoritmică, dialogul și animația, cercetând în același timp figuri inspiraționale. O modalitate creativă și accesibilă de a combina programarea, povestirea și competențele digitale. </t>
+    <t xml:space="preserve">Uploaded 4 September 2025
+În această activitate, elevii creează o poveste interactivă despre o femeie din știință folosind Scratch. Lucrând în echipe, explorează gândirea algoritmică, dialogul și animația, cercetând în același timp figuri inspiraționale. O modalitate creativă și accesibilă de a combina programarea, povestirea și competențele digitale. </t>
   </si>
   <si>
     <t>Aktivita so Scratchem</t>
   </si>
   <si>
-    <t>V tejto aktivite žiaci vytvoria interaktívny príbeh o žene vo vede pomocou Scratch. Pracujú v tímoch, skúmajú algoritmické myslenie, dialóg a animáciu a zároveň spoznávajú inšpiratívne osobnosti. Kreatívny a dostupný spôsob, ako spojiť programovanie, rozprávanie príbehov a digitálnu gramotnosť.</t>
+    <t>Uploaded 4 September 2025
+V tejto aktivite žiaci vytvoria interaktívny príbeh o žene vo vede pomocou Scratch. Pracujú v tímoch, skúmajú algoritmické myslenie, dialóg a animáciu a zároveň spoznávajú inšpiratívne osobnosti. Kreatívny a dostupný spôsob, ako spojiť programovanie, rozprávanie príbehov a digitálnu gramotnosť.</t>
   </si>
   <si>
     <t>Aktivnost v Scratchu</t>
   </si>
   <si>
-    <t>V tej aktivnosti učenci ustvarijo interaktivno zgodbo o izbrani znanstvenici s pomočjo programa Scratch. V timskem delu raziskujejo algoritmično razmišljanje, dialog in animacijo, hkrati pa spoznavajo navdihujoče osebnosti. Aktivnost je ustvarjalna in dostopna za povezovanje programiranja, pripovedovanja zgodb in digitalne pismenosti.</t>
+    <t>Uploaded 4 September 2025
+V tej aktivnosti učenci ustvarijo interaktivno zgodbo o izbrani znanstvenici s pomočjo programa Scratch. V timskem delu raziskujejo algoritmično razmišljanje, dialog in animacijo, hkrati pa spoznavajo navdihujoče osebnosti. Aktivnost je ustvarjalna in dostopna za povezovanje programiranja, pripovedovanja zgodb in digitalne pismenosti.</t>
   </si>
   <si>
     <t>Actividad con Scratch</t>
   </si>
   <si>
-    <t>En esta actividad, los estudiantes crean una historia interactiva sobre una mujer en la ciencia utilizando Scratch. Trabajando en equipos, exploran el pensamiento algorítmico, el diálogo y la animación mientras investigan figuras inspiradoras. Una forma creativa y accesible de combinar programación, narración y alfabetización digital.</t>
+    <t>Uploaded 4 September 2025
+En esta actividad, los estudiantes crean una historia interactiva sobre una mujer en la ciencia utilizando Scratch. Trabajando en equipos, exploran el pensamiento algorítmico, el diálogo y la animación mientras investigan figuras inspiradoras. Una forma creativa y accesible de combinar programación, narración y alfabetización digital.</t>
   </si>
   <si>
     <t xml:space="preserve">Scratch-harjoitus 
 </t>
   </si>
   <si>
-    <t>Tässä harjoituksessa oppilaat luovat Scratchilla interaktiivisen tarinan naisesta tieteessä. Ryhmissä he tutkivat algoritmista ajattelua, dialogia ja animaatiota samalla kun perehtyvät inspiroiviin henkilöihin. Luova ja saavutettava tapa yhdistää koodaus, tarinankerronta ja digitaaliset taidot.</t>
-  </si>
-  <si>
-    <t>I denna aktivitet skapar eleverna en interaktiv berättelse om en kvinna inom vetenskap med hjälp av Scratch. De arbetar i team och utforskar algoritmiskt tänkande, dialog och animation samtidigt som de undersöker inspirerande förebilder. Ett kreativt och tillgängligt sätt att kombinera programmering, berättande och digital kompetens.</t>
+    <t>Uploaded 4 September 2025
+Tässä harjoituksessa oppilaat luovat Scratchilla interaktiivisen tarinan naisesta tieteessä. Ryhmissä he tutkivat algoritmista ajattelua, dialogia ja animaatiota samalla kun perehtyvät inspiroiviin henkilöihin. Luova ja saavutettava tapa yhdistää koodaus, tarinankerronta ja digitaaliset taidot.</t>
+  </si>
+  <si>
+    <t>Uploaded 4 September 2025
+I denna aktivitet skapar eleverna en interaktiv berättelse om en kvinna inom vetenskap med hjälp av Scratch. De arbetar i team och utforskar algoritmiskt tänkande, dialog och animation samtidigt som de undersöker inspirerande förebilder. Ett kreativt och tillgängligt sätt att kombinera programmering, berättande och digital kompetens.</t>
   </si>
   <si>
     <t>Scratch Etkinliği</t>
   </si>
   <si>
-    <t>Bu etkinlikte, öğrenciler Scratch kullanarak bilim dünyasındaki bir kadın hakkında etkileşimli bir hikaye oluştururlar. Ekipler halinde çalışarak, ilham verici figürleri araştırırken algoritmik düşünme, diyalog ve animasyonu keşfederler. Kodlama, hikaye anlatımı ve dijital okuryazarlığı harmanlamanın yaratıcı ve erişilebilir bir yoludur.</t>
+    <t>Uploaded 4 September 2025
+Bu etkinlikte, öğrenciler Scratch kullanarak bilim dünyasındaki bir kadın hakkında etkileşimli bir hikaye oluştururlar. Ekipler halinde çalışarak, ilham verici figürleri araştırırken algoritmik düşünme, diyalog ve animasyonu keşfederler. Kodlama, hikaye anlatımı ve dijital okuryazarlığı harmanlamanın yaratıcı ve erişilebilir bir yoludur.</t>
   </si>
   <si>
     <t>Активність зі Scratch</t>
   </si>
   <si>
-    <t>Під час цієї активності учні створюють інтерактивну історію про жінку в науці за допомогою Scratch. Працюючи в командах, вони розвивають алгоритмічне мислення, опановують створення діалогів та анімацій, досліджуючи водночас надихаючі постаті. Це креативний та доступний спосіб поєднати програмування, сторітелінг і цифрову грамотність.</t>
+    <t>Uploaded 4 September 2025
+Під час цієї активності учні створюють інтерактивну історію про жінку в науці за допомогою Scratch. Працюючи в командах, вони розвивають алгоритмічне мислення, опановують створення діалогів та анімацій, досліджуючи водночас надихаючі постаті. Це креативний та доступний спосіб поєднати програмування, сторітелінг і цифрову грамотність.</t>
   </si>
   <si>
     <t>Scratch Cards</t>
   </si>
   <si>
-    <t>​The Scratch Cards are concise, printable resources designed to introduce users to fundamental Scratch coding concepts through engaging, hands-on activities. Each card focuses on a specific task, providing step-by-step instructions to help learners create interactive projects.</t>
+    <t>Uploaded 17 July 2025
+​The Scratch Cards are concise, printable resources designed to introduce users to fundamental Scratch coding concepts through engaging, hands-on activities. Each card focuses on a specific task, providing step-by-step instructions to help learners create interactive projects.</t>
   </si>
   <si>
     <t>Scratch - Educator Guide</t>
   </si>
   <si>
-    <t>​Comprehensive resource designed to assist educators in planning and conducting one-hour workshops using Scratch. It offers structured guidance to help participants, especially beginners, gain foundational coding experience through engaging activities.</t>
+    <t>Uploaded 17 July 2025
+​Comprehensive resource designed to assist educators in planning and conducting one-hour workshops using Scratch. It offers structured guidance to help participants, especially beginners, gain foundational coding experience through engaging activities.</t>
   </si>
   <si>
     <t>Learning Creative Learning</t>
   </si>
   <si>
-    <t>​Learning Creative Learning is a free online course and international community of educators exploring how to support creative learning. It offers discussions, workshops, and activities to promote project-based, interest-driven, collaborative, and playful learning. Educators can access videos and readings, discuss in an online forum, join video discussions and hands-on creative coding workshops, and experiment with innovative ways of teaching.</t>
+    <t>Uploaded 17 July 2025
+​Learning Creative Learning is a free online course and international community of educators exploring how to support creative learning. It offers discussions, workshops, and activities to promote project-based, interest-driven, collaborative, and playful learning. Educators can access videos and readings, discuss in an online forum, join video discussions and hands-on creative coding workshops, and experiment with innovative ways of teaching.</t>
   </si>
   <si>
     <t>OctoStudio</t>
   </si>
   <si>
-    <t xml:space="preserve">​OctoStudio is a playful coding platform designed for young creators. With an easy-to-use interface, kids can create interactive animations, games, and digital stories. The platform encourages experimentation and learning through play, making it a great introduction to programming for children. It is accessible for blind and low vision students using a screen reader built into tablets and phones. </t>
+    <t xml:space="preserve">Uploaded 17 July 2025
+​OctoStudio is a playful coding platform designed for young creators. With an easy-to-use interface, kids can create interactive animations, games, and digital stories. The platform encourages experimentation and learning through play, making it a great introduction to programming for children. It is accessible for blind and low vision students using a screen reader built into tablets and phones. </t>
   </si>
   <si>
     <t>OctoStudio - Create a Creature</t>
   </si>
   <si>
-    <t>​This fun activity allows children to design and animate their own digital creatures. Using simple coding blocks, they can bring their creations to life with movements and interactions. It’s a great way to introduce kids to programming while sparking creativity and imagination.</t>
+    <t>Uploaded 17 July 2025
+​This fun activity allows children to design and animate their own digital creatures. Using simple coding blocks, they can bring their creations to life with movements and interactions. It’s a great way to introduce kids to programming while sparking creativity and imagination.</t>
   </si>
   <si>
     <t>OctoStudio - Tilt Game</t>
   </si>
   <si>
-    <t>​Learn the basics of game design by creating an interactive tilt-controlled game. This activity helps kids understand motion-based programming concepts while making their own fun and engaging game. It’s a hands-on way to explore coding in a creative and interactive manner.</t>
+    <t>Uploaded 17 July 2025
+​Learn the basics of game design by creating an interactive tilt-controlled game. This activity helps kids understand motion-based programming concepts while making their own fun and engaging game. It’s a hands-on way to explore coding in a creative and interactive manner.</t>
   </si>
   <si>
     <t>OctoStudio - Exploratorium</t>
   </si>
   <si>
-    <t>​These activities offer digital creativity combined with hands-on tinkering with physical materials. Kids and educators can create unique projects that integrate coding with explorations, encouraging problem-solving and critical thinking. It’s an exciting way to combine coding with real-world play, exploration, and making.</t>
+    <t>Uploaded 17 July 2025
+​These activities offer digital creativity combined with hands-on tinkering with physical materials. Kids and educators can create unique projects that integrate coding with explorations, encouraging problem-solving and critical thinking. It’s an exciting way to combine coding with real-world play, exploration, and making.</t>
   </si>
   <si>
     <t>AI Fundamentals with IBM SkillsBuild</t>
   </si>
   <si>
-    <t>​This course introduces students to artificial intelligence (AI) and machine learning concepts using IBM tools. Participants will learn how AI is used in various industries, understand key principles, and explore practical applications. It’s a great starting point for those interested in emerging technologies.</t>
+    <t>Uploaded 17 July 2025
+​This course introduces students to artificial intelligence (AI) and machine learning concepts using IBM tools. Participants will learn how AI is used in various industries, understand key principles, and explore practical applications. It’s a great starting point for those interested in emerging technologies.</t>
   </si>
   <si>
     <t>Introduction to Data Science</t>
   </si>
   <si>
-    <t>​This course covers the fundamentals of data science, including data collection, analysis, and visualization. Participants will learn how to extract insights from data and apply analytical thinking. It's ideal for those looking to explore careers in data science and analytics.</t>
+    <t>Uploaded 17 July 2025
+​This course covers the fundamentals of data science, including data collection, analysis, and visualization. Participants will learn how to extract insights from data and apply analytical thinking. It's ideal for those looking to explore careers in data science and analytics.</t>
   </si>
   <si>
     <t>Exploring Sustainability</t>
   </si>
   <si>
-    <t>​This module explores how technology contributes to sustainability and environmental protection. It discusses the impact of digital solutions on energy efficiency, waste reduction, and responsible resource management. Learners will gain insights into green technology and sustainable practices.</t>
+    <t>Uploaded 17 July 2025
+​This module explores how technology contributes to sustainability and environmental protection. It discusses the impact of digital solutions on energy efficiency, waste reduction, and responsible resource management. Learners will gain insights into green technology and sustainable practices.</t>
   </si>
   <si>
     <t>Introduction to IoT and Digital Transformation</t>
   </si>
   <si>
-    <t>​Learn how the Internet of Things (IoT) connects devices and transforms industries. This course covers IoT applications, smart technologies, and data exchange systems. Participants will understand the role of IoT in shaping the future of smart cities, healthcare, and automation.</t>
+    <t>Uploaded 17 July 2025
+​Learn how the Internet of Things (IoT) connects devices and transforms industries. This course covers IoT applications, smart technologies, and data exchange systems. Participants will understand the role of IoT in shaping the future of smart cities, healthcare, and automation.</t>
   </si>
   <si>
     <t>Introduction to Cybersecurity</t>
   </si>
   <si>
-    <t>​With increasing cyber threats, this course introduces essential cybersecurity concepts, including online safety, data protection, and cyber attack prevention. Learners will develop foundational skills to protect digital assets and explore career opportunities in cybersecurity.</t>
+    <t>Uploaded 17 July 2025
+​With increasing cyber threats, this course introduces essential cybersecurity concepts, including online safety, data protection, and cyber attack prevention. Learners will develop foundational skills to protect digital assets and explore career opportunities in cybersecurity.</t>
   </si>
   <si>
     <t>Digital Awareness</t>
   </si>
   <si>
-    <t>​This course provides an understanding of digital literacy, online safety, and responsible technology use. It helps learners develop essential skills for navigating the digital world securely, including recognizing online threats and maintaining privacy.</t>
+    <t>Uploaded 17 July 2025
+​This course provides an understanding of digital literacy, online safety, and responsible technology use. It helps learners develop essential skills for navigating the digital world securely, including recognizing online threats and maintaining privacy.</t>
   </si>
   <si>
     <t>Using Computer and Mobile Devices</t>
   </si>
   <si>
-    <t>​This course explains how computers and mobile devices function, including hardware, software, and connectivity. Learners will explore networking basics, troubleshooting common issues, and understanding how devices communicate within digital environments.</t>
+    <t>Uploaded 17 July 2025
+​This course explains how computers and mobile devices function, including hardware, software, and connectivity. Learners will explore networking basics, troubleshooting common issues, and understanding how devices communicate within digital environments.</t>
   </si>
   <si>
     <t>Linux Unhatched</t>
   </si>
   <si>
-    <t>​A beginner-friendly introduction to Linux, covering fundamental commands and system navigation. This course is ideal for those new to the Linux environment, helping them build confidence in using open-source operating systems.</t>
+    <t>Uploaded 17 July 2025
+​A beginner-friendly introduction to Linux, covering fundamental commands and system navigation. This course is ideal for those new to the Linux environment, helping them build confidence in using open-source operating systems.</t>
   </si>
   <si>
     <t>AI in STEM Education</t>
   </si>
   <si>
-    <t>​To support teachers with preparing their students for the digital future, these five digital teaching units offer tools, methods as well as project and cooperation ideas for integrating the complex topic of AI and machine learning into the classroom. They are suited for teachers with and without previous experience in the subject and provide activities and resources for all school types, from primary to secondary education.</t>
+    <t>Uploaded 17 July 2025
+​To support teachers with preparing their students for the digital future, these five digital teaching units offer tools, methods as well as project and cooperation ideas for integrating the complex topic of AI and machine learning into the classroom. They are suited for teachers with and without previous experience in the subject and provide activities and resources for all school types, from primary to secondary education.</t>
   </si>
   <si>
     <t>AI Skills Passport | EY - Global</t>
   </si>
   <si>
-    <t xml:space="preserve">This course is a free, digital learning course for youth ages 16+ to upskill themselves on what AI is, how it's built, ethical considerations and employability pathways across using AI within sustainability, business and technology sectors. The course can be taken on mobile phone or laptop at your on pace- typically 6-10 hours of learning. At the end of the course, students receive an EY Microsoft branded certificate. </t>
+    <t xml:space="preserve">Uploaded 4 September 2025
+This course is a free, digital learning course for youth ages 16+ to upskill themselves on what AI is, how it's built, ethical considerations and employability pathways across using AI within sustainability, business and technology sectors. The course can be taken on mobile phone or laptop at your on pace- typically 6-10 hours of learning. At the end of the course, students receive an EY Microsoft branded certificate. </t>
   </si>
   <si>
     <t>HP Gaming garage</t>
   </si>
   <si>
-    <t xml:space="preserve">HP Gaming Garage fosters essential skills for the Gaming, Media, and ICT industries. With nearly 100 interactive modules, professional certification on successful completion, and access to global hackathons and incubators, the HP Gaming Garage is more than just a program. It's a launchpad for meaningful progress, designed to inspire future innovators in esports management, game design, and programming. </t>
+    <t xml:space="preserve">Uploaded 4 September 2025
+HP Gaming Garage fosters essential skills for the Gaming, Media, and ICT industries. With nearly 100 interactive modules, professional certification on successful completion, and access to global hackathons and incubators, the HP Gaming Garage is more than just a program. It's a launchpad for meaningful progress, designed to inspire future innovators in esports management, game design, and programming. </t>
   </si>
   <si>
     <t>HP AI Teacher Academy</t>
   </si>
   <si>
-    <t xml:space="preserve">The HP AI Teacher Academy courses is designed for K12 educators. This course provides hands-on exercises &amp; projects that help teachers develop their skills and confidence in using generative AI for their own teaching and learning. It aims to provide educators with essential knowledge and skills to understand, use, and evaluate generative AI systems. Through five interactive, self-guided modules, participants will learn about AI literacy, effective prompting techniques, practical applications, limitations of generative AI, and strategies for integrating AI into teaching. By the course's end, educators will be prepared to navigate AI's risks and benefits, leveraging it ethically and effectively in educational settings. </t>
+    <t xml:space="preserve">Uploaded 4 September 2025
+The HP AI Teacher Academy courses is designed for K12 educators. This course provides hands-on exercises &amp; projects that help teachers develop their skills and confidence in using generative AI for their own teaching and learning. It aims to provide educators with essential knowledge and skills to understand, use, and evaluate generative AI systems. Through five interactive, self-guided modules, participants will learn about AI literacy, effective prompting techniques, practical applications, limitations of generative AI, and strategies for integrating AI into teaching. By the course's end, educators will be prepared to navigate AI's risks and benefits, leveraging it ethically and effectively in educational settings. </t>
   </si>
   <si>
     <t>AI for Beginners</t>
   </si>
   <si>
-    <t>How can artificial intelligence (AI) help me navigate our rapidly changing technological landscape and help me prepare for the future of work? Develop a basic understanding of AI and learn how it is transforming economics, education, industries, and everyday life.</t>
+    <t>Uploaded 4 September 2025
+How can artificial intelligence (AI) help me navigate our rapidly changing technological landscape and help me prepare for the future of work? Develop a basic understanding of AI and learn how it is transforming economics, education, industries, and everyday life.</t>
   </si>
   <si>
     <t>Introduction to Digital Business Skills</t>
   </si>
   <si>
-    <t>What are the future trends of work and how can I equip myself with the knowledge and tools to thrive in an increasingly digital world?Gain insight from industry leaders and uncover best practices for how digital technologies are transforming the worlds of business and daily life.</t>
+    <t>Uploaded 4 September 2025
+What are the future trends of work and how can I equip myself with the knowledge and tools to thrive in an increasingly digital world?Gain insight from industry leaders and uncover best practices for how digital technologies are transforming the worlds of business and daily life.</t>
   </si>
   <si>
     <t>IT for Business Success</t>
   </si>
   <si>
-    <t>How do I assess what IT I should use in my business? Determine the types of technology solutions that best address your business goals and learn how different technologies directly and indirectly impact your business.</t>
+    <t>Uploaded 4 September 2025
+How do I assess what IT I should use in my business? Determine the types of technology solutions that best address your business goals and learn how different technologies directly and indirectly impact your business.</t>
   </si>
   <si>
     <t>Meet&amp;Code Inspiration library</t>
   </si>
   <si>
-    <t>It is is a free, searchable collection of coding and digital skills resources designed for organizers of youth tech events. You’ll find high-quality, curated content such as:
+    <t>Uploaded 4 September 2025
+It is is a free, searchable collection of coding and digital skills resources designed for organizers of youth tech events. You’ll find high-quality, curated content such as:
 Technology career insights, like tours of AWS data centers or Prime Video production processes.
 Themed coding challenges, for AI, STEM, climate action, and music (e.g. “Music Lab – Create music with code”).
 Ready-to-use tutorials and workshops, including resources from Code.org, Tynker, Raspberry Pi, and MIT App Inventor.
@@ -1770,20 +2041,57 @@
     <t>Digital Trust for All</t>
   </si>
   <si>
-    <t>Digital Trust for All is your gateway to becoming confident and secure in today’s digital world. Whether you're just getting started with technology or looking to strengthen your digital skills, this self-paced online course helps you understand how to safely navigate digital spaces and protect your personal information. Through three engaging modules, you’ll learn how to spot risks, build digital resilience, and take responsibility for your actions online. Each module earns you a digital badge you can showcase. Designed for everyday users, not tech experts, the program makes digital safety simple, practical, and relevant—so you can stay informed, stay protected, and be a trusted digital citizen.</t>
+    <t>Uploaded 12 September 2025
+Digital Trust for All is your gateway to becoming confident and secure in today’s digital world. Whether you're just getting started with technology or looking to strengthen your digital skills, this self-paced online course helps you understand how to safely navigate digital spaces and protect your personal information. Through three engaging modules, you’ll learn how to spot risks, build digital resilience, and take responsibility for your actions online. Each module earns you a digital badge you can showcase. Designed for everyday users, not tech experts, the program makes digital safety simple, practical, and relevant—so you can stay informed, stay protected, and be a trusted digital citizen.</t>
   </si>
   <si>
     <t>Parents Handbook</t>
   </si>
   <si>
-    <t>Introducing children to coding and digital skills is an exciting journey, but it can also feel overwhelming for parents and caregivers who may not know where to start. To make this process easier, EU Code Week has developed the Parents’ Handbook – a practical guide designed to help you support, encourage, and accompany your child as they take their first steps into the digital world.</t>
+    <t>Uploaded 3 October 2025
+Introducing children to coding and digital skills is an exciting journey, but it can also feel overwhelming for parents and caregivers who may not know where to start. To make this process easier, EU Code Week has developed the Parents’ Handbook – a practical guide designed to help you support, encourage, and accompany your child as they take their first steps into the digital world.</t>
+  </si>
+  <si>
+    <t>“Meitenes kodē labāk” sprints</t>
+  </si>
+  <si>
+    <t>Uploaded 4 September 2025
+Dinamiska 3–4 stundu darbnīca, kurā meitenes risina radošus tehnoloģiju izaicinājumus un izstrādā oriģinālus digitālos produktus. Ar praktisku vadību viņas jautrā un atbalstošā vidē iepazīstina ar kodēšanu, digitālo veidošanu un problēmu risināšanu. Lieliski piemērots zinātkāres rosināšanai un pārliecības veidošanai par tehnoloģijām — tiešsaistē vai klātienē.</t>
+  </si>
+  <si>
+    <t>„Girls Code It Better“ dirbtuvės</t>
+  </si>
+  <si>
+    <t>Uploaded 4 September 2025
+Dinamiškos 3–4 valandų dirbtuvės, kurioje merginos sprendžia kūrybinius technologijų iššūkius ir kuria originalius skaitmeninius produktus. Pagal praktinius nurodymus, jos smagioje ir palankioje aplinkoje susipažįsta su programavimu, skaitmenine kūryba ir problemų sprendimu. Puikiai tinka smalsumui sužadinti ir pasitikėjimui technologijomis ugdyti – internetu arba gyvai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Šprint “Girls Code It Better”  </t>
+  </si>
+  <si>
+    <t>Uploaded 4 September 2025
+Dynamický 3–4 hodinový workshop, kde dievčatá riešia kreatívne technologické výzvy a navrhujú originálne digitálne produkty. S praktickým vedením skúmajú programovanie, digitálnu tvorbu a riešenie problémov v zábavnom a podpornom prostredí. Ideálne na prebudenie zvedavosti a budovanie sebadôvery v oblasti technológií—online alebo prezenčne.</t>
+  </si>
+  <si>
+    <t>Kızlar Daha İyi Kod Yazıyor Sprinti</t>
+  </si>
+  <si>
+    <t>Uploaded 4 September 2025
+Kızların yaratıcı teknoloji zorluklarıyla mücadele edip özgün dijital ürünler tasarladıkları dinamik 3-4 saatlik bir atölye çalışması. Uygulamalı rehberlik eşliğinde, eğlenceli ve destekleyici bir ortamda kodlama, dijital üretim ve problem çözme becerilerini keşfediyorlar. Merak uyandırmak ve teknolojiye olan güveni artırmak için mükemmel bir seçenek - çevrimiçi veya yüz yüze.</t>
+  </si>
+  <si>
+    <t>Girls Code It Better Sprintti</t>
+  </si>
+  <si>
+    <t>Uploaded 4 September 2025
+Dynaaminen 3–4 tunnin työpaja, jossa tytöt ratkaisevat luovia teknologiahaasteita ja suunnittelevat omaperäisiä digitaalisia tuotteita. Käytännön ohjauksessa he tutustuvat ohjelmointiin, digitaaliseen luomiseen ja ongelmanratkaisuun hauskassa ja kannustavassa ympäristössä. Täydellinen tapa herättää uteliaisuutta ja vahvistaa itsevarmuutta teknologiassa—verkossa tai paikan päällä.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -1794,11 +2102,6 @@
       <sz val="11.0"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
-    </font>
-    <font>
-      <sz val="11.0"/>
-      <color theme="1"/>
-      <name val="Arial"/>
     </font>
     <font>
       <sz val="11.0"/>
@@ -1855,45 +2158,35 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="top"/>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="top"/>
+    <xf borderId="2" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2180,7 +2473,7 @@
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2208,7 +2501,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" ht="52.5" customHeight="1">
+    <row r="7" ht="72.75" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -2284,7 +2577,7 @@
       <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2484,7 +2777,7 @@
       <c r="A41" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B41" s="2" t="s">
         <v>81</v>
       </c>
     </row>
@@ -3121,7 +3414,7 @@
       </c>
     </row>
     <row r="121" ht="14.25" customHeight="1">
-      <c r="A121" s="4" t="s">
+      <c r="A121" s="3" t="s">
         <v>240</v>
       </c>
       <c r="B121" s="1" t="s">
@@ -3129,7 +3422,7 @@
       </c>
     </row>
     <row r="122" ht="14.25" customHeight="1">
-      <c r="A122" s="4" t="s">
+      <c r="A122" s="3" t="s">
         <v>242</v>
       </c>
       <c r="B122" s="1" t="s">
@@ -3137,7 +3430,7 @@
       </c>
     </row>
     <row r="123" ht="14.25" customHeight="1">
-      <c r="A123" s="4" t="s">
+      <c r="A123" s="3" t="s">
         <v>244</v>
       </c>
       <c r="B123" s="1" t="s">
@@ -3145,7 +3438,7 @@
       </c>
     </row>
     <row r="124" ht="14.25" customHeight="1">
-      <c r="A124" s="4" t="s">
+      <c r="A124" s="3" t="s">
         <v>246</v>
       </c>
       <c r="B124" s="1" t="s">
@@ -3153,7 +3446,7 @@
       </c>
     </row>
     <row r="125" ht="14.25" customHeight="1">
-      <c r="A125" s="4" t="s">
+      <c r="A125" s="3" t="s">
         <v>248</v>
       </c>
       <c r="B125" s="1" t="s">
@@ -3161,7 +3454,7 @@
       </c>
     </row>
     <row r="126" ht="14.25" customHeight="1">
-      <c r="A126" s="4" t="s">
+      <c r="A126" s="3" t="s">
         <v>250</v>
       </c>
       <c r="B126" s="1" t="s">
@@ -3177,7 +3470,7 @@
       </c>
     </row>
     <row r="128" ht="14.25" customHeight="1">
-      <c r="A128" s="4" t="s">
+      <c r="A128" s="3" t="s">
         <v>254</v>
       </c>
       <c r="B128" s="1" t="s">
@@ -3185,7 +3478,7 @@
       </c>
     </row>
     <row r="129" ht="14.25" customHeight="1">
-      <c r="A129" s="4" t="s">
+      <c r="A129" s="3" t="s">
         <v>256</v>
       </c>
       <c r="B129" s="1" t="s">
@@ -3193,7 +3486,7 @@
       </c>
     </row>
     <row r="130" ht="14.25" customHeight="1">
-      <c r="A130" s="4" t="s">
+      <c r="A130" s="3" t="s">
         <v>258</v>
       </c>
       <c r="B130" s="1" t="s">
@@ -3201,7 +3494,7 @@
       </c>
     </row>
     <row r="131" ht="14.25" customHeight="1">
-      <c r="A131" s="4" t="s">
+      <c r="A131" s="3" t="s">
         <v>260</v>
       </c>
       <c r="B131" s="1" t="s">
@@ -3209,7 +3502,7 @@
       </c>
     </row>
     <row r="132" ht="14.25" customHeight="1">
-      <c r="A132" s="4" t="s">
+      <c r="A132" s="3" t="s">
         <v>262</v>
       </c>
       <c r="B132" s="1" t="s">
@@ -3217,7 +3510,7 @@
       </c>
     </row>
     <row r="133" ht="14.25" customHeight="1">
-      <c r="A133" s="4" t="s">
+      <c r="A133" s="3" t="s">
         <v>264</v>
       </c>
       <c r="B133" s="1" t="s">
@@ -3225,7 +3518,7 @@
       </c>
     </row>
     <row r="134" ht="14.25" customHeight="1">
-      <c r="A134" s="4" t="s">
+      <c r="A134" s="3" t="s">
         <v>266</v>
       </c>
       <c r="B134" s="1" t="s">
@@ -3233,7 +3526,7 @@
       </c>
     </row>
     <row r="135" ht="14.25" customHeight="1">
-      <c r="A135" s="4" t="s">
+      <c r="A135" s="3" t="s">
         <v>268</v>
       </c>
       <c r="B135" s="1" t="s">
@@ -3241,7 +3534,7 @@
       </c>
     </row>
     <row r="136" ht="14.25" customHeight="1">
-      <c r="A136" s="4" t="s">
+      <c r="A136" s="3" t="s">
         <v>270</v>
       </c>
       <c r="B136" s="1" t="s">
@@ -3249,7 +3542,7 @@
       </c>
     </row>
     <row r="137" ht="14.25" customHeight="1">
-      <c r="A137" s="4" t="s">
+      <c r="A137" s="3" t="s">
         <v>272</v>
       </c>
       <c r="B137" s="1" t="s">
@@ -3257,7 +3550,7 @@
       </c>
     </row>
     <row r="138" ht="14.25" customHeight="1">
-      <c r="A138" s="4" t="s">
+      <c r="A138" s="3" t="s">
         <v>274</v>
       </c>
       <c r="B138" s="1" t="s">
@@ -3265,7 +3558,7 @@
       </c>
     </row>
     <row r="139" ht="14.25" customHeight="1">
-      <c r="A139" s="4" t="s">
+      <c r="A139" s="3" t="s">
         <v>276</v>
       </c>
       <c r="B139" s="1" t="s">
@@ -3273,7 +3566,7 @@
       </c>
     </row>
     <row r="140" ht="14.25" customHeight="1">
-      <c r="A140" s="4" t="s">
+      <c r="A140" s="3" t="s">
         <v>278</v>
       </c>
       <c r="B140" s="1" t="s">
@@ -3281,7 +3574,7 @@
       </c>
     </row>
     <row r="141" ht="14.25" customHeight="1">
-      <c r="A141" s="4" t="s">
+      <c r="A141" s="3" t="s">
         <v>280</v>
       </c>
       <c r="B141" s="1" t="s">
@@ -3289,7 +3582,7 @@
       </c>
     </row>
     <row r="142" ht="14.25" customHeight="1">
-      <c r="A142" s="4" t="s">
+      <c r="A142" s="3" t="s">
         <v>282</v>
       </c>
       <c r="B142" s="1" t="s">
@@ -3297,7 +3590,7 @@
       </c>
     </row>
     <row r="143" ht="14.25" customHeight="1">
-      <c r="A143" s="4" t="s">
+      <c r="A143" s="3" t="s">
         <v>284</v>
       </c>
       <c r="B143" s="1" t="s">
@@ -3305,7 +3598,7 @@
       </c>
     </row>
     <row r="144" ht="14.25" customHeight="1">
-      <c r="A144" s="4" t="s">
+      <c r="A144" s="3" t="s">
         <v>286</v>
       </c>
       <c r="B144" s="1" t="s">
@@ -3642,71 +3935,71 @@
     </row>
     <row r="186" ht="14.25" customHeight="1">
       <c r="A186" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B186" s="1" t="s">
         <v>370</v>
-      </c>
-      <c r="B186" s="1" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="187" ht="14.25" customHeight="1">
       <c r="A187" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="B187" s="1" t="s">
         <v>372</v>
-      </c>
-      <c r="B187" s="1" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="188" ht="14.25" customHeight="1">
       <c r="A188" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="B188" s="1" t="s">
         <v>374</v>
-      </c>
-      <c r="B188" s="1" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="189" ht="14.25" customHeight="1">
       <c r="A189" s="1" t="s">
-        <v>376</v>
+        <v>348</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="190" ht="14.25" customHeight="1">
       <c r="A190" s="1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="191" ht="14.25" customHeight="1">
       <c r="A191" s="1" t="s">
-        <v>352</v>
+        <v>378</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="192" ht="14.25" customHeight="1">
       <c r="A192" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="B192" s="1" t="s">
         <v>381</v>
-      </c>
-      <c r="B192" s="1" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="193" ht="14.25" customHeight="1">
       <c r="A193" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="B193" s="1" t="s">
         <v>383</v>
-      </c>
-      <c r="B193" s="1" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="194" ht="14.25" customHeight="1">
       <c r="A194" s="1" t="s">
-        <v>358</v>
+        <v>384</v>
       </c>
       <c r="B194" s="1" t="s">
         <v>385</v>
@@ -3866,47 +4159,47 @@
     </row>
     <row r="214" ht="14.25" customHeight="1">
       <c r="A214" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="B214" s="1" t="s">
         <v>424</v>
-      </c>
-      <c r="B214" s="1" t="s">
-        <v>425</v>
       </c>
     </row>
     <row r="215" ht="14.25" customHeight="1">
       <c r="A215" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="B215" s="1" t="s">
         <v>426</v>
-      </c>
-      <c r="B215" s="1" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="216" ht="14.25" customHeight="1">
       <c r="A216" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="B216" s="1" t="s">
         <v>428</v>
-      </c>
-      <c r="B216" s="1" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="217" ht="14.25" customHeight="1">
       <c r="A217" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="B217" s="1" t="s">
         <v>430</v>
-      </c>
-      <c r="B217" s="1" t="s">
-        <v>431</v>
       </c>
     </row>
     <row r="218" ht="14.25" customHeight="1">
       <c r="A218" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="B218" s="1" t="s">
         <v>432</v>
-      </c>
-      <c r="B218" s="1" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="219" ht="14.25" customHeight="1">
       <c r="A219" s="1" t="s">
-        <v>400</v>
+        <v>433</v>
       </c>
       <c r="B219" s="1" t="s">
         <v>434</v>
@@ -4058,47 +4351,47 @@
     </row>
     <row r="238" ht="14.25" customHeight="1">
       <c r="A238" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="B238" s="1" t="s">
         <v>471</v>
-      </c>
-      <c r="B238" s="1" t="s">
-        <v>472</v>
       </c>
     </row>
     <row r="239" ht="14.25" customHeight="1">
       <c r="A239" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="B239" s="1" t="s">
         <v>473</v>
-      </c>
-      <c r="B239" s="1" t="s">
-        <v>474</v>
       </c>
     </row>
     <row r="240" ht="14.25" customHeight="1">
       <c r="A240" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="B240" s="1" t="s">
         <v>475</v>
-      </c>
-      <c r="B240" s="1" t="s">
-        <v>476</v>
       </c>
     </row>
     <row r="241" ht="14.25" customHeight="1">
       <c r="A241" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="B241" s="1" t="s">
         <v>477</v>
-      </c>
-      <c r="B241" s="1" t="s">
-        <v>478</v>
       </c>
     </row>
     <row r="242" ht="14.25" customHeight="1">
       <c r="A242" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="B242" s="1" t="s">
         <v>479</v>
-      </c>
-      <c r="B242" s="1" t="s">
-        <v>480</v>
       </c>
     </row>
     <row r="243" ht="14.25" customHeight="1">
       <c r="A243" s="1" t="s">
-        <v>447</v>
+        <v>480</v>
       </c>
       <c r="B243" s="1" t="s">
         <v>481</v>
@@ -4217,7 +4510,7 @@
       </c>
     </row>
     <row r="258" ht="14.25" customHeight="1">
-      <c r="A258" s="1" t="s">
+      <c r="A258" s="4" t="s">
         <v>510</v>
       </c>
       <c r="B258" s="1" t="s">
@@ -4250,265 +4543,265 @@
     </row>
     <row r="262" ht="14.25" customHeight="1">
       <c r="A262" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="B262" s="1" t="s">
         <v>518</v>
       </c>
-      <c r="B262" s="1" t="s">
+    </row>
+    <row r="263" ht="14.25" customHeight="1">
+      <c r="A263" s="1" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="263" ht="14.25" customHeight="1">
-      <c r="A263" s="5" t="s">
+      <c r="B263" s="1" t="s">
         <v>520</v>
-      </c>
-      <c r="B263" s="1" t="s">
-        <v>521</v>
       </c>
     </row>
     <row r="264" ht="14.25" customHeight="1">
       <c r="A264" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="B264" s="1" t="s">
         <v>522</v>
       </c>
-      <c r="B264" s="1" t="s">
+    </row>
+    <row r="265" ht="14.25" customHeight="1">
+      <c r="A265" s="5" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="265" ht="14.25" customHeight="1">
-      <c r="A265" s="1" t="s">
+      <c r="B265" s="6" t="s">
         <v>524</v>
       </c>
-      <c r="B265" s="1" t="s">
+    </row>
+    <row r="266" ht="14.25" customHeight="1">
+      <c r="A266" s="7" t="s">
         <v>525</v>
       </c>
-    </row>
-    <row r="266" ht="14.25" customHeight="1">
-      <c r="A266" s="1" t="s">
+      <c r="B266" s="8" t="s">
         <v>526</v>
       </c>
-      <c r="B266" s="1" t="s">
+    </row>
+    <row r="267" ht="14.25" customHeight="1">
+      <c r="A267" s="7" t="s">
         <v>527</v>
       </c>
-    </row>
-    <row r="267" ht="14.25" customHeight="1">
-      <c r="A267" s="1" t="s">
-        <v>494</v>
-      </c>
-      <c r="B267" s="1" t="s">
+      <c r="B267" s="8" t="s">
         <v>528</v>
       </c>
     </row>
     <row r="268" ht="14.25" customHeight="1">
-      <c r="A268" s="1" t="s">
+      <c r="A268" s="7" t="s">
         <v>529</v>
       </c>
-      <c r="B268" s="1" t="s">
+      <c r="B268" s="8" t="s">
         <v>530</v>
       </c>
     </row>
     <row r="269" ht="14.25" customHeight="1">
-      <c r="A269" s="1" t="s">
+      <c r="A269" s="7" t="s">
         <v>531</v>
       </c>
-      <c r="B269" s="1" t="s">
+      <c r="B269" s="8" t="s">
         <v>532</v>
       </c>
     </row>
     <row r="270" ht="14.25" customHeight="1">
-      <c r="A270" s="6" t="s">
+      <c r="A270" s="7" t="s">
         <v>533</v>
       </c>
-      <c r="B270" s="7" t="s">
+      <c r="B270" s="8" t="s">
         <v>534</v>
       </c>
     </row>
     <row r="271" ht="14.25" customHeight="1">
-      <c r="A271" s="8" t="s">
+      <c r="A271" s="9" t="s">
         <v>535</v>
       </c>
-      <c r="B271" s="9" t="s">
+      <c r="B271" s="8" t="s">
         <v>536</v>
       </c>
     </row>
     <row r="272" ht="14.25" customHeight="1">
-      <c r="A272" s="8" t="s">
+      <c r="A272" s="7" t="s">
         <v>537</v>
       </c>
-      <c r="B272" s="9" t="s">
+      <c r="B272" s="8" t="s">
         <v>538</v>
       </c>
     </row>
     <row r="273" ht="14.25" customHeight="1">
-      <c r="A273" s="8" t="s">
+      <c r="A273" s="7" t="s">
         <v>539</v>
       </c>
-      <c r="B273" s="9" t="s">
+      <c r="B273" s="8" t="s">
         <v>540</v>
       </c>
     </row>
     <row r="274" ht="14.25" customHeight="1">
-      <c r="A274" s="8" t="s">
+      <c r="A274" s="7" t="s">
         <v>541</v>
       </c>
-      <c r="B274" s="9" t="s">
+      <c r="B274" s="8" t="s">
         <v>542</v>
       </c>
     </row>
     <row r="275" ht="14.25" customHeight="1">
-      <c r="A275" s="10" t="s">
+      <c r="A275" s="7" t="s">
         <v>543</v>
       </c>
-      <c r="B275" s="9" t="s">
+      <c r="B275" s="8" t="s">
         <v>544</v>
       </c>
     </row>
     <row r="276" ht="14.25" customHeight="1">
-      <c r="A276" s="10" t="s">
+      <c r="A276" s="7" t="s">
         <v>545</v>
       </c>
-      <c r="B276" s="9" t="s">
+      <c r="B276" s="8" t="s">
         <v>546</v>
       </c>
     </row>
     <row r="277" ht="14.25" customHeight="1">
-      <c r="A277" s="8" t="s">
+      <c r="A277" s="7" t="s">
         <v>547</v>
       </c>
-      <c r="B277" s="9" t="s">
+      <c r="B277" s="8" t="s">
         <v>548</v>
       </c>
     </row>
     <row r="278" ht="14.25" customHeight="1">
-      <c r="A278" s="8" t="s">
+      <c r="A278" s="7" t="s">
         <v>549</v>
       </c>
-      <c r="B278" s="9" t="s">
+      <c r="B278" s="8" t="s">
         <v>550</v>
       </c>
     </row>
     <row r="279" ht="14.25" customHeight="1">
-      <c r="A279" s="8" t="s">
+      <c r="A279" s="7" t="s">
         <v>551</v>
       </c>
-      <c r="B279" s="9" t="s">
+      <c r="B279" s="8" t="s">
         <v>552</v>
       </c>
     </row>
     <row r="280" ht="14.25" customHeight="1">
-      <c r="A280" s="8" t="s">
+      <c r="A280" s="7" t="s">
         <v>553</v>
       </c>
-      <c r="B280" s="9" t="s">
+      <c r="B280" s="6" t="s">
         <v>554</v>
       </c>
     </row>
     <row r="281" ht="14.25" customHeight="1">
-      <c r="A281" s="8" t="s">
+      <c r="A281" s="7" t="s">
         <v>555</v>
       </c>
-      <c r="B281" s="9" t="s">
+      <c r="B281" s="8" t="s">
         <v>556</v>
       </c>
     </row>
     <row r="282" ht="14.25" customHeight="1">
-      <c r="A282" s="8" t="s">
+      <c r="A282" s="7" t="s">
         <v>557</v>
       </c>
-      <c r="B282" s="9" t="s">
+      <c r="B282" s="8" t="s">
         <v>558</v>
       </c>
     </row>
     <row r="283" ht="14.25" customHeight="1">
-      <c r="A283" s="8" t="s">
+      <c r="A283" s="7" t="s">
         <v>559</v>
       </c>
-      <c r="B283" s="9" t="s">
+      <c r="B283" s="8" t="s">
         <v>560</v>
       </c>
     </row>
     <row r="284" ht="14.25" customHeight="1">
-      <c r="A284" s="8" t="s">
+      <c r="A284" s="7" t="s">
         <v>561</v>
       </c>
-      <c r="B284" s="9" t="s">
+      <c r="B284" s="8" t="s">
         <v>562</v>
       </c>
     </row>
     <row r="285" ht="14.25" customHeight="1">
-      <c r="A285" s="8" t="s">
+      <c r="A285" s="7" t="s">
         <v>563</v>
       </c>
-      <c r="B285" s="7" t="s">
+      <c r="B285" s="8" t="s">
         <v>564</v>
       </c>
     </row>
     <row r="286" ht="14.25" customHeight="1">
-      <c r="A286" s="8" t="s">
+      <c r="A286" s="7" t="s">
         <v>565</v>
       </c>
-      <c r="B286" s="11" t="s">
+      <c r="B286" s="8" t="s">
         <v>566</v>
       </c>
     </row>
     <row r="287" ht="14.25" customHeight="1">
-      <c r="A287" s="8" t="s">
+      <c r="A287" s="7" t="s">
         <v>567</v>
       </c>
-      <c r="B287" s="11" t="s">
+      <c r="B287" s="10" t="s">
         <v>568</v>
       </c>
     </row>
     <row r="288" ht="14.25" customHeight="1">
-      <c r="A288" s="8" t="s">
+      <c r="A288" s="7" t="s">
         <v>569</v>
       </c>
-      <c r="B288" s="11" t="s">
+      <c r="B288" s="8" t="s">
         <v>570</v>
       </c>
     </row>
     <row r="289" ht="14.25" customHeight="1">
-      <c r="A289" s="8" t="s">
+      <c r="A289" s="5" t="s">
         <v>571</v>
       </c>
-      <c r="B289" s="11" t="s">
+      <c r="B289" s="8" t="s">
         <v>572</v>
       </c>
     </row>
     <row r="290" ht="14.25" customHeight="1">
-      <c r="A290" s="8" t="s">
+      <c r="A290" s="1" t="s">
         <v>573</v>
       </c>
-      <c r="B290" s="11" t="s">
+      <c r="B290" s="1" t="s">
         <v>574</v>
       </c>
     </row>
     <row r="291" ht="14.25" customHeight="1">
-      <c r="A291" s="8" t="s">
+      <c r="A291" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="B291" s="11" t="s">
+      <c r="B291" s="1" t="s">
         <v>576</v>
       </c>
     </row>
     <row r="292" ht="14.25" customHeight="1">
-      <c r="A292" s="8" t="s">
+      <c r="A292" s="1" t="s">
         <v>577</v>
       </c>
-      <c r="B292" s="12" t="s">
+      <c r="B292" s="1" t="s">
         <v>578</v>
       </c>
     </row>
     <row r="293" ht="14.25" customHeight="1">
-      <c r="A293" s="8" t="s">
+      <c r="A293" s="1" t="s">
         <v>579</v>
       </c>
-      <c r="B293" s="9" t="s">
+      <c r="B293" s="1" t="s">
         <v>580</v>
       </c>
     </row>
     <row r="294" ht="14.25" customHeight="1">
-      <c r="A294" s="6" t="s">
+      <c r="A294" s="1" t="s">
         <v>581</v>
       </c>
-      <c r="B294" s="9" t="s">
+      <c r="B294" s="1" t="s">
         <v>582</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add newline in description when update
</commit_message>
<xml_diff>
--- a/resources/excel/Uploaded resources.xlsx
+++ b/resources/excel/Uploaded resources.xlsx
@@ -1298,23 +1298,8 @@
     <t>Aktywność Magic 8 Ball</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <rFont val="Aptos Narrow"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>Uploaded 4 September 2025
-Uczniowie poznają podstawowe</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Aptos Narrow"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t xml:space="preserve"> pojęcia programowania, tworząc cyfrową Magic 8 Ball za pomocą micro:bit i MakeCode. W zespołach projektują program, który wykorzystuje czujniki i liczby losowe do generowania odpowiedzi, gdy urządzenie jest potrząsane. Ta zabawna, praktyczna aktywność rozwija pracę zespołową, wprowadza do mechatroniki oraz rozwija umiejętności programowania i rozwiązywania problemów.</t>
-    </r>
+    <t>Uploaded 4 September 2025
+Uczniowie poznają podstawowe pojęcia programowania, tworząc cyfrową Magic 8 Ball za pomocą micro:bit i MakeCode. W zespołach projektują program, który wykorzystuje czujniki i liczby losowe do generowania odpowiedzi, gdy urządzenie jest potrząsane. Ta zabawna, praktyczna aktywność rozwija pracę zespołową, wprowadza do mechatroniki oraz rozwija umiejętności programowania i rozwiązywania problemów.</t>
   </si>
   <si>
     <t>Atividade Magic 8 Ball</t>
@@ -2091,7 +2076,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -2102,6 +2087,11 @@
       <sz val="11.0"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
     <font>
       <sz val="11.0"/>
@@ -2158,35 +2148,48 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+      <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2461,2347 +2464,2347 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" ht="14.25" customHeight="1">
+    <row r="2" ht="87.0" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" ht="72.0" customHeight="1">
+    <row r="3" ht="87.0" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" ht="14.25" customHeight="1">
+    <row r="4" ht="87.0" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" ht="14.25" customHeight="1">
+    <row r="5" ht="87.0" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" ht="57.75" customHeight="1">
+    <row r="6" ht="87.0" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" ht="72.75" customHeight="1">
+    <row r="7" ht="87.0" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" ht="14.25" customHeight="1">
+    <row r="8" ht="87.0" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" ht="14.25" customHeight="1">
+    <row r="9" ht="87.0" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" ht="75.75" customHeight="1">
+    <row r="10" ht="87.0" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" ht="14.25" customHeight="1">
+    <row r="11" ht="87.0" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" ht="14.25" customHeight="1">
+    <row r="12" ht="87.0" customHeight="1">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" ht="14.25" customHeight="1">
+    <row r="13" ht="87.0" customHeight="1">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" ht="63.0" customHeight="1">
+    <row r="14" ht="87.0" customHeight="1">
       <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" ht="14.25" customHeight="1">
+    <row r="15" ht="87.0" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" ht="69.75" customHeight="1">
+    <row r="16" ht="87.0" customHeight="1">
       <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" ht="14.25" customHeight="1">
+    <row r="17" ht="87.0" customHeight="1">
       <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" ht="14.25" customHeight="1">
+    <row r="18" ht="87.0" customHeight="1">
       <c r="A18" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" ht="77.25" customHeight="1">
+    <row r="19" ht="87.0" customHeight="1">
       <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" ht="14.25" customHeight="1">
+    <row r="20" ht="87.0" customHeight="1">
       <c r="A20" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21" ht="14.25" customHeight="1">
+    <row r="21" ht="87.0" customHeight="1">
       <c r="A21" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="22" ht="14.25" customHeight="1">
+    <row r="22" ht="87.0" customHeight="1">
       <c r="A22" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="23" ht="14.25" customHeight="1">
+    <row r="23" ht="87.0" customHeight="1">
       <c r="A23" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="24" ht="14.25" customHeight="1">
+    <row r="24" ht="87.0" customHeight="1">
       <c r="A24" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="25" ht="72.0" customHeight="1">
+    <row r="25" ht="87.0" customHeight="1">
       <c r="A25" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="26" ht="14.25" customHeight="1">
+    <row r="26" ht="87.0" customHeight="1">
       <c r="A26" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="27" ht="14.25" customHeight="1">
+    <row r="27" ht="87.0" customHeight="1">
       <c r="A27" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="28" ht="14.25" customHeight="1">
+    <row r="28" ht="87.0" customHeight="1">
       <c r="A28" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="29" ht="14.25" customHeight="1">
+    <row r="29" ht="87.0" customHeight="1">
       <c r="A29" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="30" ht="14.25" customHeight="1">
+    <row r="30" ht="87.0" customHeight="1">
       <c r="A30" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="31" ht="14.25" customHeight="1">
+    <row r="31" ht="87.0" customHeight="1">
       <c r="A31" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="32" ht="14.25" customHeight="1">
+    <row r="32" ht="87.0" customHeight="1">
       <c r="A32" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="33" ht="14.25" customHeight="1">
+    <row r="33" ht="87.0" customHeight="1">
       <c r="A33" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="34" ht="14.25" customHeight="1">
+    <row r="34" ht="87.0" customHeight="1">
       <c r="A34" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="35" ht="14.25" customHeight="1">
+    <row r="35" ht="87.0" customHeight="1">
       <c r="A35" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="36" ht="14.25" customHeight="1">
+    <row r="36" ht="87.0" customHeight="1">
       <c r="A36" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="37" ht="14.25" customHeight="1">
+    <row r="37" ht="87.0" customHeight="1">
       <c r="A37" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="38" ht="14.25" customHeight="1">
+    <row r="38" ht="87.0" customHeight="1">
       <c r="A38" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="39" ht="14.25" customHeight="1">
+    <row r="39" ht="87.0" customHeight="1">
       <c r="A39" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="40" ht="14.25" customHeight="1">
+    <row r="40" ht="87.0" customHeight="1">
       <c r="A40" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="41" ht="14.25" customHeight="1">
+    <row r="41" ht="87.0" customHeight="1">
       <c r="A41" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="42" ht="14.25" customHeight="1">
+    <row r="42" ht="87.0" customHeight="1">
       <c r="A42" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="43" ht="14.25" customHeight="1">
+    <row r="43" ht="87.0" customHeight="1">
       <c r="A43" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" s="3" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="44" ht="14.25" customHeight="1">
+    <row r="44" ht="87.0" customHeight="1">
       <c r="A44" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B44" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="45" ht="14.25" customHeight="1">
+    <row r="45" ht="87.0" customHeight="1">
       <c r="A45" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B45" s="3" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="46" ht="14.25" customHeight="1">
+    <row r="46" ht="87.0" customHeight="1">
       <c r="A46" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" s="3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="47" ht="14.25" customHeight="1">
+    <row r="47" ht="87.0" customHeight="1">
       <c r="A47" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" s="3" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="48" ht="14.25" customHeight="1">
+    <row r="48" ht="87.0" customHeight="1">
       <c r="A48" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B48" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="49" ht="14.25" customHeight="1">
+    <row r="49" ht="87.0" customHeight="1">
       <c r="A49" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B49" s="3" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="50" ht="14.25" customHeight="1">
+    <row r="50" ht="87.0" customHeight="1">
       <c r="A50" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B50" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="51" ht="14.25" customHeight="1">
+    <row r="51" ht="87.0" customHeight="1">
       <c r="A51" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B51" s="3" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="52" ht="14.25" customHeight="1">
+    <row r="52" ht="87.0" customHeight="1">
       <c r="A52" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B52" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="53" ht="14.25" customHeight="1">
+    <row r="53" ht="87.0" customHeight="1">
       <c r="A53" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B53" s="3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="54" ht="14.25" customHeight="1">
+    <row r="54" ht="87.0" customHeight="1">
       <c r="A54" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B54" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="55" ht="14.25" customHeight="1">
+    <row r="55" ht="87.0" customHeight="1">
       <c r="A55" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B55" s="3" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="56" ht="14.25" customHeight="1">
+    <row r="56" ht="87.0" customHeight="1">
       <c r="A56" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B56" s="3" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="57" ht="14.25" customHeight="1">
+    <row r="57" ht="87.0" customHeight="1">
       <c r="A57" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B57" s="3" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="58" ht="14.25" customHeight="1">
+    <row r="58" ht="87.0" customHeight="1">
       <c r="A58" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B58" s="3" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="59" ht="14.25" customHeight="1">
+    <row r="59" ht="87.0" customHeight="1">
       <c r="A59" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B59" s="3" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="60" ht="14.25" customHeight="1">
+    <row r="60" ht="87.0" customHeight="1">
       <c r="A60" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B60" s="3" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="61" ht="14.25" customHeight="1">
+    <row r="61" ht="87.0" customHeight="1">
       <c r="A61" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B61" s="3" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="62" ht="14.25" customHeight="1">
+    <row r="62" ht="87.0" customHeight="1">
       <c r="A62" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B62" s="3" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="63" ht="14.25" customHeight="1">
+    <row r="63" ht="87.0" customHeight="1">
       <c r="A63" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B63" s="3" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="64" ht="14.25" customHeight="1">
+    <row r="64" ht="87.0" customHeight="1">
       <c r="A64" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B64" s="3" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="65" ht="14.25" customHeight="1">
+    <row r="65" ht="87.0" customHeight="1">
       <c r="A65" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B65" s="3" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="66" ht="14.25" customHeight="1">
+    <row r="66" ht="87.0" customHeight="1">
       <c r="A66" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B66" s="3" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="67" ht="14.25" customHeight="1">
+    <row r="67" ht="87.0" customHeight="1">
       <c r="A67" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="B67" s="3" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="68" ht="14.25" customHeight="1">
+    <row r="68" ht="87.0" customHeight="1">
       <c r="A68" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B68" s="3" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="69" ht="14.25" customHeight="1">
+    <row r="69" ht="87.0" customHeight="1">
       <c r="A69" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B69" s="3" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="70" ht="14.25" customHeight="1">
+    <row r="70" ht="87.0" customHeight="1">
       <c r="A70" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B70" s="3" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="71" ht="14.25" customHeight="1">
+    <row r="71" ht="87.0" customHeight="1">
       <c r="A71" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B71" s="3" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="72" ht="14.25" customHeight="1">
+    <row r="72" ht="87.0" customHeight="1">
       <c r="A72" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="B72" s="3" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="73" ht="14.25" customHeight="1">
+    <row r="73" ht="87.0" customHeight="1">
       <c r="A73" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="B73" s="3" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="74" ht="14.25" customHeight="1">
+    <row r="74" ht="87.0" customHeight="1">
       <c r="A74" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="B74" s="3" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="75" ht="14.25" customHeight="1">
+    <row r="75" ht="87.0" customHeight="1">
       <c r="A75" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="B75" s="3" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="76" ht="14.25" customHeight="1">
+    <row r="76" ht="87.0" customHeight="1">
       <c r="A76" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="B76" s="3" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="77" ht="14.25" customHeight="1">
+    <row r="77" ht="87.0" customHeight="1">
       <c r="A77" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="B77" s="3" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="78" ht="14.25" customHeight="1">
+    <row r="78" ht="87.0" customHeight="1">
       <c r="A78" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="B78" s="3" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="79" ht="14.25" customHeight="1">
+    <row r="79" ht="87.0" customHeight="1">
       <c r="A79" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="B79" s="3" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="80" ht="14.25" customHeight="1">
+    <row r="80" ht="87.0" customHeight="1">
       <c r="A80" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="B80" s="3" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="81" ht="14.25" customHeight="1">
+    <row r="81" ht="87.0" customHeight="1">
       <c r="A81" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="B81" s="3" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="82" ht="14.25" customHeight="1">
+    <row r="82" ht="87.0" customHeight="1">
       <c r="A82" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="B82" s="3" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="83" ht="14.25" customHeight="1">
+    <row r="83" ht="87.0" customHeight="1">
       <c r="A83" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="B83" s="3" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="84" ht="14.25" customHeight="1">
+    <row r="84" ht="87.0" customHeight="1">
       <c r="A84" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="B84" s="3" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="85" ht="14.25" customHeight="1">
+    <row r="85" ht="87.0" customHeight="1">
       <c r="A85" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B85" s="1" t="s">
+      <c r="B85" s="3" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="86" ht="14.25" customHeight="1">
+    <row r="86" ht="87.0" customHeight="1">
       <c r="A86" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="B86" s="1" t="s">
+      <c r="B86" s="3" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="87" ht="14.25" customHeight="1">
+    <row r="87" ht="87.0" customHeight="1">
       <c r="A87" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="B87" s="1" t="s">
+      <c r="B87" s="3" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="88" ht="14.25" customHeight="1">
+    <row r="88" ht="87.0" customHeight="1">
       <c r="A88" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="B88" s="1" t="s">
+      <c r="B88" s="3" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="89" ht="14.25" customHeight="1">
+    <row r="89" ht="87.0" customHeight="1">
       <c r="A89" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="B89" s="3" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="90" ht="14.25" customHeight="1">
+    <row r="90" ht="87.0" customHeight="1">
       <c r="A90" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="B90" s="1" t="s">
+      <c r="B90" s="3" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="91" ht="14.25" customHeight="1">
+    <row r="91" ht="87.0" customHeight="1">
       <c r="A91" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B91" s="1" t="s">
+      <c r="B91" s="3" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="92" ht="14.25" customHeight="1">
+    <row r="92" ht="87.0" customHeight="1">
       <c r="A92" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="B92" s="1" t="s">
+      <c r="B92" s="3" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="93" ht="14.25" customHeight="1">
+    <row r="93" ht="87.0" customHeight="1">
       <c r="A93" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="B93" s="1" t="s">
+      <c r="B93" s="3" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="94" ht="14.25" customHeight="1">
+    <row r="94" ht="87.0" customHeight="1">
       <c r="A94" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B94" s="1" t="s">
+      <c r="B94" s="3" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="95" ht="14.25" customHeight="1">
+    <row r="95" ht="87.0" customHeight="1">
       <c r="A95" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="B95" s="1" t="s">
+      <c r="B95" s="3" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="96" ht="14.25" customHeight="1">
+    <row r="96" ht="87.0" customHeight="1">
       <c r="A96" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="B96" s="1" t="s">
+      <c r="B96" s="3" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="97" ht="14.25" customHeight="1">
+    <row r="97" ht="87.0" customHeight="1">
       <c r="A97" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="B97" s="1" t="s">
+      <c r="B97" s="3" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="98" ht="14.25" customHeight="1">
+    <row r="98" ht="87.0" customHeight="1">
       <c r="A98" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="B98" s="1" t="s">
+      <c r="B98" s="3" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="99" ht="14.25" customHeight="1">
+    <row r="99" ht="87.0" customHeight="1">
       <c r="A99" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="B99" s="1" t="s">
+      <c r="B99" s="3" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="100" ht="14.25" customHeight="1">
+    <row r="100" ht="87.0" customHeight="1">
       <c r="A100" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="B100" s="1" t="s">
+      <c r="B100" s="3" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="101" ht="14.25" customHeight="1">
+    <row r="101" ht="87.0" customHeight="1">
       <c r="A101" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="B101" s="1" t="s">
+      <c r="B101" s="3" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="102" ht="14.25" customHeight="1">
+    <row r="102" ht="87.0" customHeight="1">
       <c r="A102" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="B102" s="1" t="s">
+      <c r="B102" s="3" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="103" ht="14.25" customHeight="1">
+    <row r="103" ht="87.0" customHeight="1">
       <c r="A103" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="B103" s="1" t="s">
+      <c r="B103" s="3" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="104" ht="14.25" customHeight="1">
+    <row r="104" ht="87.0" customHeight="1">
       <c r="A104" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="B104" s="1" t="s">
+      <c r="B104" s="3" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="105" ht="14.25" customHeight="1">
+    <row r="105" ht="87.0" customHeight="1">
       <c r="A105" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="B105" s="1" t="s">
+      <c r="B105" s="3" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="106" ht="14.25" customHeight="1">
+    <row r="106" ht="87.0" customHeight="1">
       <c r="A106" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="B106" s="1" t="s">
+      <c r="B106" s="3" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="107" ht="14.25" customHeight="1">
+    <row r="107" ht="87.0" customHeight="1">
       <c r="A107" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B107" s="1" t="s">
+      <c r="B107" s="3" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="108" ht="14.25" customHeight="1">
+    <row r="108" ht="87.0" customHeight="1">
       <c r="A108" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="B108" s="1" t="s">
+      <c r="B108" s="3" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="109" ht="14.25" customHeight="1">
+    <row r="109" ht="87.0" customHeight="1">
       <c r="A109" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="B109" s="1" t="s">
+      <c r="B109" s="3" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="110" ht="14.25" customHeight="1">
+    <row r="110" ht="87.0" customHeight="1">
       <c r="A110" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="B110" s="1" t="s">
+      <c r="B110" s="3" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="111" ht="14.25" customHeight="1">
+    <row r="111" ht="87.0" customHeight="1">
       <c r="A111" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="B111" s="1" t="s">
+      <c r="B111" s="3" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="112" ht="14.25" customHeight="1">
+    <row r="112" ht="87.0" customHeight="1">
       <c r="A112" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="B112" s="1" t="s">
+      <c r="B112" s="3" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="113" ht="14.25" customHeight="1">
+    <row r="113" ht="87.0" customHeight="1">
       <c r="A113" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="B113" s="1" t="s">
+      <c r="B113" s="3" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="114" ht="14.25" customHeight="1">
+    <row r="114" ht="87.0" customHeight="1">
       <c r="A114" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="B114" s="1" t="s">
+      <c r="B114" s="3" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="115" ht="14.25" customHeight="1">
+    <row r="115" ht="87.0" customHeight="1">
       <c r="A115" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="B115" s="1" t="s">
+      <c r="B115" s="3" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="116" ht="14.25" customHeight="1">
+    <row r="116" ht="87.0" customHeight="1">
       <c r="A116" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="B116" s="1" t="s">
+      <c r="B116" s="3" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="117" ht="14.25" customHeight="1">
+    <row r="117" ht="87.0" customHeight="1">
       <c r="A117" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="B117" s="1" t="s">
+      <c r="B117" s="3" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="118" ht="14.25" customHeight="1">
+    <row r="118" ht="87.0" customHeight="1">
       <c r="A118" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="B118" s="1" t="s">
+      <c r="B118" s="3" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="119" ht="14.25" customHeight="1">
+    <row r="119" ht="87.0" customHeight="1">
       <c r="A119" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="B119" s="1" t="s">
+      <c r="B119" s="3" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="120" ht="14.25" customHeight="1">
+    <row r="120" ht="87.0" customHeight="1">
       <c r="A120" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="B120" s="1" t="s">
+      <c r="B120" s="3" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="121" ht="14.25" customHeight="1">
-      <c r="A121" s="3" t="s">
+    <row r="121" ht="87.0" customHeight="1">
+      <c r="A121" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="B121" s="1" t="s">
+      <c r="B121" s="3" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="122" ht="14.25" customHeight="1">
-      <c r="A122" s="3" t="s">
+    <row r="122" ht="87.0" customHeight="1">
+      <c r="A122" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="B122" s="1" t="s">
+      <c r="B122" s="3" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="123" ht="14.25" customHeight="1">
-      <c r="A123" s="3" t="s">
+    <row r="123" ht="87.0" customHeight="1">
+      <c r="A123" s="5" t="s">
         <v>244</v>
       </c>
-      <c r="B123" s="1" t="s">
+      <c r="B123" s="3" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="124" ht="14.25" customHeight="1">
-      <c r="A124" s="3" t="s">
+    <row r="124" ht="87.0" customHeight="1">
+      <c r="A124" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="B124" s="1" t="s">
+      <c r="B124" s="3" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="125" ht="14.25" customHeight="1">
-      <c r="A125" s="3" t="s">
+    <row r="125" ht="87.0" customHeight="1">
+      <c r="A125" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="B125" s="1" t="s">
+      <c r="B125" s="3" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="126" ht="14.25" customHeight="1">
-      <c r="A126" s="3" t="s">
+    <row r="126" ht="87.0" customHeight="1">
+      <c r="A126" s="5" t="s">
         <v>250</v>
       </c>
-      <c r="B126" s="1" t="s">
+      <c r="B126" s="3" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="127" ht="14.25" customHeight="1">
+    <row r="127" ht="87.0" customHeight="1">
       <c r="A127" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="B127" s="1" t="s">
+      <c r="B127" s="3" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="128" ht="14.25" customHeight="1">
-      <c r="A128" s="3" t="s">
+    <row r="128" ht="87.0" customHeight="1">
+      <c r="A128" s="5" t="s">
         <v>254</v>
       </c>
-      <c r="B128" s="1" t="s">
+      <c r="B128" s="3" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="129" ht="14.25" customHeight="1">
-      <c r="A129" s="3" t="s">
+    <row r="129" ht="87.0" customHeight="1">
+      <c r="A129" s="5" t="s">
         <v>256</v>
       </c>
-      <c r="B129" s="1" t="s">
+      <c r="B129" s="3" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="130" ht="14.25" customHeight="1">
-      <c r="A130" s="3" t="s">
+    <row r="130" ht="87.0" customHeight="1">
+      <c r="A130" s="5" t="s">
         <v>258</v>
       </c>
-      <c r="B130" s="1" t="s">
+      <c r="B130" s="3" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="131" ht="14.25" customHeight="1">
-      <c r="A131" s="3" t="s">
+    <row r="131" ht="87.0" customHeight="1">
+      <c r="A131" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="B131" s="1" t="s">
+      <c r="B131" s="3" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="132" ht="14.25" customHeight="1">
-      <c r="A132" s="3" t="s">
+    <row r="132" ht="87.0" customHeight="1">
+      <c r="A132" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="B132" s="1" t="s">
+      <c r="B132" s="3" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="133" ht="14.25" customHeight="1">
-      <c r="A133" s="3" t="s">
+    <row r="133" ht="87.0" customHeight="1">
+      <c r="A133" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="B133" s="1" t="s">
+      <c r="B133" s="3" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="134" ht="14.25" customHeight="1">
-      <c r="A134" s="3" t="s">
+    <row r="134" ht="87.0" customHeight="1">
+      <c r="A134" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="B134" s="1" t="s">
+      <c r="B134" s="3" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="135" ht="14.25" customHeight="1">
-      <c r="A135" s="3" t="s">
+    <row r="135" ht="87.0" customHeight="1">
+      <c r="A135" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="B135" s="1" t="s">
+      <c r="B135" s="3" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="136" ht="14.25" customHeight="1">
-      <c r="A136" s="3" t="s">
+    <row r="136" ht="87.0" customHeight="1">
+      <c r="A136" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="B136" s="1" t="s">
+      <c r="B136" s="3" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="137" ht="14.25" customHeight="1">
-      <c r="A137" s="3" t="s">
+    <row r="137" ht="87.0" customHeight="1">
+      <c r="A137" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="B137" s="1" t="s">
+      <c r="B137" s="3" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="138" ht="14.25" customHeight="1">
-      <c r="A138" s="3" t="s">
+    <row r="138" ht="87.0" customHeight="1">
+      <c r="A138" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="B138" s="1" t="s">
+      <c r="B138" s="3" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="139" ht="14.25" customHeight="1">
-      <c r="A139" s="3" t="s">
+    <row r="139" ht="87.0" customHeight="1">
+      <c r="A139" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="B139" s="1" t="s">
+      <c r="B139" s="3" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="140" ht="14.25" customHeight="1">
-      <c r="A140" s="3" t="s">
+    <row r="140" ht="87.0" customHeight="1">
+      <c r="A140" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="B140" s="1" t="s">
+      <c r="B140" s="3" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="141" ht="14.25" customHeight="1">
-      <c r="A141" s="3" t="s">
+    <row r="141" ht="87.0" customHeight="1">
+      <c r="A141" s="5" t="s">
         <v>280</v>
       </c>
-      <c r="B141" s="1" t="s">
+      <c r="B141" s="3" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="142" ht="14.25" customHeight="1">
-      <c r="A142" s="3" t="s">
+    <row r="142" ht="87.0" customHeight="1">
+      <c r="A142" s="5" t="s">
         <v>282</v>
       </c>
-      <c r="B142" s="1" t="s">
+      <c r="B142" s="3" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="143" ht="14.25" customHeight="1">
-      <c r="A143" s="3" t="s">
+    <row r="143" ht="87.0" customHeight="1">
+      <c r="A143" s="5" t="s">
         <v>284</v>
       </c>
-      <c r="B143" s="1" t="s">
+      <c r="B143" s="3" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="144" ht="14.25" customHeight="1">
-      <c r="A144" s="3" t="s">
+    <row r="144" ht="87.0" customHeight="1">
+      <c r="A144" s="5" t="s">
         <v>286</v>
       </c>
-      <c r="B144" s="1" t="s">
+      <c r="B144" s="3" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="145" ht="14.25" customHeight="1">
+    <row r="145" ht="87.0" customHeight="1">
       <c r="A145" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="B145" s="1" t="s">
+      <c r="B145" s="3" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="146" ht="14.25" customHeight="1">
+    <row r="146" ht="87.0" customHeight="1">
       <c r="A146" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="B146" s="1" t="s">
+      <c r="B146" s="3" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="147" ht="14.25" customHeight="1">
+    <row r="147" ht="87.0" customHeight="1">
       <c r="A147" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="B147" s="1" t="s">
+      <c r="B147" s="3" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="148" ht="14.25" customHeight="1">
+    <row r="148" ht="87.0" customHeight="1">
       <c r="A148" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="B148" s="1" t="s">
+      <c r="B148" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="149" ht="14.25" customHeight="1">
+    <row r="149" ht="87.0" customHeight="1">
       <c r="A149" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="B149" s="1" t="s">
+      <c r="B149" s="3" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="150" ht="14.25" customHeight="1">
+    <row r="150" ht="87.0" customHeight="1">
       <c r="A150" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="B150" s="1" t="s">
+      <c r="B150" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="151" ht="14.25" customHeight="1">
+    <row r="151" ht="87.0" customHeight="1">
       <c r="A151" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="B151" s="1" t="s">
+      <c r="B151" s="3" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="152" ht="14.25" customHeight="1">
+    <row r="152" ht="87.0" customHeight="1">
       <c r="A152" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="B152" s="1" t="s">
+      <c r="B152" s="3" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="153" ht="14.25" customHeight="1">
+    <row r="153" ht="87.0" customHeight="1">
       <c r="A153" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="B153" s="1" t="s">
+      <c r="B153" s="3" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="154" ht="14.25" customHeight="1">
+    <row r="154" ht="87.0" customHeight="1">
       <c r="A154" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="B154" s="1" t="s">
+      <c r="B154" s="3" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="155" ht="14.25" customHeight="1">
+    <row r="155" ht="87.0" customHeight="1">
       <c r="A155" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="B155" s="1" t="s">
+      <c r="B155" s="3" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="156" ht="14.25" customHeight="1">
+    <row r="156" ht="87.0" customHeight="1">
       <c r="A156" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="B156" s="1" t="s">
+      <c r="B156" s="3" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="157" ht="14.25" customHeight="1">
+    <row r="157" ht="87.0" customHeight="1">
       <c r="A157" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="B157" s="1" t="s">
+      <c r="B157" s="3" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="158" ht="14.25" customHeight="1">
+    <row r="158" ht="87.0" customHeight="1">
       <c r="A158" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="B158" s="1" t="s">
+      <c r="B158" s="3" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="159" ht="14.25" customHeight="1">
+    <row r="159" ht="87.0" customHeight="1">
       <c r="A159" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="B159" s="1" t="s">
+      <c r="B159" s="3" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="160" ht="14.25" customHeight="1">
+    <row r="160" ht="87.0" customHeight="1">
       <c r="A160" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="B160" s="1" t="s">
+      <c r="B160" s="3" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="161" ht="14.25" customHeight="1">
+    <row r="161" ht="87.0" customHeight="1">
       <c r="A161" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="B161" s="1" t="s">
+      <c r="B161" s="3" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="162" ht="14.25" customHeight="1">
+    <row r="162" ht="87.0" customHeight="1">
       <c r="A162" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="B162" s="1" t="s">
+      <c r="B162" s="3" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="163" ht="14.25" customHeight="1">
+    <row r="163" ht="87.0" customHeight="1">
       <c r="A163" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="B163" s="1" t="s">
+      <c r="B163" s="3" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="164" ht="14.25" customHeight="1">
+    <row r="164" ht="87.0" customHeight="1">
       <c r="A164" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="B164" s="1" t="s">
+      <c r="B164" s="3" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="165" ht="14.25" customHeight="1">
+    <row r="165" ht="87.0" customHeight="1">
       <c r="A165" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="B165" s="1" t="s">
+      <c r="B165" s="3" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="166" ht="14.25" customHeight="1">
+    <row r="166" ht="87.0" customHeight="1">
       <c r="A166" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="B166" s="1" t="s">
+      <c r="B166" s="3" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="167" ht="14.25" customHeight="1">
+    <row r="167" ht="87.0" customHeight="1">
       <c r="A167" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="B167" s="1" t="s">
+      <c r="B167" s="3" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="168" ht="14.25" customHeight="1">
+    <row r="168" ht="87.0" customHeight="1">
       <c r="A168" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="B168" s="1" t="s">
+      <c r="B168" s="3" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="169" ht="14.25" customHeight="1">
+    <row r="169" ht="87.0" customHeight="1">
       <c r="A169" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="B169" s="1" t="s">
+      <c r="B169" s="3" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="170" ht="14.25" customHeight="1">
+    <row r="170" ht="87.0" customHeight="1">
       <c r="A170" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="B170" s="1" t="s">
+      <c r="B170" s="3" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="171" ht="14.25" customHeight="1">
+    <row r="171" ht="87.0" customHeight="1">
       <c r="A171" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="B171" s="1" t="s">
+      <c r="B171" s="3" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="172" ht="14.25" customHeight="1">
+    <row r="172" ht="87.0" customHeight="1">
       <c r="A172" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="B172" s="1" t="s">
+      <c r="B172" s="3" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="173" ht="14.25" customHeight="1">
+    <row r="173" ht="87.0" customHeight="1">
       <c r="A173" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="B173" s="1" t="s">
+      <c r="B173" s="3" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="174" ht="14.25" customHeight="1">
+    <row r="174" ht="87.0" customHeight="1">
       <c r="A174" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="B174" s="1" t="s">
+      <c r="B174" s="3" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="175" ht="14.25" customHeight="1">
+    <row r="175" ht="87.0" customHeight="1">
       <c r="A175" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="B175" s="1" t="s">
+      <c r="B175" s="3" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="176" ht="14.25" customHeight="1">
+    <row r="176" ht="87.0" customHeight="1">
       <c r="A176" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="B176" s="1" t="s">
+      <c r="B176" s="3" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="177" ht="14.25" customHeight="1">
+    <row r="177" ht="87.0" customHeight="1">
       <c r="A177" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="B177" s="1" t="s">
+      <c r="B177" s="3" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="178" ht="14.25" customHeight="1">
+    <row r="178" ht="87.0" customHeight="1">
       <c r="A178" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="B178" s="1" t="s">
+      <c r="B178" s="3" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="179" ht="14.25" customHeight="1">
+    <row r="179" ht="87.0" customHeight="1">
       <c r="A179" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="B179" s="1" t="s">
+      <c r="B179" s="3" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="180" ht="14.25" customHeight="1">
+    <row r="180" ht="87.0" customHeight="1">
       <c r="A180" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="B180" s="1" t="s">
+      <c r="B180" s="3" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="181" ht="14.25" customHeight="1">
+    <row r="181" ht="87.0" customHeight="1">
       <c r="A181" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="B181" s="1" t="s">
+      <c r="B181" s="3" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="182" ht="14.25" customHeight="1">
+    <row r="182" ht="87.0" customHeight="1">
       <c r="A182" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="B182" s="1" t="s">
+      <c r="B182" s="3" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="183" ht="14.25" customHeight="1">
+    <row r="183" ht="87.0" customHeight="1">
       <c r="A183" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="B183" s="1" t="s">
+      <c r="B183" s="3" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="184" ht="14.25" customHeight="1">
+    <row r="184" ht="87.0" customHeight="1">
       <c r="A184" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="B184" s="1" t="s">
+      <c r="B184" s="3" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="185" ht="14.25" customHeight="1">
+    <row r="185" ht="87.0" customHeight="1">
       <c r="A185" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="B185" s="1" t="s">
+      <c r="B185" s="3" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="186" ht="14.25" customHeight="1">
+    <row r="186" ht="87.0" customHeight="1">
       <c r="A186" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="B186" s="1" t="s">
+      <c r="B186" s="3" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="187" ht="14.25" customHeight="1">
+    <row r="187" ht="87.0" customHeight="1">
       <c r="A187" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="B187" s="1" t="s">
+      <c r="B187" s="3" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="188" ht="14.25" customHeight="1">
+    <row r="188" ht="87.0" customHeight="1">
       <c r="A188" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="B188" s="1" t="s">
+      <c r="B188" s="3" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="189" ht="14.25" customHeight="1">
+    <row r="189" ht="87.0" customHeight="1">
       <c r="A189" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="B189" s="1" t="s">
+      <c r="B189" s="3" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="190" ht="14.25" customHeight="1">
+    <row r="190" ht="87.0" customHeight="1">
       <c r="A190" s="1" t="s">
         <v>376</v>
       </c>
-      <c r="B190" s="1" t="s">
+      <c r="B190" s="3" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="191" ht="14.25" customHeight="1">
+    <row r="191" ht="87.0" customHeight="1">
       <c r="A191" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="B191" s="1" t="s">
+      <c r="B191" s="3" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="192" ht="14.25" customHeight="1">
+    <row r="192" ht="87.0" customHeight="1">
       <c r="A192" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="B192" s="1" t="s">
+      <c r="B192" s="3" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="193" ht="14.25" customHeight="1">
+    <row r="193" ht="87.0" customHeight="1">
       <c r="A193" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="B193" s="1" t="s">
+      <c r="B193" s="3" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="194" ht="14.25" customHeight="1">
+    <row r="194" ht="87.0" customHeight="1">
       <c r="A194" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="B194" s="1" t="s">
+      <c r="B194" s="3" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="195" ht="14.25" customHeight="1">
+    <row r="195" ht="87.0" customHeight="1">
       <c r="A195" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="B195" s="1" t="s">
+      <c r="B195" s="3" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="196" ht="14.25" customHeight="1">
+    <row r="196" ht="87.0" customHeight="1">
       <c r="A196" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="B196" s="1" t="s">
+      <c r="B196" s="3" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="197" ht="14.25" customHeight="1">
+    <row r="197" ht="87.0" customHeight="1">
       <c r="A197" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="B197" s="1" t="s">
+      <c r="B197" s="3" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="198" ht="14.25" customHeight="1">
+    <row r="198" ht="87.0" customHeight="1">
       <c r="A198" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="B198" s="1" t="s">
+      <c r="B198" s="3" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="199" ht="14.25" customHeight="1">
+    <row r="199" ht="87.0" customHeight="1">
       <c r="A199" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="B199" s="1" t="s">
+      <c r="B199" s="3" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="200" ht="14.25" customHeight="1">
+    <row r="200" ht="87.0" customHeight="1">
       <c r="A200" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="B200" s="1" t="s">
+      <c r="B200" s="3" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="201" ht="14.25" customHeight="1">
+    <row r="201" ht="87.0" customHeight="1">
       <c r="A201" s="1" t="s">
         <v>398</v>
       </c>
-      <c r="B201" s="1" t="s">
+      <c r="B201" s="3" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="202" ht="14.25" customHeight="1">
+    <row r="202" ht="87.0" customHeight="1">
       <c r="A202" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="B202" s="1" t="s">
+      <c r="B202" s="3" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="203" ht="14.25" customHeight="1">
+    <row r="203" ht="87.0" customHeight="1">
       <c r="A203" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="B203" s="1" t="s">
+      <c r="B203" s="3" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="204" ht="14.25" customHeight="1">
+    <row r="204" ht="87.0" customHeight="1">
       <c r="A204" s="1" t="s">
         <v>404</v>
       </c>
-      <c r="B204" s="1" t="s">
+      <c r="B204" s="3" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="205" ht="14.25" customHeight="1">
+    <row r="205" ht="87.0" customHeight="1">
       <c r="A205" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="B205" s="1" t="s">
+      <c r="B205" s="3" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="206" ht="14.25" customHeight="1">
+    <row r="206" ht="87.0" customHeight="1">
       <c r="A206" s="1" t="s">
         <v>408</v>
       </c>
-      <c r="B206" s="1" t="s">
+      <c r="B206" s="3" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="207" ht="14.25" customHeight="1">
+    <row r="207" ht="87.0" customHeight="1">
       <c r="A207" s="1" t="s">
         <v>410</v>
       </c>
-      <c r="B207" s="1" t="s">
+      <c r="B207" s="3" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="208" ht="14.25" customHeight="1">
+    <row r="208" ht="87.0" customHeight="1">
       <c r="A208" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="B208" s="1" t="s">
+      <c r="B208" s="3" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="209" ht="14.25" customHeight="1">
+    <row r="209" ht="87.0" customHeight="1">
       <c r="A209" s="1" t="s">
         <v>414</v>
       </c>
-      <c r="B209" s="1" t="s">
+      <c r="B209" s="3" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="210" ht="14.25" customHeight="1">
+    <row r="210" ht="87.0" customHeight="1">
       <c r="A210" s="1" t="s">
         <v>416</v>
       </c>
-      <c r="B210" s="1" t="s">
+      <c r="B210" s="3" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="211" ht="14.25" customHeight="1">
+    <row r="211" ht="87.0" customHeight="1">
       <c r="A211" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="B211" s="1" t="s">
+      <c r="B211" s="3" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="212" ht="14.25" customHeight="1">
+    <row r="212" ht="87.0" customHeight="1">
       <c r="A212" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="B212" s="1" t="s">
+      <c r="B212" s="3" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="213" ht="14.25" customHeight="1">
+    <row r="213" ht="87.0" customHeight="1">
       <c r="A213" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="B213" s="1" t="s">
+      <c r="B213" s="3" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="214" ht="14.25" customHeight="1">
+    <row r="214" ht="87.0" customHeight="1">
       <c r="A214" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="B214" s="1" t="s">
+      <c r="B214" s="3" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="215" ht="14.25" customHeight="1">
+    <row r="215" ht="87.0" customHeight="1">
       <c r="A215" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="B215" s="1" t="s">
+      <c r="B215" s="3" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="216" ht="14.25" customHeight="1">
+    <row r="216" ht="87.0" customHeight="1">
       <c r="A216" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="B216" s="1" t="s">
+      <c r="B216" s="3" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="217" ht="14.25" customHeight="1">
+    <row r="217" ht="87.0" customHeight="1">
       <c r="A217" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="B217" s="1" t="s">
+      <c r="B217" s="3" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="218" ht="14.25" customHeight="1">
+    <row r="218" ht="87.0" customHeight="1">
       <c r="A218" s="1" t="s">
         <v>431</v>
       </c>
-      <c r="B218" s="1" t="s">
+      <c r="B218" s="3" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="219" ht="14.25" customHeight="1">
+    <row r="219" ht="87.0" customHeight="1">
       <c r="A219" s="1" t="s">
         <v>433</v>
       </c>
-      <c r="B219" s="1" t="s">
+      <c r="B219" s="3" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="220" ht="14.25" customHeight="1">
+    <row r="220" ht="87.0" customHeight="1">
       <c r="A220" s="1" t="s">
         <v>435</v>
       </c>
-      <c r="B220" s="1" t="s">
+      <c r="B220" s="3" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="221" ht="14.25" customHeight="1">
+    <row r="221" ht="87.0" customHeight="1">
       <c r="A221" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="B221" s="1" t="s">
+      <c r="B221" s="3" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="222" ht="14.25" customHeight="1">
+    <row r="222" ht="87.0" customHeight="1">
       <c r="A222" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="B222" s="1" t="s">
+      <c r="B222" s="3" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="223" ht="14.25" customHeight="1">
+    <row r="223" ht="87.0" customHeight="1">
       <c r="A223" s="1" t="s">
         <v>441</v>
       </c>
-      <c r="B223" s="1" t="s">
+      <c r="B223" s="3" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="224" ht="14.25" customHeight="1">
+    <row r="224" ht="87.0" customHeight="1">
       <c r="A224" s="1" t="s">
         <v>443</v>
       </c>
-      <c r="B224" s="1" t="s">
+      <c r="B224" s="3" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="225" ht="14.25" customHeight="1">
+    <row r="225" ht="87.0" customHeight="1">
       <c r="A225" s="1" t="s">
         <v>445</v>
       </c>
-      <c r="B225" s="1" t="s">
+      <c r="B225" s="3" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="226" ht="14.25" customHeight="1">
+    <row r="226" ht="87.0" customHeight="1">
       <c r="A226" s="1" t="s">
         <v>447</v>
       </c>
-      <c r="B226" s="1" t="s">
+      <c r="B226" s="3" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="227" ht="14.25" customHeight="1">
+    <row r="227" ht="87.0" customHeight="1">
       <c r="A227" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="B227" s="1" t="s">
+      <c r="B227" s="3" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="228" ht="14.25" customHeight="1">
+    <row r="228" ht="87.0" customHeight="1">
       <c r="A228" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="B228" s="1" t="s">
+      <c r="B228" s="3" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="229" ht="14.25" customHeight="1">
+    <row r="229" ht="87.0" customHeight="1">
       <c r="A229" s="1" t="s">
         <v>453</v>
       </c>
-      <c r="B229" s="1" t="s">
+      <c r="B229" s="3" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="230" ht="14.25" customHeight="1">
+    <row r="230" ht="87.0" customHeight="1">
       <c r="A230" s="1" t="s">
         <v>455</v>
       </c>
-      <c r="B230" s="1" t="s">
+      <c r="B230" s="3" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="231" ht="14.25" customHeight="1">
+    <row r="231" ht="87.0" customHeight="1">
       <c r="A231" s="1" t="s">
         <v>457</v>
       </c>
-      <c r="B231" s="1" t="s">
+      <c r="B231" s="3" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="232" ht="14.25" customHeight="1">
+    <row r="232" ht="87.0" customHeight="1">
       <c r="A232" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="B232" s="1" t="s">
+      <c r="B232" s="3" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="233" ht="14.25" customHeight="1">
+    <row r="233" ht="87.0" customHeight="1">
       <c r="A233" s="1" t="s">
         <v>461</v>
       </c>
-      <c r="B233" s="1" t="s">
+      <c r="B233" s="3" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="234" ht="14.25" customHeight="1">
+    <row r="234" ht="87.0" customHeight="1">
       <c r="A234" s="1" t="s">
         <v>463</v>
       </c>
-      <c r="B234" s="1" t="s">
+      <c r="B234" s="3" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="235" ht="14.25" customHeight="1">
+    <row r="235" ht="87.0" customHeight="1">
       <c r="A235" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="B235" s="1" t="s">
+      <c r="B235" s="3" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="236" ht="14.25" customHeight="1">
+    <row r="236" ht="87.0" customHeight="1">
       <c r="A236" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="B236" s="1" t="s">
+      <c r="B236" s="3" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="237" ht="14.25" customHeight="1">
+    <row r="237" ht="87.0" customHeight="1">
       <c r="A237" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="B237" s="1" t="s">
+      <c r="B237" s="3" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="238" ht="14.25" customHeight="1">
+    <row r="238" ht="87.0" customHeight="1">
       <c r="A238" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="B238" s="1" t="s">
+      <c r="B238" s="3" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="239" ht="14.25" customHeight="1">
+    <row r="239" ht="87.0" customHeight="1">
       <c r="A239" s="1" t="s">
         <v>472</v>
       </c>
-      <c r="B239" s="1" t="s">
+      <c r="B239" s="3" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="240" ht="14.25" customHeight="1">
+    <row r="240" ht="87.0" customHeight="1">
       <c r="A240" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="B240" s="1" t="s">
+      <c r="B240" s="3" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="241" ht="14.25" customHeight="1">
+    <row r="241" ht="87.0" customHeight="1">
       <c r="A241" s="1" t="s">
         <v>476</v>
       </c>
-      <c r="B241" s="1" t="s">
+      <c r="B241" s="3" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="242" ht="14.25" customHeight="1">
+    <row r="242" ht="87.0" customHeight="1">
       <c r="A242" s="1" t="s">
         <v>478</v>
       </c>
-      <c r="B242" s="1" t="s">
+      <c r="B242" s="3" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="243" ht="14.25" customHeight="1">
+    <row r="243" ht="87.0" customHeight="1">
       <c r="A243" s="1" t="s">
         <v>480</v>
       </c>
-      <c r="B243" s="1" t="s">
+      <c r="B243" s="3" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="244" ht="14.25" customHeight="1">
+    <row r="244" ht="87.0" customHeight="1">
       <c r="A244" s="1" t="s">
         <v>482</v>
       </c>
-      <c r="B244" s="1" t="s">
+      <c r="B244" s="3" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="245" ht="14.25" customHeight="1">
+    <row r="245" ht="87.0" customHeight="1">
       <c r="A245" s="1" t="s">
         <v>484</v>
       </c>
-      <c r="B245" s="1" t="s">
+      <c r="B245" s="3" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="246" ht="14.25" customHeight="1">
+    <row r="246" ht="87.0" customHeight="1">
       <c r="A246" s="1" t="s">
         <v>486</v>
       </c>
-      <c r="B246" s="1" t="s">
+      <c r="B246" s="3" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="247" ht="14.25" customHeight="1">
+    <row r="247" ht="87.0" customHeight="1">
       <c r="A247" s="1" t="s">
         <v>488</v>
       </c>
-      <c r="B247" s="1" t="s">
+      <c r="B247" s="3" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="248" ht="14.25" customHeight="1">
+    <row r="248" ht="87.0" customHeight="1">
       <c r="A248" s="1" t="s">
         <v>490</v>
       </c>
-      <c r="B248" s="1" t="s">
+      <c r="B248" s="3" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="249" ht="14.25" customHeight="1">
+    <row r="249" ht="87.0" customHeight="1">
       <c r="A249" s="1" t="s">
         <v>492</v>
       </c>
-      <c r="B249" s="1" t="s">
+      <c r="B249" s="3" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="250" ht="14.25" customHeight="1">
+    <row r="250" ht="87.0" customHeight="1">
       <c r="A250" s="1" t="s">
         <v>494</v>
       </c>
-      <c r="B250" s="1" t="s">
+      <c r="B250" s="3" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="251" ht="14.25" customHeight="1">
+    <row r="251" ht="87.0" customHeight="1">
       <c r="A251" s="1" t="s">
         <v>496</v>
       </c>
-      <c r="B251" s="1" t="s">
+      <c r="B251" s="3" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="252" ht="14.25" customHeight="1">
+    <row r="252" ht="87.0" customHeight="1">
       <c r="A252" s="1" t="s">
         <v>498</v>
       </c>
-      <c r="B252" s="1" t="s">
+      <c r="B252" s="3" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="253" ht="14.25" customHeight="1">
+    <row r="253" ht="87.0" customHeight="1">
       <c r="A253" s="1" t="s">
         <v>500</v>
       </c>
-      <c r="B253" s="1" t="s">
+      <c r="B253" s="3" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="254" ht="14.25" customHeight="1">
+    <row r="254" ht="87.0" customHeight="1">
       <c r="A254" s="1" t="s">
         <v>502</v>
       </c>
-      <c r="B254" s="1" t="s">
+      <c r="B254" s="3" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="255" ht="14.25" customHeight="1">
+    <row r="255" ht="87.0" customHeight="1">
       <c r="A255" s="1" t="s">
         <v>504</v>
       </c>
-      <c r="B255" s="1" t="s">
+      <c r="B255" s="3" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="256" ht="14.25" customHeight="1">
+    <row r="256" ht="87.0" customHeight="1">
       <c r="A256" s="1" t="s">
         <v>506</v>
       </c>
-      <c r="B256" s="1" t="s">
+      <c r="B256" s="3" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="257" ht="14.25" customHeight="1">
+    <row r="257" ht="87.0" customHeight="1">
       <c r="A257" s="1" t="s">
         <v>508</v>
       </c>
-      <c r="B257" s="1" t="s">
+      <c r="B257" s="3" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="258" ht="14.25" customHeight="1">
-      <c r="A258" s="4" t="s">
+    <row r="258" ht="87.0" customHeight="1">
+      <c r="A258" s="6" t="s">
         <v>510</v>
       </c>
-      <c r="B258" s="1" t="s">
+      <c r="B258" s="3" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="259" ht="14.25" customHeight="1">
+    <row r="259" ht="87.0" customHeight="1">
       <c r="A259" s="1" t="s">
         <v>512</v>
       </c>
-      <c r="B259" s="1" t="s">
+      <c r="B259" s="3" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="260" ht="14.25" customHeight="1">
+    <row r="260" ht="87.0" customHeight="1">
       <c r="A260" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="B260" s="1" t="s">
+      <c r="B260" s="3" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="261" ht="14.25" customHeight="1">
+    <row r="261" ht="87.0" customHeight="1">
       <c r="A261" s="1" t="s">
         <v>516</v>
       </c>
-      <c r="B261" s="1" t="s">
+      <c r="B261" s="3" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="262" ht="14.25" customHeight="1">
+    <row r="262" ht="87.0" customHeight="1">
       <c r="A262" s="1" t="s">
         <v>484</v>
       </c>
-      <c r="B262" s="1" t="s">
+      <c r="B262" s="3" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="263" ht="14.25" customHeight="1">
+    <row r="263" ht="87.0" customHeight="1">
       <c r="A263" s="1" t="s">
         <v>519</v>
       </c>
-      <c r="B263" s="1" t="s">
+      <c r="B263" s="3" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="264" ht="14.25" customHeight="1">
+    <row r="264" ht="87.0" customHeight="1">
       <c r="A264" s="1" t="s">
         <v>521</v>
       </c>
-      <c r="B264" s="1" t="s">
+      <c r="B264" s="3" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="265" ht="14.25" customHeight="1">
-      <c r="A265" s="5" t="s">
+    <row r="265" ht="87.0" customHeight="1">
+      <c r="A265" s="7" t="s">
         <v>523</v>
       </c>
-      <c r="B265" s="6" t="s">
+      <c r="B265" s="8" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="266" ht="14.25" customHeight="1">
-      <c r="A266" s="7" t="s">
+    <row r="266" ht="87.0" customHeight="1">
+      <c r="A266" s="9" t="s">
         <v>525</v>
       </c>
-      <c r="B266" s="8" t="s">
+      <c r="B266" s="10" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="267" ht="14.25" customHeight="1">
-      <c r="A267" s="7" t="s">
+    <row r="267" ht="87.0" customHeight="1">
+      <c r="A267" s="9" t="s">
         <v>527</v>
       </c>
-      <c r="B267" s="8" t="s">
+      <c r="B267" s="10" t="s">
         <v>528</v>
       </c>
     </row>
-    <row r="268" ht="14.25" customHeight="1">
-      <c r="A268" s="7" t="s">
+    <row r="268" ht="87.0" customHeight="1">
+      <c r="A268" s="9" t="s">
         <v>529</v>
       </c>
-      <c r="B268" s="8" t="s">
+      <c r="B268" s="10" t="s">
         <v>530</v>
       </c>
     </row>
-    <row r="269" ht="14.25" customHeight="1">
-      <c r="A269" s="7" t="s">
+    <row r="269" ht="87.0" customHeight="1">
+      <c r="A269" s="9" t="s">
         <v>531</v>
       </c>
-      <c r="B269" s="8" t="s">
+      <c r="B269" s="10" t="s">
         <v>532</v>
       </c>
     </row>
-    <row r="270" ht="14.25" customHeight="1">
-      <c r="A270" s="7" t="s">
+    <row r="270" ht="87.0" customHeight="1">
+      <c r="A270" s="9" t="s">
         <v>533</v>
       </c>
-      <c r="B270" s="8" t="s">
+      <c r="B270" s="10" t="s">
         <v>534</v>
       </c>
     </row>
-    <row r="271" ht="14.25" customHeight="1">
-      <c r="A271" s="9" t="s">
+    <row r="271" ht="87.0" customHeight="1">
+      <c r="A271" s="11" t="s">
         <v>535</v>
       </c>
-      <c r="B271" s="8" t="s">
+      <c r="B271" s="10" t="s">
         <v>536</v>
       </c>
     </row>
-    <row r="272" ht="14.25" customHeight="1">
-      <c r="A272" s="7" t="s">
+    <row r="272" ht="87.0" customHeight="1">
+      <c r="A272" s="9" t="s">
         <v>537</v>
       </c>
-      <c r="B272" s="8" t="s">
+      <c r="B272" s="10" t="s">
         <v>538</v>
       </c>
     </row>
-    <row r="273" ht="14.25" customHeight="1">
-      <c r="A273" s="7" t="s">
+    <row r="273" ht="87.0" customHeight="1">
+      <c r="A273" s="9" t="s">
         <v>539</v>
       </c>
-      <c r="B273" s="8" t="s">
+      <c r="B273" s="10" t="s">
         <v>540</v>
       </c>
     </row>
-    <row r="274" ht="14.25" customHeight="1">
-      <c r="A274" s="7" t="s">
+    <row r="274" ht="87.0" customHeight="1">
+      <c r="A274" s="9" t="s">
         <v>541</v>
       </c>
-      <c r="B274" s="8" t="s">
+      <c r="B274" s="10" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="275" ht="14.25" customHeight="1">
-      <c r="A275" s="7" t="s">
+    <row r="275" ht="87.0" customHeight="1">
+      <c r="A275" s="9" t="s">
         <v>543</v>
       </c>
-      <c r="B275" s="8" t="s">
+      <c r="B275" s="10" t="s">
         <v>544</v>
       </c>
     </row>
-    <row r="276" ht="14.25" customHeight="1">
-      <c r="A276" s="7" t="s">
+    <row r="276" ht="87.0" customHeight="1">
+      <c r="A276" s="9" t="s">
         <v>545</v>
       </c>
-      <c r="B276" s="8" t="s">
+      <c r="B276" s="10" t="s">
         <v>546</v>
       </c>
     </row>
-    <row r="277" ht="14.25" customHeight="1">
-      <c r="A277" s="7" t="s">
+    <row r="277" ht="87.0" customHeight="1">
+      <c r="A277" s="9" t="s">
         <v>547</v>
       </c>
-      <c r="B277" s="8" t="s">
+      <c r="B277" s="10" t="s">
         <v>548</v>
       </c>
     </row>
-    <row r="278" ht="14.25" customHeight="1">
-      <c r="A278" s="7" t="s">
+    <row r="278" ht="87.0" customHeight="1">
+      <c r="A278" s="9" t="s">
         <v>549</v>
       </c>
-      <c r="B278" s="8" t="s">
+      <c r="B278" s="10" t="s">
         <v>550</v>
       </c>
     </row>
-    <row r="279" ht="14.25" customHeight="1">
-      <c r="A279" s="7" t="s">
+    <row r="279" ht="87.0" customHeight="1">
+      <c r="A279" s="9" t="s">
         <v>551</v>
       </c>
-      <c r="B279" s="8" t="s">
+      <c r="B279" s="10" t="s">
         <v>552</v>
       </c>
     </row>
-    <row r="280" ht="14.25" customHeight="1">
-      <c r="A280" s="7" t="s">
+    <row r="280" ht="87.0" customHeight="1">
+      <c r="A280" s="9" t="s">
         <v>553</v>
       </c>
-      <c r="B280" s="6" t="s">
+      <c r="B280" s="8" t="s">
         <v>554</v>
       </c>
     </row>
-    <row r="281" ht="14.25" customHeight="1">
-      <c r="A281" s="7" t="s">
+    <row r="281" ht="87.0" customHeight="1">
+      <c r="A281" s="9" t="s">
         <v>555</v>
       </c>
-      <c r="B281" s="8" t="s">
+      <c r="B281" s="12" t="s">
         <v>556</v>
       </c>
     </row>
-    <row r="282" ht="14.25" customHeight="1">
-      <c r="A282" s="7" t="s">
+    <row r="282" ht="87.0" customHeight="1">
+      <c r="A282" s="9" t="s">
         <v>557</v>
       </c>
-      <c r="B282" s="8" t="s">
+      <c r="B282" s="12" t="s">
         <v>558</v>
       </c>
     </row>
-    <row r="283" ht="14.25" customHeight="1">
-      <c r="A283" s="7" t="s">
+    <row r="283" ht="87.0" customHeight="1">
+      <c r="A283" s="9" t="s">
         <v>559</v>
       </c>
-      <c r="B283" s="8" t="s">
+      <c r="B283" s="12" t="s">
         <v>560</v>
       </c>
     </row>
-    <row r="284" ht="14.25" customHeight="1">
-      <c r="A284" s="7" t="s">
+    <row r="284" ht="87.0" customHeight="1">
+      <c r="A284" s="9" t="s">
         <v>561</v>
       </c>
-      <c r="B284" s="8" t="s">
+      <c r="B284" s="12" t="s">
         <v>562</v>
       </c>
     </row>
-    <row r="285" ht="14.25" customHeight="1">
-      <c r="A285" s="7" t="s">
+    <row r="285" ht="87.0" customHeight="1">
+      <c r="A285" s="9" t="s">
         <v>563</v>
       </c>
-      <c r="B285" s="8" t="s">
+      <c r="B285" s="12" t="s">
         <v>564</v>
       </c>
     </row>
-    <row r="286" ht="14.25" customHeight="1">
-      <c r="A286" s="7" t="s">
+    <row r="286" ht="87.0" customHeight="1">
+      <c r="A286" s="9" t="s">
         <v>565</v>
       </c>
-      <c r="B286" s="8" t="s">
+      <c r="B286" s="12" t="s">
         <v>566</v>
       </c>
     </row>
-    <row r="287" ht="14.25" customHeight="1">
-      <c r="A287" s="7" t="s">
+    <row r="287" ht="87.0" customHeight="1">
+      <c r="A287" s="9" t="s">
         <v>567</v>
       </c>
-      <c r="B287" s="10" t="s">
+      <c r="B287" s="13" t="s">
         <v>568</v>
       </c>
     </row>
-    <row r="288" ht="14.25" customHeight="1">
-      <c r="A288" s="7" t="s">
+    <row r="288" ht="87.0" customHeight="1">
+      <c r="A288" s="9" t="s">
         <v>569</v>
       </c>
-      <c r="B288" s="8" t="s">
+      <c r="B288" s="10" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="289" ht="14.25" customHeight="1">
-      <c r="A289" s="5" t="s">
+    <row r="289" ht="87.0" customHeight="1">
+      <c r="A289" s="7" t="s">
         <v>571</v>
       </c>
-      <c r="B289" s="8" t="s">
+      <c r="B289" s="10" t="s">
         <v>572</v>
       </c>
     </row>
-    <row r="290" ht="14.25" customHeight="1">
+    <row r="290" ht="87.0" customHeight="1">
       <c r="A290" s="1" t="s">
         <v>573</v>
       </c>
-      <c r="B290" s="1" t="s">
+      <c r="B290" s="2" t="s">
         <v>574</v>
       </c>
     </row>
-    <row r="291" ht="14.25" customHeight="1">
+    <row r="291" ht="87.0" customHeight="1">
       <c r="A291" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="B291" s="1" t="s">
+      <c r="B291" s="3" t="s">
         <v>576</v>
       </c>
     </row>
-    <row r="292" ht="14.25" customHeight="1">
+    <row r="292" ht="87.0" customHeight="1">
       <c r="A292" s="1" t="s">
         <v>577</v>
       </c>
-      <c r="B292" s="1" t="s">
+      <c r="B292" s="3" t="s">
         <v>578</v>
       </c>
     </row>
-    <row r="293" ht="14.25" customHeight="1">
+    <row r="293" ht="87.0" customHeight="1">
       <c r="A293" s="1" t="s">
         <v>579</v>
       </c>
-      <c r="B293" s="1" t="s">
+      <c r="B293" s="3" t="s">
         <v>580</v>
       </c>
     </row>
-    <row r="294" ht="14.25" customHeight="1">
+    <row r="294" ht="87.0" customHeight="1">
       <c r="A294" s="1" t="s">
         <v>581</v>
       </c>
-      <c r="B294" s="1" t="s">
+      <c r="B294" s="3" t="s">
         <v>582</v>
       </c>
     </row>

</xml_diff>